<commit_message>
missing lateralisation values in excel (fix #53)
</commit_message>
<xml_diff>
--- a/resources/syst_review_single_table.xlsx
+++ b/resources/syst_review_single_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\AnacondaProjects\PhD\Semiology-Visualisation-Tool\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCBDEBE-AC57-483B-AE55-AD17A3A76971}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122A89D4-CB4F-43B4-87D6-103C10231F3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8983,73 +8983,73 @@
                   <c:v>228</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>236</c:v>
+                  <c:v>254</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>241</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>248</c:v>
+                  <c:v>266</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>249</c:v>
+                  <c:v>267</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>269</c:v>
+                  <c:v>287</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>282</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>296</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>300</c:v>
+                  <c:v>319</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>303</c:v>
+                  <c:v>322</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>303</c:v>
+                  <c:v>322</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>387</c:v>
+                  <c:v>406</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>391</c:v>
+                  <c:v>410</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>395</c:v>
+                  <c:v>414</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>403</c:v>
+                  <c:v>422</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>413</c:v>
+                  <c:v>432</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>413</c:v>
+                  <c:v>432</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>422</c:v>
+                  <c:v>441</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>422</c:v>
+                  <c:v>441</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>422</c:v>
+                  <c:v>441</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>428</c:v>
+                  <c:v>447</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>520</c:v>
+                  <c:v>539</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>528</c:v>
+                  <c:v>547</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>564</c:v>
+                  <c:v>583</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10430,11 +10430,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DT1102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="CW3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="E449" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="CZ2" sqref="R1:DD1048576"/>
+      <selection pane="bottomRight" activeCell="J462" sqref="J462"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -23526,6 +23526,9 @@
       <c r="I279" s="41" t="s">
         <v>122</v>
       </c>
+      <c r="J279" s="5">
+        <v>1</v>
+      </c>
       <c r="O279" s="5">
         <v>1</v>
       </c>
@@ -23589,6 +23592,9 @@
       <c r="I280" s="41" t="s">
         <v>122</v>
       </c>
+      <c r="J280" s="5">
+        <v>3</v>
+      </c>
       <c r="N280" s="5">
         <v>1</v>
       </c>
@@ -23655,6 +23661,9 @@
       <c r="I281" s="41" t="s">
         <v>122</v>
       </c>
+      <c r="J281" s="5">
+        <v>3</v>
+      </c>
       <c r="N281" s="5">
         <v>1</v>
       </c>
@@ -23721,6 +23730,9 @@
       <c r="I282" s="41" t="s">
         <v>122</v>
       </c>
+      <c r="J282" s="5">
+        <v>1</v>
+      </c>
       <c r="O282" s="5">
         <v>1</v>
       </c>
@@ -23775,6 +23787,9 @@
       <c r="I283" s="41" t="s">
         <v>122</v>
       </c>
+      <c r="J283" s="5">
+        <v>2</v>
+      </c>
       <c r="O283" s="5">
         <v>2</v>
       </c>
@@ -23835,6 +23850,9 @@
       <c r="I284" s="41" t="s">
         <v>122</v>
       </c>
+      <c r="J284" s="5">
+        <v>1</v>
+      </c>
       <c r="O284" s="5">
         <v>1</v>
       </c>
@@ -23889,6 +23907,9 @@
       <c r="I285" s="41" t="s">
         <v>122</v>
       </c>
+      <c r="J285" s="5">
+        <v>1</v>
+      </c>
       <c r="O285" s="5">
         <v>1</v>
       </c>
@@ -23943,6 +23964,9 @@
       <c r="I286" s="41" t="s">
         <v>122</v>
       </c>
+      <c r="J286" s="5">
+        <v>1</v>
+      </c>
       <c r="O286" s="5">
         <v>1</v>
       </c>
@@ -23997,6 +24021,9 @@
       <c r="I287" s="41" t="s">
         <v>122</v>
       </c>
+      <c r="J287" s="5">
+        <v>1</v>
+      </c>
       <c r="N287" s="5">
         <v>1</v>
       </c>
@@ -24054,6 +24081,9 @@
       <c r="I288" s="41" t="s">
         <v>122</v>
       </c>
+      <c r="J288" s="5">
+        <v>1</v>
+      </c>
       <c r="N288" s="5">
         <v>1</v>
       </c>
@@ -24099,6 +24129,9 @@
       <c r="I289" s="41" t="s">
         <v>122</v>
       </c>
+      <c r="J289" s="5">
+        <v>1</v>
+      </c>
       <c r="N289" s="5">
         <v>1</v>
       </c>
@@ -24144,6 +24177,9 @@
       <c r="I290" s="41" t="s">
         <v>122</v>
       </c>
+      <c r="J290" s="5">
+        <v>1</v>
+      </c>
       <c r="O290" s="5">
         <v>1</v>
       </c>
@@ -24197,6 +24233,9 @@
       <c r="H291" s="41"/>
       <c r="I291" s="41" t="s">
         <v>122</v>
+      </c>
+      <c r="J291" s="5">
+        <v>1</v>
       </c>
       <c r="O291" s="5">
         <v>1</v>
@@ -33458,7 +33497,9 @@
       <c r="I462" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="J462" s="5"/>
+      <c r="J462" s="5">
+        <v>1</v>
+      </c>
       <c r="K462" s="5">
         <v>1</v>
       </c>
@@ -73582,7 +73623,7 @@
       </c>
       <c r="F6" s="53">
         <f>SUM(Main!J2:J321)</f>
-        <v>236</v>
+        <v>254</v>
       </c>
       <c r="G6" s="53">
         <f>SUM(Main!P2:P321)</f>
@@ -73637,7 +73678,7 @@
       </c>
       <c r="F8" s="53">
         <f>SUM(Main!$J$2:J365)</f>
-        <v>248</v>
+        <v>266</v>
       </c>
       <c r="G8" s="78">
         <f>SUM(Main!$P$2:P365)</f>
@@ -73665,7 +73706,7 @@
       </c>
       <c r="F9" s="53">
         <f>SUM(Main!$J$2:J370)</f>
-        <v>249</v>
+        <v>267</v>
       </c>
       <c r="G9" s="53">
         <f>SUM(Main!$P$2:P370)</f>
@@ -73693,7 +73734,7 @@
       </c>
       <c r="F10" s="53">
         <f>SUM(Main!$J$2:J398)</f>
-        <v>269</v>
+        <v>287</v>
       </c>
       <c r="G10" s="53">
         <f>SUM(Main!$P$2:P398)</f>
@@ -73721,7 +73762,7 @@
       </c>
       <c r="F11" s="53">
         <f>SUM(Main!$J$2:J428)</f>
-        <v>282</v>
+        <v>300</v>
       </c>
       <c r="G11" s="53">
         <f>SUM(Main!$P$2:P428)</f>
@@ -73772,7 +73813,7 @@
       </c>
       <c r="F13" s="53">
         <f>SUM(Main!$J$2:J519)</f>
-        <v>300</v>
+        <v>319</v>
       </c>
       <c r="G13" s="53">
         <f>SUM(Main!$P$2:P519)</f>
@@ -73798,7 +73839,7 @@
       </c>
       <c r="F14" s="53">
         <f>SUM(Main!$J$2:J543)</f>
-        <v>303</v>
+        <v>322</v>
       </c>
       <c r="G14" s="53">
         <f>SUM(Main!$P$2:P543)</f>
@@ -73826,7 +73867,7 @@
       </c>
       <c r="F15" s="53">
         <f>SUM(Main!$J$2:J583)</f>
-        <v>303</v>
+        <v>322</v>
       </c>
       <c r="G15" s="53">
         <f>SUM(Main!$P$2:P583)</f>
@@ -73854,7 +73895,7 @@
       </c>
       <c r="F16" s="53">
         <f>SUM(Main!$J$2:J610)</f>
-        <v>387</v>
+        <v>406</v>
       </c>
       <c r="G16" s="53">
         <f>SUM(Main!$P$2:P610)</f>
@@ -73882,7 +73923,7 @@
       </c>
       <c r="F17" s="53">
         <f>SUM(Main!$J$2:J648)</f>
-        <v>391</v>
+        <v>410</v>
       </c>
       <c r="G17" s="53">
         <f>SUM(Main!$P$2:P648)</f>
@@ -73910,7 +73951,7 @@
       </c>
       <c r="F18" s="53">
         <f>SUM(Main!$J$2:J658)</f>
-        <v>395</v>
+        <v>414</v>
       </c>
       <c r="G18" s="53">
         <f>SUM(Main!$P$2:P658)</f>
@@ -73937,7 +73978,7 @@
       </c>
       <c r="F19" s="53">
         <f>SUM(Main!$J$2:J723)</f>
-        <v>403</v>
+        <v>422</v>
       </c>
       <c r="G19" s="53">
         <f>SUM(Main!$P$2:P723)</f>
@@ -73963,7 +74004,7 @@
       </c>
       <c r="F20" s="53">
         <f>SUM(Main!$J$2:J735)</f>
-        <v>413</v>
+        <v>432</v>
       </c>
       <c r="G20" s="53">
         <f>SUM(Main!$P$2:P735)</f>
@@ -73989,7 +74030,7 @@
       </c>
       <c r="F21" s="53">
         <f>SUM(Main!$J$2:J754)</f>
-        <v>413</v>
+        <v>432</v>
       </c>
       <c r="G21" s="53">
         <f>SUM(Main!$P$2:P754)</f>
@@ -74015,7 +74056,7 @@
       </c>
       <c r="F22" s="53">
         <f>SUM(Main!$J$2:J770)</f>
-        <v>422</v>
+        <v>441</v>
       </c>
       <c r="G22" s="53">
         <f>SUM(Main!$P$2:P770)</f>
@@ -74041,7 +74082,7 @@
       </c>
       <c r="F23" s="53">
         <f>SUM(Main!$J$2:J770)</f>
-        <v>422</v>
+        <v>441</v>
       </c>
       <c r="G23" s="53">
         <f>SUM(Main!$P$2:P770)</f>
@@ -74067,7 +74108,7 @@
       </c>
       <c r="F24" s="53">
         <f>SUM(Main!$J$2:J770)</f>
-        <v>422</v>
+        <v>441</v>
       </c>
       <c r="G24" s="53">
         <f>SUM(Main!$P$2:P770)</f>
@@ -74093,7 +74134,7 @@
       </c>
       <c r="F25" s="53">
         <f>SUM(Main!$J$2:J813)</f>
-        <v>428</v>
+        <v>447</v>
       </c>
       <c r="G25" s="53">
         <f>SUM(Main!$P$2:P813)</f>
@@ -74119,7 +74160,7 @@
       </c>
       <c r="F26" s="53">
         <f>SUM(Main!$J$2:J885)</f>
-        <v>520</v>
+        <v>539</v>
       </c>
       <c r="G26" s="53">
         <f>SUM(Main!$P$2:P885)</f>
@@ -74149,7 +74190,7 @@
       </c>
       <c r="F27" s="53">
         <f>SUM(Main!$J$2:J933)</f>
-        <v>528</v>
+        <v>547</v>
       </c>
       <c r="G27" s="53">
         <f>SUM(Main!$P$2:P933)</f>
@@ -74175,7 +74216,7 @@
       </c>
       <c r="F28" s="53">
         <f>SUM(Main!$J$2:J1038)</f>
-        <v>564</v>
+        <v>583</v>
       </c>
       <c r="G28" s="53">
         <f>SUM(Main!$P$2:P1038)</f>

</xml_diff>

<commit_message>
Fill missing values in query_semiology (#58)
* missing lateralisation values in excel (fix #53)

* autofill to prevent future NaN/zero errors
</commit_message>
<xml_diff>
--- a/resources/syst_review_single_table.xlsx
+++ b/resources/syst_review_single_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\AnacondaProjects\PhD\Semiology-Visualisation-Tool\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCBDEBE-AC57-483B-AE55-AD17A3A76971}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122A89D4-CB4F-43B4-87D6-103C10231F3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8983,73 +8983,73 @@
                   <c:v>228</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>236</c:v>
+                  <c:v>254</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>241</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>248</c:v>
+                  <c:v>266</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>249</c:v>
+                  <c:v>267</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>269</c:v>
+                  <c:v>287</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>282</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>296</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>300</c:v>
+                  <c:v>319</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>303</c:v>
+                  <c:v>322</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>303</c:v>
+                  <c:v>322</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>387</c:v>
+                  <c:v>406</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>391</c:v>
+                  <c:v>410</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>395</c:v>
+                  <c:v>414</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>403</c:v>
+                  <c:v>422</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>413</c:v>
+                  <c:v>432</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>413</c:v>
+                  <c:v>432</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>422</c:v>
+                  <c:v>441</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>422</c:v>
+                  <c:v>441</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>422</c:v>
+                  <c:v>441</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>428</c:v>
+                  <c:v>447</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>520</c:v>
+                  <c:v>539</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>528</c:v>
+                  <c:v>547</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>564</c:v>
+                  <c:v>583</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10430,11 +10430,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DT1102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="CW3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="E449" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="CZ2" sqref="R1:DD1048576"/>
+      <selection pane="bottomRight" activeCell="J462" sqref="J462"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -23526,6 +23526,9 @@
       <c r="I279" s="41" t="s">
         <v>122</v>
       </c>
+      <c r="J279" s="5">
+        <v>1</v>
+      </c>
       <c r="O279" s="5">
         <v>1</v>
       </c>
@@ -23589,6 +23592,9 @@
       <c r="I280" s="41" t="s">
         <v>122</v>
       </c>
+      <c r="J280" s="5">
+        <v>3</v>
+      </c>
       <c r="N280" s="5">
         <v>1</v>
       </c>
@@ -23655,6 +23661,9 @@
       <c r="I281" s="41" t="s">
         <v>122</v>
       </c>
+      <c r="J281" s="5">
+        <v>3</v>
+      </c>
       <c r="N281" s="5">
         <v>1</v>
       </c>
@@ -23721,6 +23730,9 @@
       <c r="I282" s="41" t="s">
         <v>122</v>
       </c>
+      <c r="J282" s="5">
+        <v>1</v>
+      </c>
       <c r="O282" s="5">
         <v>1</v>
       </c>
@@ -23775,6 +23787,9 @@
       <c r="I283" s="41" t="s">
         <v>122</v>
       </c>
+      <c r="J283" s="5">
+        <v>2</v>
+      </c>
       <c r="O283" s="5">
         <v>2</v>
       </c>
@@ -23835,6 +23850,9 @@
       <c r="I284" s="41" t="s">
         <v>122</v>
       </c>
+      <c r="J284" s="5">
+        <v>1</v>
+      </c>
       <c r="O284" s="5">
         <v>1</v>
       </c>
@@ -23889,6 +23907,9 @@
       <c r="I285" s="41" t="s">
         <v>122</v>
       </c>
+      <c r="J285" s="5">
+        <v>1</v>
+      </c>
       <c r="O285" s="5">
         <v>1</v>
       </c>
@@ -23943,6 +23964,9 @@
       <c r="I286" s="41" t="s">
         <v>122</v>
       </c>
+      <c r="J286" s="5">
+        <v>1</v>
+      </c>
       <c r="O286" s="5">
         <v>1</v>
       </c>
@@ -23997,6 +24021,9 @@
       <c r="I287" s="41" t="s">
         <v>122</v>
       </c>
+      <c r="J287" s="5">
+        <v>1</v>
+      </c>
       <c r="N287" s="5">
         <v>1</v>
       </c>
@@ -24054,6 +24081,9 @@
       <c r="I288" s="41" t="s">
         <v>122</v>
       </c>
+      <c r="J288" s="5">
+        <v>1</v>
+      </c>
       <c r="N288" s="5">
         <v>1</v>
       </c>
@@ -24099,6 +24129,9 @@
       <c r="I289" s="41" t="s">
         <v>122</v>
       </c>
+      <c r="J289" s="5">
+        <v>1</v>
+      </c>
       <c r="N289" s="5">
         <v>1</v>
       </c>
@@ -24144,6 +24177,9 @@
       <c r="I290" s="41" t="s">
         <v>122</v>
       </c>
+      <c r="J290" s="5">
+        <v>1</v>
+      </c>
       <c r="O290" s="5">
         <v>1</v>
       </c>
@@ -24197,6 +24233,9 @@
       <c r="H291" s="41"/>
       <c r="I291" s="41" t="s">
         <v>122</v>
+      </c>
+      <c r="J291" s="5">
+        <v>1</v>
       </c>
       <c r="O291" s="5">
         <v>1</v>
@@ -33458,7 +33497,9 @@
       <c r="I462" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="J462" s="5"/>
+      <c r="J462" s="5">
+        <v>1</v>
+      </c>
       <c r="K462" s="5">
         <v>1</v>
       </c>
@@ -73582,7 +73623,7 @@
       </c>
       <c r="F6" s="53">
         <f>SUM(Main!J2:J321)</f>
-        <v>236</v>
+        <v>254</v>
       </c>
       <c r="G6" s="53">
         <f>SUM(Main!P2:P321)</f>
@@ -73637,7 +73678,7 @@
       </c>
       <c r="F8" s="53">
         <f>SUM(Main!$J$2:J365)</f>
-        <v>248</v>
+        <v>266</v>
       </c>
       <c r="G8" s="78">
         <f>SUM(Main!$P$2:P365)</f>
@@ -73665,7 +73706,7 @@
       </c>
       <c r="F9" s="53">
         <f>SUM(Main!$J$2:J370)</f>
-        <v>249</v>
+        <v>267</v>
       </c>
       <c r="G9" s="53">
         <f>SUM(Main!$P$2:P370)</f>
@@ -73693,7 +73734,7 @@
       </c>
       <c r="F10" s="53">
         <f>SUM(Main!$J$2:J398)</f>
-        <v>269</v>
+        <v>287</v>
       </c>
       <c r="G10" s="53">
         <f>SUM(Main!$P$2:P398)</f>
@@ -73721,7 +73762,7 @@
       </c>
       <c r="F11" s="53">
         <f>SUM(Main!$J$2:J428)</f>
-        <v>282</v>
+        <v>300</v>
       </c>
       <c r="G11" s="53">
         <f>SUM(Main!$P$2:P428)</f>
@@ -73772,7 +73813,7 @@
       </c>
       <c r="F13" s="53">
         <f>SUM(Main!$J$2:J519)</f>
-        <v>300</v>
+        <v>319</v>
       </c>
       <c r="G13" s="53">
         <f>SUM(Main!$P$2:P519)</f>
@@ -73798,7 +73839,7 @@
       </c>
       <c r="F14" s="53">
         <f>SUM(Main!$J$2:J543)</f>
-        <v>303</v>
+        <v>322</v>
       </c>
       <c r="G14" s="53">
         <f>SUM(Main!$P$2:P543)</f>
@@ -73826,7 +73867,7 @@
       </c>
       <c r="F15" s="53">
         <f>SUM(Main!$J$2:J583)</f>
-        <v>303</v>
+        <v>322</v>
       </c>
       <c r="G15" s="53">
         <f>SUM(Main!$P$2:P583)</f>
@@ -73854,7 +73895,7 @@
       </c>
       <c r="F16" s="53">
         <f>SUM(Main!$J$2:J610)</f>
-        <v>387</v>
+        <v>406</v>
       </c>
       <c r="G16" s="53">
         <f>SUM(Main!$P$2:P610)</f>
@@ -73882,7 +73923,7 @@
       </c>
       <c r="F17" s="53">
         <f>SUM(Main!$J$2:J648)</f>
-        <v>391</v>
+        <v>410</v>
       </c>
       <c r="G17" s="53">
         <f>SUM(Main!$P$2:P648)</f>
@@ -73910,7 +73951,7 @@
       </c>
       <c r="F18" s="53">
         <f>SUM(Main!$J$2:J658)</f>
-        <v>395</v>
+        <v>414</v>
       </c>
       <c r="G18" s="53">
         <f>SUM(Main!$P$2:P658)</f>
@@ -73937,7 +73978,7 @@
       </c>
       <c r="F19" s="53">
         <f>SUM(Main!$J$2:J723)</f>
-        <v>403</v>
+        <v>422</v>
       </c>
       <c r="G19" s="53">
         <f>SUM(Main!$P$2:P723)</f>
@@ -73963,7 +74004,7 @@
       </c>
       <c r="F20" s="53">
         <f>SUM(Main!$J$2:J735)</f>
-        <v>413</v>
+        <v>432</v>
       </c>
       <c r="G20" s="53">
         <f>SUM(Main!$P$2:P735)</f>
@@ -73989,7 +74030,7 @@
       </c>
       <c r="F21" s="53">
         <f>SUM(Main!$J$2:J754)</f>
-        <v>413</v>
+        <v>432</v>
       </c>
       <c r="G21" s="53">
         <f>SUM(Main!$P$2:P754)</f>
@@ -74015,7 +74056,7 @@
       </c>
       <c r="F22" s="53">
         <f>SUM(Main!$J$2:J770)</f>
-        <v>422</v>
+        <v>441</v>
       </c>
       <c r="G22" s="53">
         <f>SUM(Main!$P$2:P770)</f>
@@ -74041,7 +74082,7 @@
       </c>
       <c r="F23" s="53">
         <f>SUM(Main!$J$2:J770)</f>
-        <v>422</v>
+        <v>441</v>
       </c>
       <c r="G23" s="53">
         <f>SUM(Main!$P$2:P770)</f>
@@ -74067,7 +74108,7 @@
       </c>
       <c r="F24" s="53">
         <f>SUM(Main!$J$2:J770)</f>
-        <v>422</v>
+        <v>441</v>
       </c>
       <c r="G24" s="53">
         <f>SUM(Main!$P$2:P770)</f>
@@ -74093,7 +74134,7 @@
       </c>
       <c r="F25" s="53">
         <f>SUM(Main!$J$2:J813)</f>
-        <v>428</v>
+        <v>447</v>
       </c>
       <c r="G25" s="53">
         <f>SUM(Main!$P$2:P813)</f>
@@ -74119,7 +74160,7 @@
       </c>
       <c r="F26" s="53">
         <f>SUM(Main!$J$2:J885)</f>
-        <v>520</v>
+        <v>539</v>
       </c>
       <c r="G26" s="53">
         <f>SUM(Main!$P$2:P885)</f>
@@ -74149,7 +74190,7 @@
       </c>
       <c r="F27" s="53">
         <f>SUM(Main!$J$2:J933)</f>
-        <v>528</v>
+        <v>547</v>
       </c>
       <c r="G27" s="53">
         <f>SUM(Main!$P$2:P933)</f>
@@ -74175,7 +74216,7 @@
       </c>
       <c r="F28" s="53">
         <f>SUM(Main!$J$2:J1038)</f>
-        <v>564</v>
+        <v>583</v>
       </c>
       <c r="G28" s="53">
         <f>SUM(Main!$P$2:P1038)</f>

</xml_diff>

<commit_message>
minor clean up of cells in excel file
</commit_message>
<xml_diff>
--- a/resources/syst_review_single_table.xlsx
+++ b/resources/syst_review_single_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\AnacondaProjects\PhD\Semiology-Visualisation-Tool\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{974600EB-BBE5-47AD-8BAC-F01671A7224E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0564EB-E5BB-4E77-AB79-5245DCAB810A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6992" uniqueCount="2159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6991" uniqueCount="2158">
   <si>
     <t xml:space="preserve">Semiology </t>
   </si>
@@ -6387,9 +6387,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Right Insula White Matter</t>
-  </si>
-  <si>
-    <t>p</t>
   </si>
   <si>
     <t xml:space="preserve"> Right Cingulate White Matter</t>
@@ -10397,10 +10394,10 @@
   <dimension ref="A1:DU1102"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="CB3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="CW2" sqref="CW2"/>
+      <selection pane="bottomRight" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -10769,7 +10766,7 @@
         <v>57</v>
       </c>
       <c r="BA2" s="25" t="s">
-        <v>2153</v>
+        <v>2152</v>
       </c>
       <c r="BB2" s="25" t="s">
         <v>58</v>
@@ -10796,7 +10793,7 @@
         <v>65</v>
       </c>
       <c r="BJ2" s="25" t="s">
-        <v>2154</v>
+        <v>2153</v>
       </c>
       <c r="BK2" s="25" t="s">
         <v>66</v>
@@ -72781,7 +72778,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="66" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="B3" s="61">
         <v>109</v>
@@ -72792,7 +72789,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="66" t="s">
-        <v>2061</v>
+        <v>2060</v>
       </c>
       <c r="B4" s="61">
         <v>110</v>
@@ -72808,7 +72805,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>2064</v>
+        <v>2063</v>
       </c>
       <c r="B5" s="61">
         <v>115</v>
@@ -72826,7 +72823,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>2065</v>
+        <v>2064</v>
       </c>
       <c r="B6" s="61">
         <v>116</v>
@@ -72844,7 +72841,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="66" t="s">
-        <v>2076</v>
+        <v>2075</v>
       </c>
       <c r="B7" s="61">
         <v>129</v>
@@ -72860,7 +72857,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="66" t="s">
-        <v>2077</v>
+        <v>2076</v>
       </c>
       <c r="B8" s="61">
         <v>130</v>
@@ -72876,7 +72873,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>2080</v>
+        <v>2079</v>
       </c>
       <c r="B9" s="61">
         <v>135</v>
@@ -72894,7 +72891,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>2081</v>
+        <v>2080</v>
       </c>
       <c r="B10" s="61">
         <v>136</v>
@@ -72912,7 +72909,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>2090</v>
+        <v>2089</v>
       </c>
       <c r="B11" s="61">
         <v>145</v>
@@ -72930,7 +72927,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>2091</v>
+        <v>2090</v>
       </c>
       <c r="B12" s="61">
         <v>146</v>
@@ -72948,7 +72945,7 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="B13" s="61">
         <v>157</v>
@@ -72966,7 +72963,7 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>2103</v>
+        <v>2102</v>
       </c>
       <c r="B14" s="61">
         <v>158</v>
@@ -72984,7 +72981,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="66" t="s">
-        <v>2104</v>
+        <v>2103</v>
       </c>
       <c r="B15" s="61">
         <v>161</v>
@@ -73000,7 +72997,7 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="66" t="s">
-        <v>2105</v>
+        <v>2104</v>
       </c>
       <c r="B16" s="61">
         <v>162</v>
@@ -73011,7 +73008,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="66" t="s">
-        <v>2138</v>
+        <v>2137</v>
       </c>
       <c r="B17" s="53">
         <v>197</v>
@@ -73022,7 +73019,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="66" t="s">
-        <v>2139</v>
+        <v>2138</v>
       </c>
       <c r="B18" s="53">
         <v>198</v>
@@ -73087,12 +73084,12 @@
         <v>79</v>
       </c>
       <c r="J2" s="133" t="s">
-        <v>2156</v>
+        <v>2155</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
       <c r="B3" s="61">
         <v>101</v>
@@ -73113,7 +73110,7 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>2053</v>
+        <v>2052</v>
       </c>
       <c r="B4" s="61">
         <v>102</v>
@@ -73134,7 +73131,7 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>2084</v>
+        <v>2083</v>
       </c>
       <c r="B5" s="61">
         <v>139</v>
@@ -73148,7 +73145,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>2085</v>
+        <v>2084</v>
       </c>
       <c r="B6" s="61">
         <v>140</v>
@@ -73162,7 +73159,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>2110</v>
+        <v>2109</v>
       </c>
       <c r="B7" s="61">
         <v>167</v>
@@ -73179,7 +73176,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>2111</v>
+        <v>2110</v>
       </c>
       <c r="B8" s="61">
         <v>168</v>
@@ -73196,7 +73193,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>2157</v>
+        <v>2156</v>
       </c>
       <c r="B9" s="61">
         <v>83</v>
@@ -73210,7 +73207,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>2158</v>
+        <v>2157</v>
       </c>
       <c r="B10" s="61">
         <v>91</v>
@@ -73235,12 +73232,13 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25">
@@ -73287,7 +73285,7 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>2054</v>
+        <v>2053</v>
       </c>
       <c r="B3" s="61">
         <v>103</v>
@@ -73313,7 +73311,7 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>2055</v>
+        <v>2054</v>
       </c>
       <c r="B4" s="61">
         <v>104</v>
@@ -73339,7 +73337,7 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>2116</v>
+        <v>2115</v>
       </c>
       <c r="B5" s="61">
         <v>173</v>
@@ -73359,7 +73357,7 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>2117</v>
+        <v>2116</v>
       </c>
       <c r="B6" s="61">
         <v>174</v>
@@ -73393,28 +73391,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2AF3FB6-8F7D-4474-A830-E874EC2C2727}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1">
-      <c r="D1" s="145"/>
-      <c r="E1" s="145"/>
-    </row>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1"/>
     <row r="2" spans="1:5" ht="26.25">
       <c r="C2" s="101" t="s">
         <v>104</v>
       </c>
-      <c r="D2" s="144"/>
-      <c r="E2" s="144"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
@@ -73426,8 +73419,6 @@
       <c r="C3" s="61">
         <v>60</v>
       </c>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
@@ -73439,15 +73430,11 @@
       <c r="C4" s="61">
         <v>61</v>
       </c>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="117"/>
       <c r="B5" s="53"/>
       <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="117"/>
@@ -74796,10 +74783,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F189"/>
+  <dimension ref="A1:D189"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -75199,7 +75186,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:4">
       <c r="A49" s="117" t="s">
         <v>2034</v>
       </c>
@@ -75207,7 +75194,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:4">
       <c r="A50" s="117" t="s">
         <v>2035</v>
       </c>
@@ -75215,7 +75202,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:4">
       <c r="A51" s="117" t="s">
         <v>2036</v>
       </c>
@@ -75223,108 +75210,105 @@
         <v>81</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:4">
       <c r="A52" s="117" t="s">
         <v>2037</v>
       </c>
       <c r="C52" s="53">
         <v>82</v>
       </c>
-      <c r="F52" t="s">
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="117" t="s">
         <v>2038</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53" s="117" t="s">
-        <v>2039</v>
       </c>
       <c r="C53" s="53">
         <v>83</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:4">
       <c r="A54" s="117" t="s">
-        <v>2040</v>
+        <v>2039</v>
       </c>
       <c r="C54" s="53">
         <v>84</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:4">
       <c r="A55" s="117" t="s">
-        <v>2041</v>
+        <v>2040</v>
       </c>
       <c r="C55" s="53">
         <v>85</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:4">
       <c r="A56" s="117" t="s">
-        <v>2042</v>
+        <v>2041</v>
       </c>
       <c r="C56" s="53">
         <v>86</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:4">
       <c r="A57" s="117" t="s">
-        <v>2043</v>
+        <v>2042</v>
       </c>
       <c r="B57" s="53">
         <v>87</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:4">
       <c r="A58" s="117" t="s">
-        <v>2044</v>
+        <v>2043</v>
       </c>
       <c r="D58" s="53">
         <v>89</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:4">
       <c r="A59" s="117" t="s">
-        <v>2045</v>
+        <v>2044</v>
       </c>
       <c r="D59" s="53">
         <v>90</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:4">
       <c r="A60" s="117" t="s">
-        <v>2046</v>
+        <v>2045</v>
       </c>
       <c r="D60" s="53">
         <v>91</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:4">
       <c r="A61" s="117" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
       <c r="D61" s="53">
         <v>92</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:4">
       <c r="A62" s="117" t="s">
-        <v>2048</v>
+        <v>2047</v>
       </c>
       <c r="D62" s="53">
         <v>93</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:4">
       <c r="A63" s="117" t="s">
-        <v>2049</v>
+        <v>2048</v>
       </c>
       <c r="D63" s="53">
         <v>94</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:4">
       <c r="A64" s="117" t="s">
-        <v>2050</v>
+        <v>2049</v>
       </c>
       <c r="C64" s="53">
         <v>96</v>
@@ -75332,7 +75316,7 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="117" t="s">
-        <v>2051</v>
+        <v>2050</v>
       </c>
       <c r="D65" s="53">
         <v>97</v>
@@ -75340,7 +75324,7 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="117" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
       <c r="C66" s="53">
         <v>101</v>
@@ -75348,7 +75332,7 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="117" t="s">
-        <v>2053</v>
+        <v>2052</v>
       </c>
       <c r="D67" s="53">
         <v>102</v>
@@ -75356,7 +75340,7 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="117" t="s">
-        <v>2054</v>
+        <v>2053</v>
       </c>
       <c r="C68" s="53">
         <v>103</v>
@@ -75364,7 +75348,7 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="117" t="s">
-        <v>2055</v>
+        <v>2054</v>
       </c>
       <c r="D69" s="53">
         <v>104</v>
@@ -75372,7 +75356,7 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="117" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
       <c r="C70" s="53">
         <v>105</v>
@@ -75380,7 +75364,7 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="117" t="s">
-        <v>2057</v>
+        <v>2056</v>
       </c>
       <c r="D71" s="53">
         <v>106</v>
@@ -75388,7 +75372,7 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="117" t="s">
-        <v>2058</v>
+        <v>2057</v>
       </c>
       <c r="C72" s="53">
         <v>107</v>
@@ -75396,7 +75380,7 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="117" t="s">
-        <v>2059</v>
+        <v>2058</v>
       </c>
       <c r="D73" s="53">
         <v>108</v>
@@ -75404,7 +75388,7 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="117" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="C74" s="53">
         <v>109</v>
@@ -75412,7 +75396,7 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="117" t="s">
-        <v>2061</v>
+        <v>2060</v>
       </c>
       <c r="D75" s="53">
         <v>110</v>
@@ -75420,7 +75404,7 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="117" t="s">
-        <v>2062</v>
+        <v>2061</v>
       </c>
       <c r="C76" s="53">
         <v>113</v>
@@ -75428,7 +75412,7 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="117" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
       <c r="D77" s="53">
         <v>114</v>
@@ -75436,7 +75420,7 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="117" t="s">
-        <v>2064</v>
+        <v>2063</v>
       </c>
       <c r="C78" s="53">
         <v>115</v>
@@ -75444,7 +75428,7 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="117" t="s">
-        <v>2065</v>
+        <v>2064</v>
       </c>
       <c r="D79" s="53">
         <v>116</v>
@@ -75452,7 +75436,7 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="117" t="s">
-        <v>2066</v>
+        <v>2065</v>
       </c>
       <c r="C80" s="53">
         <v>117</v>
@@ -75460,7 +75444,7 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="117" t="s">
-        <v>2067</v>
+        <v>2066</v>
       </c>
       <c r="D81" s="53">
         <v>118</v>
@@ -75468,7 +75452,7 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="117" t="s">
-        <v>2068</v>
+        <v>2067</v>
       </c>
       <c r="C82" s="53">
         <v>119</v>
@@ -75476,7 +75460,7 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="117" t="s">
-        <v>2069</v>
+        <v>2068</v>
       </c>
       <c r="D83" s="53">
         <v>120</v>
@@ -75484,7 +75468,7 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="117" t="s">
-        <v>2070</v>
+        <v>2069</v>
       </c>
       <c r="C84" s="53">
         <v>121</v>
@@ -75492,7 +75476,7 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="117" t="s">
-        <v>2071</v>
+        <v>2070</v>
       </c>
       <c r="D85" s="53">
         <v>122</v>
@@ -75500,7 +75484,7 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="117" t="s">
-        <v>2072</v>
+        <v>2071</v>
       </c>
       <c r="C86" s="53">
         <v>123</v>
@@ -75508,7 +75492,7 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="117" t="s">
-        <v>2073</v>
+        <v>2072</v>
       </c>
       <c r="D87" s="53">
         <v>124</v>
@@ -75516,7 +75500,7 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="117" t="s">
-        <v>2074</v>
+        <v>2073</v>
       </c>
       <c r="C88" s="53">
         <v>125</v>
@@ -75524,7 +75508,7 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="117" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
       <c r="D89" s="53">
         <v>126</v>
@@ -75532,7 +75516,7 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="117" t="s">
-        <v>2076</v>
+        <v>2075</v>
       </c>
       <c r="C90" s="53">
         <v>129</v>
@@ -75540,7 +75524,7 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="117" t="s">
-        <v>2077</v>
+        <v>2076</v>
       </c>
       <c r="D91" s="53">
         <v>130</v>
@@ -75548,7 +75532,7 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="117" t="s">
-        <v>2078</v>
+        <v>2077</v>
       </c>
       <c r="C92" s="53">
         <v>133</v>
@@ -75556,7 +75540,7 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="117" t="s">
-        <v>2079</v>
+        <v>2078</v>
       </c>
       <c r="D93" s="53">
         <v>134</v>
@@ -75564,7 +75548,7 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="117" t="s">
-        <v>2080</v>
+        <v>2079</v>
       </c>
       <c r="C94" s="53">
         <v>135</v>
@@ -75572,7 +75556,7 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="117" t="s">
-        <v>2081</v>
+        <v>2080</v>
       </c>
       <c r="D95" s="53">
         <v>136</v>
@@ -75580,7 +75564,7 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="117" t="s">
-        <v>2082</v>
+        <v>2081</v>
       </c>
       <c r="C96" s="53">
         <v>137</v>
@@ -75588,7 +75572,7 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="117" t="s">
-        <v>2083</v>
+        <v>2082</v>
       </c>
       <c r="D97" s="53">
         <v>138</v>
@@ -75596,7 +75580,7 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="117" t="s">
-        <v>2084</v>
+        <v>2083</v>
       </c>
       <c r="C98" s="53">
         <v>139</v>
@@ -75604,7 +75588,7 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="117" t="s">
-        <v>2085</v>
+        <v>2084</v>
       </c>
       <c r="D99" s="53">
         <v>140</v>
@@ -75612,7 +75596,7 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="117" t="s">
-        <v>2086</v>
+        <v>2085</v>
       </c>
       <c r="C100" s="53">
         <v>141</v>
@@ -75620,7 +75604,7 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="117" t="s">
-        <v>2087</v>
+        <v>2086</v>
       </c>
       <c r="D101" s="53">
         <v>142</v>
@@ -75628,7 +75612,7 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="117" t="s">
-        <v>2088</v>
+        <v>2087</v>
       </c>
       <c r="C102" s="53">
         <v>143</v>
@@ -75636,7 +75620,7 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="117" t="s">
-        <v>2089</v>
+        <v>2088</v>
       </c>
       <c r="D103" s="53">
         <v>144</v>
@@ -75644,7 +75628,7 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="117" t="s">
-        <v>2090</v>
+        <v>2089</v>
       </c>
       <c r="C104" s="53">
         <v>145</v>
@@ -75652,7 +75636,7 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="117" t="s">
-        <v>2091</v>
+        <v>2090</v>
       </c>
       <c r="D105" s="53">
         <v>146</v>
@@ -75660,7 +75644,7 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="117" t="s">
-        <v>2092</v>
+        <v>2091</v>
       </c>
       <c r="C106" s="53">
         <v>147</v>
@@ -75668,7 +75652,7 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="117" t="s">
-        <v>2093</v>
+        <v>2092</v>
       </c>
       <c r="D107" s="53">
         <v>148</v>
@@ -75676,7 +75660,7 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="117" t="s">
-        <v>2094</v>
+        <v>2093</v>
       </c>
       <c r="C108" s="53">
         <v>149</v>
@@ -75684,7 +75668,7 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="117" t="s">
-        <v>2095</v>
+        <v>2094</v>
       </c>
       <c r="D109" s="53">
         <v>150</v>
@@ -75692,7 +75676,7 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="117" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="C110" s="53">
         <v>151</v>
@@ -75700,7 +75684,7 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="117" t="s">
-        <v>2097</v>
+        <v>2096</v>
       </c>
       <c r="D111" s="53">
         <v>152</v>
@@ -75708,7 +75692,7 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="117" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
       <c r="C112" s="53">
         <v>153</v>
@@ -75716,7 +75700,7 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="117" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
       <c r="D113" s="53">
         <v>154</v>
@@ -75724,7 +75708,7 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="117" t="s">
-        <v>2100</v>
+        <v>2099</v>
       </c>
       <c r="C114" s="53">
         <v>155</v>
@@ -75732,7 +75716,7 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="117" t="s">
-        <v>2101</v>
+        <v>2100</v>
       </c>
       <c r="D115" s="53">
         <v>156</v>
@@ -75740,7 +75724,7 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="117" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="C116" s="53">
         <v>157</v>
@@ -75748,7 +75732,7 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="117" t="s">
-        <v>2103</v>
+        <v>2102</v>
       </c>
       <c r="D117" s="53">
         <v>158</v>
@@ -75756,7 +75740,7 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="117" t="s">
-        <v>2104</v>
+        <v>2103</v>
       </c>
       <c r="C118" s="53">
         <v>161</v>
@@ -75764,7 +75748,7 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="117" t="s">
-        <v>2105</v>
+        <v>2104</v>
       </c>
       <c r="D119" s="53">
         <v>162</v>
@@ -75772,7 +75756,7 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="117" t="s">
-        <v>2106</v>
+        <v>2105</v>
       </c>
       <c r="C120" s="53">
         <v>163</v>
@@ -75780,7 +75764,7 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="117" t="s">
-        <v>2107</v>
+        <v>2106</v>
       </c>
       <c r="D121" s="53">
         <v>164</v>
@@ -75788,7 +75772,7 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="117" t="s">
-        <v>2108</v>
+        <v>2107</v>
       </c>
       <c r="C122" s="53">
         <v>165</v>
@@ -75796,7 +75780,7 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="117" t="s">
-        <v>2109</v>
+        <v>2108</v>
       </c>
       <c r="D123" s="53">
         <v>166</v>
@@ -75804,7 +75788,7 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="117" t="s">
-        <v>2110</v>
+        <v>2109</v>
       </c>
       <c r="C124" s="53">
         <v>167</v>
@@ -75812,7 +75796,7 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="117" t="s">
-        <v>2111</v>
+        <v>2110</v>
       </c>
       <c r="D125" s="53">
         <v>168</v>
@@ -75820,7 +75804,7 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="117" t="s">
-        <v>2112</v>
+        <v>2111</v>
       </c>
       <c r="C126" s="53">
         <v>169</v>
@@ -75828,7 +75812,7 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="117" t="s">
-        <v>2113</v>
+        <v>2112</v>
       </c>
       <c r="D127" s="53">
         <v>170</v>
@@ -75836,7 +75820,7 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="117" t="s">
-        <v>2114</v>
+        <v>2113</v>
       </c>
       <c r="C128" s="53">
         <v>171</v>
@@ -75844,7 +75828,7 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="117" t="s">
-        <v>2115</v>
+        <v>2114</v>
       </c>
       <c r="D129" s="53">
         <v>172</v>
@@ -75852,7 +75836,7 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="117" t="s">
-        <v>2116</v>
+        <v>2115</v>
       </c>
       <c r="C130" s="53">
         <v>173</v>
@@ -75860,7 +75844,7 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="117" t="s">
-        <v>2117</v>
+        <v>2116</v>
       </c>
       <c r="D131" s="53">
         <v>174</v>
@@ -75868,7 +75852,7 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="117" t="s">
-        <v>2118</v>
+        <v>2117</v>
       </c>
       <c r="C132" s="53">
         <v>175</v>
@@ -75876,7 +75860,7 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="117" t="s">
-        <v>2119</v>
+        <v>2118</v>
       </c>
       <c r="D133" s="53">
         <v>176</v>
@@ -75884,7 +75868,7 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="117" t="s">
-        <v>2120</v>
+        <v>2119</v>
       </c>
       <c r="C134" s="53">
         <v>177</v>
@@ -75892,7 +75876,7 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="117" t="s">
-        <v>2121</v>
+        <v>2120</v>
       </c>
       <c r="D135" s="53">
         <v>178</v>
@@ -75900,7 +75884,7 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="117" t="s">
-        <v>2122</v>
+        <v>2121</v>
       </c>
       <c r="C136" s="53">
         <v>179</v>
@@ -75908,7 +75892,7 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="117" t="s">
-        <v>2123</v>
+        <v>2122</v>
       </c>
       <c r="D137" s="53">
         <v>180</v>
@@ -75916,7 +75900,7 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="117" t="s">
-        <v>2124</v>
+        <v>2123</v>
       </c>
       <c r="C138" s="53">
         <v>181</v>
@@ -75924,7 +75908,7 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="117" t="s">
-        <v>2125</v>
+        <v>2124</v>
       </c>
       <c r="D139" s="53">
         <v>182</v>
@@ -75932,7 +75916,7 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="117" t="s">
-        <v>2126</v>
+        <v>2125</v>
       </c>
       <c r="C140" s="53">
         <v>183</v>
@@ -75940,7 +75924,7 @@
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="117" t="s">
-        <v>2127</v>
+        <v>2126</v>
       </c>
       <c r="D141" s="53">
         <v>184</v>
@@ -75948,7 +75932,7 @@
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="117" t="s">
-        <v>2128</v>
+        <v>2127</v>
       </c>
       <c r="C142" s="53">
         <v>185</v>
@@ -75956,7 +75940,7 @@
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="117" t="s">
-        <v>2129</v>
+        <v>2128</v>
       </c>
       <c r="D143" s="53">
         <v>186</v>
@@ -75964,7 +75948,7 @@
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="117" t="s">
-        <v>2130</v>
+        <v>2129</v>
       </c>
       <c r="C144" s="53">
         <v>187</v>
@@ -75972,7 +75956,7 @@
     </row>
     <row r="145" spans="1:4">
       <c r="A145" s="117" t="s">
-        <v>2131</v>
+        <v>2130</v>
       </c>
       <c r="D145" s="53">
         <v>188</v>
@@ -75980,7 +75964,7 @@
     </row>
     <row r="146" spans="1:4">
       <c r="A146" s="117" t="s">
-        <v>2132</v>
+        <v>2131</v>
       </c>
       <c r="C146" s="53">
         <v>191</v>
@@ -75988,7 +75972,7 @@
     </row>
     <row r="147" spans="1:4">
       <c r="A147" s="117" t="s">
-        <v>2133</v>
+        <v>2132</v>
       </c>
       <c r="D147" s="53">
         <v>192</v>
@@ -75996,7 +75980,7 @@
     </row>
     <row r="148" spans="1:4">
       <c r="A148" s="117" t="s">
-        <v>2134</v>
+        <v>2133</v>
       </c>
       <c r="C148" s="53">
         <v>193</v>
@@ -76004,7 +75988,7 @@
     </row>
     <row r="149" spans="1:4">
       <c r="A149" s="117" t="s">
-        <v>2135</v>
+        <v>2134</v>
       </c>
       <c r="D149" s="53">
         <v>194</v>
@@ -76012,7 +75996,7 @@
     </row>
     <row r="150" spans="1:4">
       <c r="A150" s="117" t="s">
-        <v>2136</v>
+        <v>2135</v>
       </c>
       <c r="C150" s="53">
         <v>195</v>
@@ -76020,7 +76004,7 @@
     </row>
     <row r="151" spans="1:4">
       <c r="A151" s="117" t="s">
-        <v>2137</v>
+        <v>2136</v>
       </c>
       <c r="D151" s="53">
         <v>196</v>
@@ -76028,7 +76012,7 @@
     </row>
     <row r="152" spans="1:4">
       <c r="A152" s="117" t="s">
-        <v>2138</v>
+        <v>2137</v>
       </c>
       <c r="C152" s="53">
         <v>197</v>
@@ -76036,7 +76020,7 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="117" t="s">
-        <v>2139</v>
+        <v>2138</v>
       </c>
       <c r="D153" s="53">
         <v>198</v>
@@ -76044,7 +76028,7 @@
     </row>
     <row r="154" spans="1:4">
       <c r="A154" s="117" t="s">
-        <v>2140</v>
+        <v>2139</v>
       </c>
       <c r="C154" s="53">
         <v>199</v>
@@ -76052,7 +76036,7 @@
     </row>
     <row r="155" spans="1:4">
       <c r="A155" s="117" t="s">
-        <v>2141</v>
+        <v>2140</v>
       </c>
       <c r="D155" s="53">
         <v>200</v>
@@ -76060,7 +76044,7 @@
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="117" t="s">
-        <v>2142</v>
+        <v>2141</v>
       </c>
       <c r="C156" s="53">
         <v>201</v>
@@ -76068,7 +76052,7 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157" s="117" t="s">
-        <v>2143</v>
+        <v>2142</v>
       </c>
       <c r="D157" s="53">
         <v>202</v>
@@ -76076,7 +76060,7 @@
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="117" t="s">
-        <v>2144</v>
+        <v>2143</v>
       </c>
       <c r="C158" s="53">
         <v>203</v>
@@ -76084,7 +76068,7 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" s="117" t="s">
-        <v>2145</v>
+        <v>2144</v>
       </c>
       <c r="D159" s="53">
         <v>204</v>
@@ -76092,7 +76076,7 @@
     </row>
     <row r="160" spans="1:4">
       <c r="A160" s="117" t="s">
-        <v>2146</v>
+        <v>2145</v>
       </c>
       <c r="C160" s="53">
         <v>205</v>
@@ -76100,7 +76084,7 @@
     </row>
     <row r="161" spans="1:4">
       <c r="A161" s="117" t="s">
-        <v>2147</v>
+        <v>2146</v>
       </c>
       <c r="D161" s="53">
         <v>206</v>
@@ -76108,7 +76092,7 @@
     </row>
     <row r="162" spans="1:4">
       <c r="A162" s="117" t="s">
-        <v>2148</v>
+        <v>2147</v>
       </c>
       <c r="C162" s="53">
         <v>207</v>
@@ -76116,7 +76100,7 @@
     </row>
     <row r="163" spans="1:4">
       <c r="A163" s="117" t="s">
-        <v>2149</v>
+        <v>2148</v>
       </c>
       <c r="D163" s="53">
         <v>208</v>
@@ -76292,7 +76276,7 @@
     </row>
     <row r="185" spans="1:4">
       <c r="A185" s="117" t="s">
-        <v>2043</v>
+        <v>2042</v>
       </c>
       <c r="B185" s="53">
         <v>87</v>
@@ -76300,7 +76284,7 @@
     </row>
     <row r="186" spans="1:4">
       <c r="A186" s="117" t="s">
-        <v>2050</v>
+        <v>2049</v>
       </c>
       <c r="C186" s="53">
         <v>96</v>
@@ -76308,7 +76292,7 @@
     </row>
     <row r="187" spans="1:4">
       <c r="A187" s="117" t="s">
-        <v>2051</v>
+        <v>2050</v>
       </c>
       <c r="D187" s="53">
         <v>97</v>
@@ -76316,7 +76300,7 @@
     </row>
     <row r="188" spans="1:4">
       <c r="A188" s="117" t="s">
-        <v>2150</v>
+        <v>2149</v>
       </c>
       <c r="D188" s="53">
         <v>76</v>
@@ -76340,7 +76324,7 @@
   <dimension ref="A1:B163"/>
   <sheetViews>
     <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:B38"/>
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -76353,10 +76337,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="60" customFormat="1">
       <c r="A1" s="58" t="s">
+        <v>2150</v>
+      </c>
+      <c r="B1" s="59" t="s">
         <v>2151</v>
-      </c>
-      <c r="B1" s="59" t="s">
-        <v>2152</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -76769,7 +76753,7 @@
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>2039</v>
+        <v>2038</v>
       </c>
       <c r="B53" s="61">
         <v>83</v>
@@ -76777,7 +76761,7 @@
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>2040</v>
+        <v>2039</v>
       </c>
       <c r="B54" s="61">
         <v>84</v>
@@ -76785,7 +76769,7 @@
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>2041</v>
+        <v>2040</v>
       </c>
       <c r="B55" s="61">
         <v>85</v>
@@ -76793,7 +76777,7 @@
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>2042</v>
+        <v>2041</v>
       </c>
       <c r="B56" s="61">
         <v>86</v>
@@ -76801,7 +76785,7 @@
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>2043</v>
+        <v>2042</v>
       </c>
       <c r="B57" s="61">
         <v>87</v>
@@ -76809,7 +76793,7 @@
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>2044</v>
+        <v>2043</v>
       </c>
       <c r="B58" s="61">
         <v>89</v>
@@ -76817,7 +76801,7 @@
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>2045</v>
+        <v>2044</v>
       </c>
       <c r="B59" s="61">
         <v>90</v>
@@ -76825,7 +76809,7 @@
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>2046</v>
+        <v>2045</v>
       </c>
       <c r="B60" s="61">
         <v>91</v>
@@ -76833,7 +76817,7 @@
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
       <c r="B61" s="61">
         <v>92</v>
@@ -76841,7 +76825,7 @@
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>2048</v>
+        <v>2047</v>
       </c>
       <c r="B62" s="61">
         <v>93</v>
@@ -76849,7 +76833,7 @@
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>2049</v>
+        <v>2048</v>
       </c>
       <c r="B63" s="61">
         <v>94</v>
@@ -76857,7 +76841,7 @@
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>2050</v>
+        <v>2049</v>
       </c>
       <c r="B64" s="61">
         <v>96</v>
@@ -76865,7 +76849,7 @@
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>2051</v>
+        <v>2050</v>
       </c>
       <c r="B65" s="61">
         <v>97</v>
@@ -76873,7 +76857,7 @@
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
       <c r="B66" s="61">
         <v>101</v>
@@ -76881,7 +76865,7 @@
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>2053</v>
+        <v>2052</v>
       </c>
       <c r="B67" s="61">
         <v>102</v>
@@ -76889,7 +76873,7 @@
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>2054</v>
+        <v>2053</v>
       </c>
       <c r="B68" s="61">
         <v>103</v>
@@ -76897,7 +76881,7 @@
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>2055</v>
+        <v>2054</v>
       </c>
       <c r="B69" s="61">
         <v>104</v>
@@ -76905,7 +76889,7 @@
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
       <c r="B70" s="61">
         <v>105</v>
@@ -76913,7 +76897,7 @@
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>2057</v>
+        <v>2056</v>
       </c>
       <c r="B71" s="61">
         <v>106</v>
@@ -76921,7 +76905,7 @@
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>2058</v>
+        <v>2057</v>
       </c>
       <c r="B72" s="61">
         <v>107</v>
@@ -76929,7 +76913,7 @@
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>2059</v>
+        <v>2058</v>
       </c>
       <c r="B73" s="61">
         <v>108</v>
@@ -76937,7 +76921,7 @@
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="B74" s="61">
         <v>109</v>
@@ -76945,7 +76929,7 @@
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>2061</v>
+        <v>2060</v>
       </c>
       <c r="B75" s="61">
         <v>110</v>
@@ -76953,7 +76937,7 @@
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>2062</v>
+        <v>2061</v>
       </c>
       <c r="B76" s="61">
         <v>113</v>
@@ -76961,7 +76945,7 @@
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
       <c r="B77" s="61">
         <v>114</v>
@@ -76969,7 +76953,7 @@
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>2064</v>
+        <v>2063</v>
       </c>
       <c r="B78" s="61">
         <v>115</v>
@@ -76977,7 +76961,7 @@
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>2065</v>
+        <v>2064</v>
       </c>
       <c r="B79" s="61">
         <v>116</v>
@@ -76985,7 +76969,7 @@
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>2066</v>
+        <v>2065</v>
       </c>
       <c r="B80" s="61">
         <v>117</v>
@@ -76993,7 +76977,7 @@
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>2067</v>
+        <v>2066</v>
       </c>
       <c r="B81" s="61">
         <v>118</v>
@@ -77001,7 +76985,7 @@
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>2068</v>
+        <v>2067</v>
       </c>
       <c r="B82" s="61">
         <v>119</v>
@@ -77009,7 +76993,7 @@
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>2069</v>
+        <v>2068</v>
       </c>
       <c r="B83" s="61">
         <v>120</v>
@@ -77017,7 +77001,7 @@
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>2070</v>
+        <v>2069</v>
       </c>
       <c r="B84" s="61">
         <v>121</v>
@@ -77025,7 +77009,7 @@
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>2071</v>
+        <v>2070</v>
       </c>
       <c r="B85" s="61">
         <v>122</v>
@@ -77033,7 +77017,7 @@
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>2072</v>
+        <v>2071</v>
       </c>
       <c r="B86" s="61">
         <v>123</v>
@@ -77041,7 +77025,7 @@
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>2073</v>
+        <v>2072</v>
       </c>
       <c r="B87" s="61">
         <v>124</v>
@@ -77049,7 +77033,7 @@
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>2074</v>
+        <v>2073</v>
       </c>
       <c r="B88" s="61">
         <v>125</v>
@@ -77057,7 +77041,7 @@
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
       <c r="B89" s="61">
         <v>126</v>
@@ -77065,7 +77049,7 @@
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>2076</v>
+        <v>2075</v>
       </c>
       <c r="B90" s="61">
         <v>129</v>
@@ -77073,7 +77057,7 @@
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>2077</v>
+        <v>2076</v>
       </c>
       <c r="B91" s="61">
         <v>130</v>
@@ -77081,7 +77065,7 @@
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
-        <v>2078</v>
+        <v>2077</v>
       </c>
       <c r="B92" s="61">
         <v>133</v>
@@ -77089,7 +77073,7 @@
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>2079</v>
+        <v>2078</v>
       </c>
       <c r="B93" s="61">
         <v>134</v>
@@ -77097,7 +77081,7 @@
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>2080</v>
+        <v>2079</v>
       </c>
       <c r="B94" s="61">
         <v>135</v>
@@ -77105,7 +77089,7 @@
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>2081</v>
+        <v>2080</v>
       </c>
       <c r="B95" s="61">
         <v>136</v>
@@ -77113,7 +77097,7 @@
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>2082</v>
+        <v>2081</v>
       </c>
       <c r="B96" s="61">
         <v>137</v>
@@ -77121,7 +77105,7 @@
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>2083</v>
+        <v>2082</v>
       </c>
       <c r="B97" s="61">
         <v>138</v>
@@ -77129,7 +77113,7 @@
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>2084</v>
+        <v>2083</v>
       </c>
       <c r="B98" s="61">
         <v>139</v>
@@ -77137,7 +77121,7 @@
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>2085</v>
+        <v>2084</v>
       </c>
       <c r="B99" s="61">
         <v>140</v>
@@ -77145,7 +77129,7 @@
     </row>
     <row r="100" spans="1:2" s="62" customFormat="1">
       <c r="A100" t="s">
-        <v>2086</v>
+        <v>2085</v>
       </c>
       <c r="B100" s="61">
         <v>141</v>
@@ -77153,7 +77137,7 @@
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>2087</v>
+        <v>2086</v>
       </c>
       <c r="B101" s="61">
         <v>142</v>
@@ -77161,7 +77145,7 @@
     </row>
     <row r="102" spans="1:2">
       <c r="A102" t="s">
-        <v>2088</v>
+        <v>2087</v>
       </c>
       <c r="B102" s="61">
         <v>143</v>
@@ -77169,7 +77153,7 @@
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>2089</v>
+        <v>2088</v>
       </c>
       <c r="B103" s="61">
         <v>144</v>
@@ -77177,7 +77161,7 @@
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>2090</v>
+        <v>2089</v>
       </c>
       <c r="B104" s="61">
         <v>145</v>
@@ -77185,7 +77169,7 @@
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>2091</v>
+        <v>2090</v>
       </c>
       <c r="B105" s="61">
         <v>146</v>
@@ -77193,7 +77177,7 @@
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>2092</v>
+        <v>2091</v>
       </c>
       <c r="B106" s="61">
         <v>147</v>
@@ -77201,7 +77185,7 @@
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>2093</v>
+        <v>2092</v>
       </c>
       <c r="B107" s="61">
         <v>148</v>
@@ -77209,7 +77193,7 @@
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>2094</v>
+        <v>2093</v>
       </c>
       <c r="B108" s="61">
         <v>149</v>
@@ -77217,7 +77201,7 @@
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>2095</v>
+        <v>2094</v>
       </c>
       <c r="B109" s="61">
         <v>150</v>
@@ -77225,7 +77209,7 @@
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="B110" s="61">
         <v>151</v>
@@ -77233,7 +77217,7 @@
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="s">
-        <v>2097</v>
+        <v>2096</v>
       </c>
       <c r="B111" s="61">
         <v>152</v>
@@ -77241,7 +77225,7 @@
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
       <c r="B112" s="61">
         <v>153</v>
@@ -77249,7 +77233,7 @@
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
       <c r="B113" s="61">
         <v>154</v>
@@ -77257,7 +77241,7 @@
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>2100</v>
+        <v>2099</v>
       </c>
       <c r="B114" s="61">
         <v>155</v>
@@ -77265,7 +77249,7 @@
     </row>
     <row r="115" spans="1:2">
       <c r="A115" t="s">
-        <v>2101</v>
+        <v>2100</v>
       </c>
       <c r="B115" s="61">
         <v>156</v>
@@ -77273,7 +77257,7 @@
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="B116" s="61">
         <v>157</v>
@@ -77281,7 +77265,7 @@
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>2103</v>
+        <v>2102</v>
       </c>
       <c r="B117" s="61">
         <v>158</v>
@@ -77289,7 +77273,7 @@
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>2104</v>
+        <v>2103</v>
       </c>
       <c r="B118" s="61">
         <v>161</v>
@@ -77297,7 +77281,7 @@
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="s">
-        <v>2105</v>
+        <v>2104</v>
       </c>
       <c r="B119" s="61">
         <v>162</v>
@@ -77305,7 +77289,7 @@
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="s">
-        <v>2106</v>
+        <v>2105</v>
       </c>
       <c r="B120" s="61">
         <v>163</v>
@@ -77313,7 +77297,7 @@
     </row>
     <row r="121" spans="1:2">
       <c r="A121" t="s">
-        <v>2107</v>
+        <v>2106</v>
       </c>
       <c r="B121" s="61">
         <v>164</v>
@@ -77321,7 +77305,7 @@
     </row>
     <row r="122" spans="1:2">
       <c r="A122" t="s">
-        <v>2108</v>
+        <v>2107</v>
       </c>
       <c r="B122" s="61">
         <v>165</v>
@@ -77329,7 +77313,7 @@
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
-        <v>2109</v>
+        <v>2108</v>
       </c>
       <c r="B123" s="61">
         <v>166</v>
@@ -77337,7 +77321,7 @@
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>2110</v>
+        <v>2109</v>
       </c>
       <c r="B124" s="61">
         <v>167</v>
@@ -77345,7 +77329,7 @@
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>2111</v>
+        <v>2110</v>
       </c>
       <c r="B125" s="61">
         <v>168</v>
@@ -77353,7 +77337,7 @@
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>2112</v>
+        <v>2111</v>
       </c>
       <c r="B126" s="61">
         <v>169</v>
@@ -77361,7 +77345,7 @@
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>2113</v>
+        <v>2112</v>
       </c>
       <c r="B127" s="61">
         <v>170</v>
@@ -77369,7 +77353,7 @@
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>2114</v>
+        <v>2113</v>
       </c>
       <c r="B128" s="61">
         <v>171</v>
@@ -77377,7 +77361,7 @@
     </row>
     <row r="129" spans="1:2">
       <c r="A129" t="s">
-        <v>2115</v>
+        <v>2114</v>
       </c>
       <c r="B129" s="61">
         <v>172</v>
@@ -77385,7 +77369,7 @@
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>2116</v>
+        <v>2115</v>
       </c>
       <c r="B130" s="61">
         <v>173</v>
@@ -77393,7 +77377,7 @@
     </row>
     <row r="131" spans="1:2">
       <c r="A131" t="s">
-        <v>2117</v>
+        <v>2116</v>
       </c>
       <c r="B131" s="61">
         <v>174</v>
@@ -77401,7 +77385,7 @@
     </row>
     <row r="132" spans="1:2">
       <c r="A132" t="s">
-        <v>2118</v>
+        <v>2117</v>
       </c>
       <c r="B132" s="61">
         <v>175</v>
@@ -77409,7 +77393,7 @@
     </row>
     <row r="133" spans="1:2">
       <c r="A133" t="s">
-        <v>2119</v>
+        <v>2118</v>
       </c>
       <c r="B133" s="61">
         <v>176</v>
@@ -77417,7 +77401,7 @@
     </row>
     <row r="134" spans="1:2">
       <c r="A134" t="s">
-        <v>2120</v>
+        <v>2119</v>
       </c>
       <c r="B134" s="61">
         <v>177</v>
@@ -77425,7 +77409,7 @@
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>2121</v>
+        <v>2120</v>
       </c>
       <c r="B135" s="61">
         <v>178</v>
@@ -77433,7 +77417,7 @@
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>2122</v>
+        <v>2121</v>
       </c>
       <c r="B136" s="61">
         <v>179</v>
@@ -77441,7 +77425,7 @@
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>2123</v>
+        <v>2122</v>
       </c>
       <c r="B137" s="53">
         <v>180</v>
@@ -77449,7 +77433,7 @@
     </row>
     <row r="138" spans="1:2">
       <c r="A138" t="s">
-        <v>2124</v>
+        <v>2123</v>
       </c>
       <c r="B138" s="53">
         <v>181</v>
@@ -77457,7 +77441,7 @@
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>2125</v>
+        <v>2124</v>
       </c>
       <c r="B139" s="53">
         <v>182</v>
@@ -77465,7 +77449,7 @@
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>2126</v>
+        <v>2125</v>
       </c>
       <c r="B140" s="53">
         <v>183</v>
@@ -77473,7 +77457,7 @@
     </row>
     <row r="141" spans="1:2">
       <c r="A141" t="s">
-        <v>2127</v>
+        <v>2126</v>
       </c>
       <c r="B141" s="53">
         <v>184</v>
@@ -77481,7 +77465,7 @@
     </row>
     <row r="142" spans="1:2">
       <c r="A142" t="s">
-        <v>2128</v>
+        <v>2127</v>
       </c>
       <c r="B142" s="53">
         <v>185</v>
@@ -77489,7 +77473,7 @@
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>2129</v>
+        <v>2128</v>
       </c>
       <c r="B143" s="53">
         <v>186</v>
@@ -77497,7 +77481,7 @@
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>2130</v>
+        <v>2129</v>
       </c>
       <c r="B144" s="53">
         <v>187</v>
@@ -77505,7 +77489,7 @@
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>2131</v>
+        <v>2130</v>
       </c>
       <c r="B145" s="53">
         <v>188</v>
@@ -77513,7 +77497,7 @@
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>2132</v>
+        <v>2131</v>
       </c>
       <c r="B146" s="53">
         <v>191</v>
@@ -77521,7 +77505,7 @@
     </row>
     <row r="147" spans="1:2">
       <c r="A147" t="s">
-        <v>2133</v>
+        <v>2132</v>
       </c>
       <c r="B147" s="53">
         <v>192</v>
@@ -77529,7 +77513,7 @@
     </row>
     <row r="148" spans="1:2">
       <c r="A148" t="s">
-        <v>2134</v>
+        <v>2133</v>
       </c>
       <c r="B148" s="53">
         <v>193</v>
@@ -77537,7 +77521,7 @@
     </row>
     <row r="149" spans="1:2">
       <c r="A149" t="s">
-        <v>2135</v>
+        <v>2134</v>
       </c>
       <c r="B149" s="53">
         <v>194</v>
@@ -77545,7 +77529,7 @@
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>2136</v>
+        <v>2135</v>
       </c>
       <c r="B150" s="53">
         <v>195</v>
@@ -77553,7 +77537,7 @@
     </row>
     <row r="151" spans="1:2">
       <c r="A151" t="s">
-        <v>2137</v>
+        <v>2136</v>
       </c>
       <c r="B151" s="53">
         <v>196</v>
@@ -77561,7 +77545,7 @@
     </row>
     <row r="152" spans="1:2">
       <c r="A152" t="s">
-        <v>2138</v>
+        <v>2137</v>
       </c>
       <c r="B152" s="53">
         <v>197</v>
@@ -77569,7 +77553,7 @@
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>2139</v>
+        <v>2138</v>
       </c>
       <c r="B153" s="53">
         <v>198</v>
@@ -77577,7 +77561,7 @@
     </row>
     <row r="154" spans="1:2">
       <c r="A154" t="s">
-        <v>2140</v>
+        <v>2139</v>
       </c>
       <c r="B154" s="53">
         <v>199</v>
@@ -77585,7 +77569,7 @@
     </row>
     <row r="155" spans="1:2">
       <c r="A155" t="s">
-        <v>2141</v>
+        <v>2140</v>
       </c>
       <c r="B155" s="53">
         <v>200</v>
@@ -77593,7 +77577,7 @@
     </row>
     <row r="156" spans="1:2">
       <c r="A156" t="s">
-        <v>2142</v>
+        <v>2141</v>
       </c>
       <c r="B156" s="53">
         <v>201</v>
@@ -77601,7 +77585,7 @@
     </row>
     <row r="157" spans="1:2">
       <c r="A157" t="s">
-        <v>2143</v>
+        <v>2142</v>
       </c>
       <c r="B157" s="53">
         <v>202</v>
@@ -77609,7 +77593,7 @@
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>2144</v>
+        <v>2143</v>
       </c>
       <c r="B158" s="53">
         <v>203</v>
@@ -77617,7 +77601,7 @@
     </row>
     <row r="159" spans="1:2">
       <c r="A159" t="s">
-        <v>2145</v>
+        <v>2144</v>
       </c>
       <c r="B159" s="53">
         <v>204</v>
@@ -77625,7 +77609,7 @@
     </row>
     <row r="160" spans="1:2">
       <c r="A160" t="s">
-        <v>2146</v>
+        <v>2145</v>
       </c>
       <c r="B160" s="53">
         <v>205</v>
@@ -77633,7 +77617,7 @@
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>2147</v>
+        <v>2146</v>
       </c>
       <c r="B161" s="53">
         <v>206</v>
@@ -77641,7 +77625,7 @@
     </row>
     <row r="162" spans="1:2">
       <c r="A162" t="s">
-        <v>2148</v>
+        <v>2147</v>
       </c>
       <c r="B162" s="53">
         <v>207</v>
@@ -77649,7 +77633,7 @@
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
-        <v>2149</v>
+        <v>2148</v>
       </c>
       <c r="B163" s="53">
         <v>208</v>
@@ -77678,10 +77662,10 @@
   <sheetData>
     <row r="1" spans="1:3" s="60" customFormat="1">
       <c r="A1" s="58" t="s">
+        <v>2150</v>
+      </c>
+      <c r="B1" s="59" t="s">
         <v>2151</v>
-      </c>
-      <c r="B1" s="59" t="s">
-        <v>2152</v>
       </c>
       <c r="C1" s="52"/>
     </row>
@@ -77875,7 +77859,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>2043</v>
+        <v>2042</v>
       </c>
       <c r="B23" s="61">
         <v>87</v>
@@ -77883,7 +77867,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>2050</v>
+        <v>2049</v>
       </c>
       <c r="B24" s="61">
         <v>96</v>
@@ -77891,7 +77875,7 @@
     </row>
     <row r="25" spans="1:3" s="54" customFormat="1">
       <c r="A25" t="s">
-        <v>2051</v>
+        <v>2050</v>
       </c>
       <c r="B25" s="61">
         <v>97</v>
@@ -77900,7 +77884,7 @@
     </row>
     <row r="26" spans="1:3" s="54" customFormat="1">
       <c r="A26" t="s">
-        <v>2150</v>
+        <v>2149</v>
       </c>
       <c r="B26" s="61">
         <v>76</v>
@@ -78151,7 +78135,7 @@
     </row>
     <row r="7" spans="1:23">
       <c r="A7" t="s">
-        <v>2066</v>
+        <v>2065</v>
       </c>
       <c r="B7" s="61">
         <v>117</v>
@@ -78175,7 +78159,7 @@
     </row>
     <row r="8" spans="1:23">
       <c r="A8" t="s">
-        <v>2067</v>
+        <v>2066</v>
       </c>
       <c r="B8" s="61">
         <v>118</v>
@@ -78199,7 +78183,7 @@
     </row>
     <row r="9" spans="1:23">
       <c r="A9" t="s">
-        <v>2072</v>
+        <v>2071</v>
       </c>
       <c r="B9" s="61">
         <v>123</v>
@@ -78225,7 +78209,7 @@
     </row>
     <row r="10" spans="1:23">
       <c r="A10" t="s">
-        <v>2073</v>
+        <v>2072</v>
       </c>
       <c r="B10" s="61">
         <v>124</v>
@@ -78251,7 +78235,7 @@
     </row>
     <row r="11" spans="1:23">
       <c r="A11" t="s">
-        <v>2078</v>
+        <v>2077</v>
       </c>
       <c r="B11" s="61">
         <v>133</v>
@@ -78276,7 +78260,7 @@
     </row>
     <row r="12" spans="1:23">
       <c r="A12" t="s">
-        <v>2079</v>
+        <v>2078</v>
       </c>
       <c r="B12" s="61">
         <v>134</v>
@@ -78301,7 +78285,7 @@
     </row>
     <row r="13" spans="1:23">
       <c r="A13" t="s">
-        <v>2100</v>
+        <v>2099</v>
       </c>
       <c r="B13" s="61">
         <v>155</v>
@@ -78323,7 +78307,7 @@
     </row>
     <row r="14" spans="1:23">
       <c r="A14" t="s">
-        <v>2101</v>
+        <v>2100</v>
       </c>
       <c r="B14" s="61">
         <v>156</v>
@@ -78345,7 +78329,7 @@
     </row>
     <row r="15" spans="1:23">
       <c r="A15" t="s">
-        <v>2114</v>
+        <v>2113</v>
       </c>
       <c r="B15" s="61">
         <v>171</v>
@@ -78374,7 +78358,7 @@
     </row>
     <row r="16" spans="1:23">
       <c r="A16" t="s">
-        <v>2115</v>
+        <v>2114</v>
       </c>
       <c r="B16" s="61">
         <v>172</v>
@@ -78403,7 +78387,7 @@
     </row>
     <row r="17" spans="1:24">
       <c r="A17" t="s">
-        <v>2124</v>
+        <v>2123</v>
       </c>
       <c r="B17" s="53">
         <v>181</v>
@@ -78428,7 +78412,7 @@
     </row>
     <row r="18" spans="1:24">
       <c r="A18" t="s">
-        <v>2125</v>
+        <v>2124</v>
       </c>
       <c r="B18" s="53">
         <v>182</v>
@@ -78453,7 +78437,7 @@
     </row>
     <row r="19" spans="1:24">
       <c r="A19" t="s">
-        <v>2128</v>
+        <v>2127</v>
       </c>
       <c r="B19" s="53">
         <v>185</v>
@@ -78475,7 +78459,7 @@
     </row>
     <row r="20" spans="1:24">
       <c r="A20" t="s">
-        <v>2129</v>
+        <v>2128</v>
       </c>
       <c r="B20" s="53">
         <v>186</v>
@@ -78495,7 +78479,7 @@
     </row>
     <row r="21" spans="1:24">
       <c r="A21" t="s">
-        <v>2142</v>
+        <v>2141</v>
       </c>
       <c r="B21" s="53">
         <v>201</v>
@@ -78515,7 +78499,7 @@
     </row>
     <row r="22" spans="1:24">
       <c r="A22" t="s">
-        <v>2143</v>
+        <v>2142</v>
       </c>
       <c r="B22" s="53">
         <v>202</v>
@@ -78535,7 +78519,7 @@
     </row>
     <row r="23" spans="1:24">
       <c r="A23" t="s">
-        <v>2144</v>
+        <v>2143</v>
       </c>
       <c r="B23" s="53">
         <v>203</v>
@@ -78549,7 +78533,7 @@
     </row>
     <row r="24" spans="1:24">
       <c r="A24" t="s">
-        <v>2145</v>
+        <v>2144</v>
       </c>
       <c r="B24" s="53">
         <v>204</v>
@@ -78563,7 +78547,7 @@
     </row>
     <row r="25" spans="1:24">
       <c r="A25" t="s">
-        <v>2148</v>
+        <v>2147</v>
       </c>
       <c r="B25" s="53">
         <v>207</v>
@@ -78583,7 +78567,7 @@
     </row>
     <row r="26" spans="1:24">
       <c r="A26" t="s">
-        <v>2149</v>
+        <v>2148</v>
       </c>
       <c r="B26" s="53">
         <v>208</v>
@@ -78934,7 +78918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AG324"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="AG52" sqref="C52:AG52"/>
     </sheetView>
   </sheetViews>
@@ -79028,7 +79012,7 @@
         <v>57</v>
       </c>
       <c r="R2" s="25" t="s">
-        <v>2153</v>
+        <v>2152</v>
       </c>
       <c r="S2" s="25" t="s">
         <v>58</v>
@@ -79055,7 +79039,7 @@
         <v>65</v>
       </c>
       <c r="AA2" s="25" t="s">
-        <v>2154</v>
+        <v>2153</v>
       </c>
       <c r="AB2" s="25" t="s">
         <v>66</v>
@@ -79078,7 +79062,7 @@
     </row>
     <row r="5" spans="1:33">
       <c r="A5" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
       <c r="B5" s="61">
         <v>105</v>
@@ -79100,7 +79084,7 @@
     </row>
     <row r="6" spans="1:33">
       <c r="A6" t="s">
-        <v>2057</v>
+        <v>2056</v>
       </c>
       <c r="B6" s="61">
         <v>106</v>
@@ -79122,7 +79106,7 @@
     </row>
     <row r="7" spans="1:33">
       <c r="A7" t="s">
-        <v>2068</v>
+        <v>2067</v>
       </c>
       <c r="B7" s="61">
         <v>119</v>
@@ -79138,7 +79122,7 @@
     </row>
     <row r="8" spans="1:33">
       <c r="A8" t="s">
-        <v>2069</v>
+        <v>2068</v>
       </c>
       <c r="B8" s="61">
         <v>120</v>
@@ -79154,7 +79138,7 @@
     </row>
     <row r="9" spans="1:33">
       <c r="A9" t="s">
-        <v>2070</v>
+        <v>2069</v>
       </c>
       <c r="B9" s="61">
         <v>121</v>
@@ -79181,7 +79165,7 @@
     </row>
     <row r="10" spans="1:33">
       <c r="A10" t="s">
-        <v>2071</v>
+        <v>2070</v>
       </c>
       <c r="B10" s="61">
         <v>122</v>
@@ -79208,7 +79192,7 @@
     </row>
     <row r="11" spans="1:33">
       <c r="A11" s="119" t="s">
-        <v>2074</v>
+        <v>2073</v>
       </c>
       <c r="B11" s="61">
         <v>125</v>
@@ -79226,7 +79210,7 @@
     </row>
     <row r="12" spans="1:33">
       <c r="A12" s="119" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
       <c r="B12" s="61">
         <v>126</v>
@@ -79244,7 +79228,7 @@
     </row>
     <row r="13" spans="1:33">
       <c r="A13" t="s">
-        <v>2082</v>
+        <v>2081</v>
       </c>
       <c r="B13" s="61">
         <v>137</v>
@@ -79266,7 +79250,7 @@
     </row>
     <row r="14" spans="1:33">
       <c r="A14" t="s">
-        <v>2083</v>
+        <v>2082</v>
       </c>
       <c r="B14" s="61">
         <v>138</v>
@@ -79288,7 +79272,7 @@
     </row>
     <row r="15" spans="1:33">
       <c r="A15" s="68" t="s">
-        <v>2086</v>
+        <v>2085</v>
       </c>
       <c r="B15" s="61">
         <v>141</v>
@@ -79304,7 +79288,7 @@
     </row>
     <row r="16" spans="1:33">
       <c r="A16" s="68" t="s">
-        <v>2087</v>
+        <v>2086</v>
       </c>
       <c r="B16" s="61">
         <v>142</v>
@@ -79319,7 +79303,7 @@
     </row>
     <row r="17" spans="1:27">
       <c r="A17" t="s">
-        <v>2088</v>
+        <v>2087</v>
       </c>
       <c r="B17" s="61">
         <v>143</v>
@@ -79343,7 +79327,7 @@
     </row>
     <row r="18" spans="1:27">
       <c r="A18" t="s">
-        <v>2089</v>
+        <v>2088</v>
       </c>
       <c r="B18" s="61">
         <v>144</v>
@@ -79367,7 +79351,7 @@
     </row>
     <row r="19" spans="1:27">
       <c r="A19" t="s">
-        <v>2092</v>
+        <v>2091</v>
       </c>
       <c r="B19" s="61">
         <v>147</v>
@@ -79388,7 +79372,7 @@
     </row>
     <row r="20" spans="1:27">
       <c r="A20" t="s">
-        <v>2093</v>
+        <v>2092</v>
       </c>
       <c r="B20" s="61">
         <v>148</v>
@@ -79409,7 +79393,7 @@
     </row>
     <row r="21" spans="1:27">
       <c r="A21" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="B21" s="61">
         <v>151</v>
@@ -79425,7 +79409,7 @@
     </row>
     <row r="22" spans="1:27">
       <c r="A22" t="s">
-        <v>2097</v>
+        <v>2096</v>
       </c>
       <c r="B22" s="61">
         <v>152</v>
@@ -79441,7 +79425,7 @@
     </row>
     <row r="23" spans="1:27">
       <c r="A23" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
       <c r="B23" s="61">
         <v>153</v>
@@ -79456,7 +79440,7 @@
     </row>
     <row r="24" spans="1:27">
       <c r="A24" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
       <c r="B24" s="61">
         <v>154</v>
@@ -79471,7 +79455,7 @@
     </row>
     <row r="25" spans="1:27">
       <c r="A25" t="s">
-        <v>2106</v>
+        <v>2105</v>
       </c>
       <c r="B25" s="61">
         <v>163</v>
@@ -79489,7 +79473,7 @@
     </row>
     <row r="26" spans="1:27">
       <c r="A26" t="s">
-        <v>2107</v>
+        <v>2106</v>
       </c>
       <c r="B26" s="61">
         <v>164</v>
@@ -79507,7 +79491,7 @@
     </row>
     <row r="27" spans="1:27">
       <c r="A27" t="s">
-        <v>2108</v>
+        <v>2107</v>
       </c>
       <c r="B27" s="61">
         <v>165</v>
@@ -79525,7 +79509,7 @@
     </row>
     <row r="28" spans="1:27">
       <c r="A28" t="s">
-        <v>2109</v>
+        <v>2108</v>
       </c>
       <c r="B28" s="61">
         <v>166</v>
@@ -79543,7 +79527,7 @@
     </row>
     <row r="29" spans="1:27">
       <c r="A29" t="s">
-        <v>2122</v>
+        <v>2121</v>
       </c>
       <c r="B29" s="61">
         <v>179</v>
@@ -79564,7 +79548,7 @@
     </row>
     <row r="30" spans="1:27">
       <c r="A30" t="s">
-        <v>2123</v>
+        <v>2122</v>
       </c>
       <c r="B30" s="53">
         <v>180</v>
@@ -79585,7 +79569,7 @@
     </row>
     <row r="31" spans="1:27">
       <c r="A31" t="s">
-        <v>2126</v>
+        <v>2125</v>
       </c>
       <c r="B31" s="53">
         <v>183</v>
@@ -79604,7 +79588,7 @@
     </row>
     <row r="32" spans="1:27">
       <c r="A32" t="s">
-        <v>2127</v>
+        <v>2126</v>
       </c>
       <c r="B32" s="53">
         <v>184</v>
@@ -79623,7 +79607,7 @@
     </row>
     <row r="33" spans="1:33">
       <c r="A33" s="66" t="s">
-        <v>2130</v>
+        <v>2129</v>
       </c>
       <c r="B33" s="53">
         <v>187</v>
@@ -79635,7 +79619,7 @@
     </row>
     <row r="34" spans="1:33">
       <c r="A34" s="66" t="s">
-        <v>2131</v>
+        <v>2130</v>
       </c>
       <c r="B34" s="53">
         <v>188</v>
@@ -79647,7 +79631,7 @@
     </row>
     <row r="35" spans="1:33">
       <c r="A35" t="s">
-        <v>2132</v>
+        <v>2131</v>
       </c>
       <c r="B35" s="53">
         <v>191</v>
@@ -79666,7 +79650,7 @@
     </row>
     <row r="36" spans="1:33">
       <c r="A36" t="s">
-        <v>2133</v>
+        <v>2132</v>
       </c>
       <c r="B36" s="53">
         <v>192</v>
@@ -79685,7 +79669,7 @@
     </row>
     <row r="37" spans="1:33">
       <c r="A37" t="s">
-        <v>2134</v>
+        <v>2133</v>
       </c>
       <c r="B37" s="53">
         <v>193</v>
@@ -79724,7 +79708,7 @@
     </row>
     <row r="38" spans="1:33">
       <c r="A38" t="s">
-        <v>2135</v>
+        <v>2134</v>
       </c>
       <c r="B38" s="53">
         <v>194</v>
@@ -79763,7 +79747,7 @@
     </row>
     <row r="39" spans="1:33">
       <c r="A39" t="s">
-        <v>2146</v>
+        <v>2145</v>
       </c>
       <c r="B39" s="53">
         <v>205</v>
@@ -79781,7 +79765,7 @@
     </row>
     <row r="40" spans="1:33">
       <c r="A40" t="s">
-        <v>2147</v>
+        <v>2146</v>
       </c>
       <c r="B40" s="53">
         <v>206</v>
@@ -80063,7 +80047,7 @@
         <v>83</v>
       </c>
       <c r="G2" s="120" t="s">
-        <v>2155</v>
+        <v>2154</v>
       </c>
       <c r="H2" s="71" t="s">
         <v>85</v>
@@ -80080,7 +80064,7 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>2058</v>
+        <v>2057</v>
       </c>
       <c r="B3" s="61">
         <v>107</v>
@@ -80103,7 +80087,7 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>2059</v>
+        <v>2058</v>
       </c>
       <c r="B4" s="61">
         <v>108</v>
@@ -80120,7 +80104,7 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="66" t="s">
-        <v>2062</v>
+        <v>2061</v>
       </c>
       <c r="B5" s="61">
         <v>113</v>
@@ -80132,7 +80116,7 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="66" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
       <c r="B6" s="61">
         <v>114</v>
@@ -80144,7 +80128,7 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>2094</v>
+        <v>2093</v>
       </c>
       <c r="B7" s="61">
         <v>149</v>
@@ -80158,7 +80142,7 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>2095</v>
+        <v>2094</v>
       </c>
       <c r="B8" s="61">
         <v>150</v>
@@ -80172,7 +80156,7 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>2112</v>
+        <v>2111</v>
       </c>
       <c r="B9" s="61">
         <v>169</v>
@@ -80187,7 +80171,7 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>2113</v>
+        <v>2112</v>
       </c>
       <c r="B10" s="61">
         <v>170</v>
@@ -80202,7 +80186,7 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>2118</v>
+        <v>2117</v>
       </c>
       <c r="B11" s="61">
         <v>175</v>
@@ -80217,7 +80201,7 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>2119</v>
+        <v>2118</v>
       </c>
       <c r="B12" s="61">
         <v>176</v>
@@ -80232,7 +80216,7 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" t="s">
-        <v>2120</v>
+        <v>2119</v>
       </c>
       <c r="B13" s="61">
         <v>177</v>
@@ -80248,7 +80232,7 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" t="s">
-        <v>2121</v>
+        <v>2120</v>
       </c>
       <c r="B14" s="61">
         <v>178</v>
@@ -80263,7 +80247,7 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>2136</v>
+        <v>2135</v>
       </c>
       <c r="B15" s="53">
         <v>195</v>
@@ -80280,7 +80264,7 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>2137</v>
+        <v>2136</v>
       </c>
       <c r="B16" s="53">
         <v>196</v>
@@ -80297,7 +80281,7 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>2140</v>
+        <v>2139</v>
       </c>
       <c r="B17" s="53">
         <v>199</v>
@@ -80312,7 +80296,7 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>2141</v>
+        <v>2140</v>
       </c>
       <c r="B18" s="53">
         <v>200</v>
@@ -80327,7 +80311,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>2112</v>
+        <v>2111</v>
       </c>
       <c r="B19" s="61">
         <v>169</v>
@@ -80338,7 +80322,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>2113</v>
+        <v>2112</v>
       </c>
       <c r="B20" s="61">
         <v>170</v>
@@ -80349,7 +80333,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="117" t="s">
-        <v>2042</v>
+        <v>2041</v>
       </c>
       <c r="B21" s="53">
         <v>86</v>
@@ -80360,7 +80344,7 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="117" t="s">
-        <v>2049</v>
+        <v>2048</v>
       </c>
       <c r="B22" s="53">
         <v>94</v>

</xml_diff>

<commit_message>
update data to remove decimal points
</commit_message>
<xml_diff>
--- a/resources/syst_review_single_table.xlsx
+++ b/resources/syst_review_single_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\AnacondaProjects\PhD\Semiology-Visualisation-Tool\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0564EB-E5BB-4E77-AB79-5245DCAB810A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFFA6E94-C829-4BF1-893B-0EB8B55C3F61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -9171,73 +9171,73 @@
                   <c:v>1041</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1109.5</c:v>
+                  <c:v>1110</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1119.5</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00">
-                  <c:v>1152.5</c:v>
+                  <c:v>1153</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1157.5</c:v>
+                  <c:v>1158</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1182.5</c:v>
+                  <c:v>1183</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1280.5</c:v>
+                  <c:v>1281</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1357.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1388.5</c:v>
+                  <c:v>1389</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1497.5</c:v>
+                  <c:v>1498</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1552.5</c:v>
+                  <c:v>1553</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1643.5</c:v>
+                  <c:v>1644</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1683.5</c:v>
+                  <c:v>1684</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1695.5</c:v>
+                  <c:v>1696</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1835.5</c:v>
+                  <c:v>1836</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1885.5</c:v>
+                  <c:v>1886</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2355.5</c:v>
+                  <c:v>2356</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2363.5</c:v>
+                  <c:v>2364</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2363.5</c:v>
+                  <c:v>2364</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2363.5</c:v>
+                  <c:v>2364</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2434.5</c:v>
+                  <c:v>2435</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2669.5</c:v>
+                  <c:v>2670</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2938.5</c:v>
+                  <c:v>2939</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3174.5</c:v>
+                  <c:v>3175</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10393,11 +10393,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DU1102"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="F581" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J2" sqref="J2"/>
+      <selection pane="bottomRight" activeCell="F609" sqref="F609"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -19977,13 +19977,13 @@
       <c r="H198" s="41"/>
       <c r="I198" s="41"/>
       <c r="P198" s="5">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="R198" s="5">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="S198" s="5">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="DG198" s="5" t="s">
         <v>121</v>
@@ -73827,7 +73827,7 @@
       </c>
       <c r="G6" s="53">
         <f>SUM(Main!P2:P321)</f>
-        <v>1109.5</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="7" spans="1:13" s="53" customFormat="1">
@@ -73882,7 +73882,7 @@
       </c>
       <c r="G8" s="77">
         <f>SUM(Main!$P$2:P365)</f>
-        <v>1152.5</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="53" customFormat="1">
@@ -73910,7 +73910,7 @@
       </c>
       <c r="G9" s="53">
         <f>SUM(Main!$P$2:P370)</f>
-        <v>1157.5</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="10" spans="1:13" s="53" customFormat="1">
@@ -73938,7 +73938,7 @@
       </c>
       <c r="G10" s="53">
         <f>SUM(Main!$P$2:P398)</f>
-        <v>1182.5</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="11" spans="1:13" s="53" customFormat="1">
@@ -73966,7 +73966,7 @@
       </c>
       <c r="G11" s="53">
         <f>SUM(Main!$P$2:P428)</f>
-        <v>1280.5</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -74017,7 +74017,7 @@
       </c>
       <c r="G13" s="53">
         <f>SUM(Main!$P$2:P519)</f>
-        <v>1388.5</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="14" spans="1:13" s="53" customFormat="1">
@@ -74043,7 +74043,7 @@
       </c>
       <c r="G14" s="53">
         <f>SUM(Main!$P$2:P543)</f>
-        <v>1497.5</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="15" spans="1:13" s="53" customFormat="1">
@@ -74071,7 +74071,7 @@
       </c>
       <c r="G15" s="53">
         <f>SUM(Main!$P$2:P583)</f>
-        <v>1552.5</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="53" customFormat="1">
@@ -74099,7 +74099,7 @@
       </c>
       <c r="G16" s="53">
         <f>SUM(Main!$P$2:P610)</f>
-        <v>1643.5</v>
+        <v>1644</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -74127,7 +74127,7 @@
       </c>
       <c r="G17" s="53">
         <f>SUM(Main!$P$2:P648)</f>
-        <v>1683.5</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -74155,7 +74155,7 @@
       </c>
       <c r="G18" s="53">
         <f>SUM(Main!$P$2:P658)</f>
-        <v>1695.5</v>
+        <v>1696</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -74182,7 +74182,7 @@
       </c>
       <c r="G19" s="53">
         <f>SUM(Main!$P$2:P723)</f>
-        <v>1835.5</v>
+        <v>1836</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -74208,7 +74208,7 @@
       </c>
       <c r="G20" s="53">
         <f>SUM(Main!$P$2:P735)</f>
-        <v>1885.5</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -74234,7 +74234,7 @@
       </c>
       <c r="G21" s="53">
         <f>SUM(Main!$P$2:P754)</f>
-        <v>2355.5</v>
+        <v>2356</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -74260,7 +74260,7 @@
       </c>
       <c r="G22" s="53">
         <f>SUM(Main!$P$2:P770)</f>
-        <v>2363.5</v>
+        <v>2364</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -74286,7 +74286,7 @@
       </c>
       <c r="G23" s="53">
         <f>SUM(Main!$P$2:P770)</f>
-        <v>2363.5</v>
+        <v>2364</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -74312,7 +74312,7 @@
       </c>
       <c r="G24" s="53">
         <f>SUM(Main!$P$2:P770)</f>
-        <v>2363.5</v>
+        <v>2364</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -74338,7 +74338,7 @@
       </c>
       <c r="G25" s="53">
         <f>SUM(Main!$P$2:P813)</f>
-        <v>2434.5</v>
+        <v>2435</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -74364,7 +74364,7 @@
       </c>
       <c r="G26" s="53">
         <f>SUM(Main!$P$2:P885)</f>
-        <v>2669.5</v>
+        <v>2670</v>
       </c>
       <c r="H26" t="s">
         <v>1916</v>
@@ -74394,7 +74394,7 @@
       </c>
       <c r="G27" s="53">
         <f>SUM(Main!$P$2:P933)</f>
-        <v>2938.5</v>
+        <v>2939</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -74420,7 +74420,7 @@
       </c>
       <c r="G28" s="53">
         <f>SUM(Main!$P$2:P1038)</f>
-        <v>3174.5</v>
+        <v>3175</v>
       </c>
       <c r="H28" t="s">
         <v>1917</v>
@@ -74785,7 +74785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D189"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
remove duplicated precuneus in GIF PL mappings
</commit_message>
<xml_diff>
--- a/resources/syst_review_single_table.xlsx
+++ b/resources/syst_review_single_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\AnacondaProjects\PhD\Semiology-Visualisation-Tool\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2301A9D-56B6-4BDE-80EE-D869413FF17F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0519EB0C-BC0B-492E-97D5-18A222571757}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6991" uniqueCount="2158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6989" uniqueCount="2158">
   <si>
     <t xml:space="preserve">Semiology </t>
   </si>
@@ -10390,11 +10390,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DU1102"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="F581" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="AA724" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F609" sqref="F609"/>
+      <selection pane="bottomRight" activeCell="D744" sqref="D744:Q744"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -78915,7 +78915,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AG324"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="AI18" sqref="AI18"/>
     </sheetView>
   </sheetViews>
@@ -80084,10 +80084,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -80383,51 +80383,29 @@
       <c r="G18" s="53"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" t="s">
-        <v>2111</v>
-      </c>
-      <c r="B19" s="61">
-        <v>169</v>
-      </c>
-      <c r="C19" s="61">
-        <v>169</v>
+      <c r="A19" s="116" t="s">
+        <v>2041</v>
+      </c>
+      <c r="B19" s="53">
+        <v>86</v>
+      </c>
+      <c r="C19" s="53">
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" t="s">
-        <v>2112</v>
-      </c>
-      <c r="B20" s="61">
-        <v>170</v>
-      </c>
-      <c r="C20" s="61">
-        <v>170</v>
+      <c r="A20" s="116" t="s">
+        <v>2048</v>
+      </c>
+      <c r="B20" s="53">
+        <v>94</v>
+      </c>
+      <c r="C20" s="53">
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="116" t="s">
-        <v>2041</v>
-      </c>
-      <c r="B21" s="53">
-        <v>86</v>
-      </c>
-      <c r="C21" s="53">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="116" t="s">
-        <v>2048</v>
-      </c>
-      <c r="B22" s="53">
-        <v>94</v>
-      </c>
-      <c r="C22" s="53">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="B23" s="53"/>
+      <c r="B21" s="53"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
GIF FL mappings corrected prefrontal and premotor frontals using slicer segmentations
</commit_message>
<xml_diff>
--- a/resources/syst_review_single_table.xlsx
+++ b/resources/syst_review_single_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\AnacondaProjects\PhD\Semiology-Visualisation-Tool\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0519EB0C-BC0B-492E-97D5-18A222571757}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535155EB-1852-416C-A8B3-582C0426201F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -76320,7 +76320,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B163"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A101" workbookViewId="0">
       <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
@@ -78915,8 +78915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AG324"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AI18" sqref="AI18"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="M42" sqref="M42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -79068,9 +79068,7 @@
         <v>105</v>
       </c>
       <c r="D5" s="53"/>
-      <c r="E5" s="53">
-        <v>105</v>
-      </c>
+      <c r="E5" s="53"/>
       <c r="G5" s="5"/>
       <c r="H5" s="53">
         <v>105</v>
@@ -79090,9 +79088,7 @@
         <v>106</v>
       </c>
       <c r="D6" s="53"/>
-      <c r="E6" s="53">
-        <v>106</v>
-      </c>
+      <c r="E6" s="53"/>
       <c r="G6" s="5"/>
       <c r="H6" s="53">
         <v>106</v>
@@ -79146,9 +79142,7 @@
       <c r="D9" s="53">
         <v>121</v>
       </c>
-      <c r="E9" s="53">
-        <v>121</v>
-      </c>
+      <c r="E9" s="53"/>
       <c r="F9" s="53"/>
       <c r="G9" s="5"/>
       <c r="S9" s="53">
@@ -79171,9 +79165,7 @@
       <c r="D10" s="53">
         <v>122</v>
       </c>
-      <c r="E10" s="53">
-        <v>122</v>
-      </c>
+      <c r="E10" s="53"/>
       <c r="F10" s="53"/>
       <c r="G10" s="5"/>
       <c r="S10" s="53">
@@ -79194,9 +79186,7 @@
         <v>125</v>
       </c>
       <c r="D11" s="53"/>
-      <c r="E11" s="53">
-        <v>125</v>
-      </c>
+      <c r="E11" s="53"/>
       <c r="G11" s="5">
         <v>125</v>
       </c>
@@ -79212,9 +79202,7 @@
         <v>126</v>
       </c>
       <c r="D12" s="53"/>
-      <c r="E12" s="53">
-        <v>126</v>
-      </c>
+      <c r="E12" s="53"/>
       <c r="G12" s="5">
         <v>126</v>
       </c>
@@ -79230,9 +79218,7 @@
         <v>137</v>
       </c>
       <c r="D13" s="53"/>
-      <c r="E13" s="53">
-        <v>137</v>
-      </c>
+      <c r="E13" s="53"/>
       <c r="G13" s="5"/>
       <c r="H13" s="53">
         <v>137</v>
@@ -79240,6 +79226,9 @@
       <c r="K13" s="53">
         <v>137</v>
       </c>
+      <c r="AC13" s="53">
+        <v>137</v>
+      </c>
     </row>
     <row r="14" spans="1:33">
       <c r="A14" t="s">
@@ -79252,14 +79241,15 @@
         <v>138</v>
       </c>
       <c r="D14" s="53"/>
-      <c r="E14" s="53">
-        <v>138</v>
-      </c>
+      <c r="E14" s="53"/>
       <c r="G14" s="5"/>
       <c r="H14" s="53">
         <v>138</v>
       </c>
       <c r="K14" s="53">
+        <v>138</v>
+      </c>
+      <c r="AC14" s="53">
         <v>138</v>
       </c>
     </row>
@@ -79383,9 +79373,6 @@
         <v>147</v>
       </c>
       <c r="D19" s="53"/>
-      <c r="E19" s="53">
-        <v>147</v>
-      </c>
       <c r="H19" s="53">
         <v>147</v>
       </c>
@@ -79404,9 +79391,6 @@
         <v>148</v>
       </c>
       <c r="D20" s="53"/>
-      <c r="E20" s="53">
-        <v>148</v>
-      </c>
       <c r="H20" s="53">
         <v>148</v>
       </c>
@@ -79457,10 +79441,16 @@
         <v>153</v>
       </c>
       <c r="D23" s="53"/>
+      <c r="E23" s="53">
+        <v>153</v>
+      </c>
       <c r="R23">
         <v>153</v>
       </c>
       <c r="Z23" s="53">
+        <v>153</v>
+      </c>
+      <c r="AA23" s="53">
         <v>153</v>
       </c>
       <c r="AE23" s="53">
@@ -79478,10 +79468,16 @@
         <v>154</v>
       </c>
       <c r="D24" s="53"/>
+      <c r="E24" s="53">
+        <v>154</v>
+      </c>
       <c r="R24">
         <v>154</v>
       </c>
       <c r="Z24" s="53">
+        <v>154</v>
+      </c>
+      <c r="AA24" s="53">
         <v>154</v>
       </c>
       <c r="AE24" s="53">
@@ -79502,15 +79498,25 @@
       <c r="E25" s="53">
         <v>163</v>
       </c>
+      <c r="F25" s="53">
+        <v>163</v>
+      </c>
       <c r="V25" s="53">
         <v>163</v>
       </c>
       <c r="Y25" s="53">
         <v>163</v>
       </c>
-      <c r="AE25" s="53">
+      <c r="Z25" s="53">
         <v>163</v>
       </c>
+      <c r="AB25" s="53">
+        <v>163</v>
+      </c>
+      <c r="AD25" s="53">
+        <v>163</v>
+      </c>
+      <c r="AE25" s="53"/>
     </row>
     <row r="26" spans="1:31">
       <c r="A26" t="s">
@@ -79526,15 +79532,25 @@
       <c r="E26" s="53">
         <v>164</v>
       </c>
+      <c r="F26" s="53">
+        <v>164</v>
+      </c>
       <c r="V26" s="53">
         <v>164</v>
       </c>
       <c r="Y26" s="53">
         <v>164</v>
       </c>
-      <c r="AE26" s="53">
+      <c r="Z26" s="53">
         <v>164</v>
       </c>
+      <c r="AB26" s="53">
+        <v>164</v>
+      </c>
+      <c r="AD26" s="53">
+        <v>164</v>
+      </c>
+      <c r="AE26" s="53"/>
     </row>
     <row r="27" spans="1:31">
       <c r="A27" t="s">
@@ -79553,6 +79569,9 @@
       <c r="W27" s="53">
         <v>165</v>
       </c>
+      <c r="AC27" s="53">
+        <v>165</v>
+      </c>
     </row>
     <row r="28" spans="1:31">
       <c r="A28" t="s">
@@ -79571,6 +79590,9 @@
       <c r="W28" s="53">
         <v>166</v>
       </c>
+      <c r="AC28" s="53">
+        <v>166</v>
+      </c>
     </row>
     <row r="29" spans="1:31">
       <c r="A29" t="s">
@@ -79583,9 +79605,6 @@
         <v>179</v>
       </c>
       <c r="D29" s="53"/>
-      <c r="E29" s="53">
-        <v>179</v>
-      </c>
       <c r="H29" s="53">
         <v>179</v>
       </c>
@@ -79604,9 +79623,6 @@
         <v>180</v>
       </c>
       <c r="D30" s="53"/>
-      <c r="E30" s="53">
-        <v>180</v>
-      </c>
       <c r="H30" s="53">
         <v>180</v>
       </c>
@@ -79687,6 +79703,10 @@
         <v>191</v>
       </c>
       <c r="D35" s="53"/>
+      <c r="E35" s="53">
+        <v>191</v>
+      </c>
+      <c r="F35" s="53"/>
       <c r="Q35" s="53">
         <v>191</v>
       </c>
@@ -79700,13 +79720,10 @@
       <c r="AA35" s="53">
         <v>191</v>
       </c>
-      <c r="AB35" s="53">
-        <v>191</v>
-      </c>
-      <c r="AC35" s="53">
-        <v>191</v>
-      </c>
-      <c r="AD35" s="53">
+      <c r="AB35" s="53"/>
+      <c r="AC35" s="53"/>
+      <c r="AD35" s="53"/>
+      <c r="AE35" s="53">
         <v>191</v>
       </c>
     </row>
@@ -79721,6 +79738,10 @@
         <v>192</v>
       </c>
       <c r="D36" s="53"/>
+      <c r="E36" s="53">
+        <v>192</v>
+      </c>
+      <c r="F36" s="53"/>
       <c r="Q36" s="53">
         <v>192</v>
       </c>
@@ -79734,13 +79755,10 @@
       <c r="AA36" s="53">
         <v>192</v>
       </c>
-      <c r="AB36" s="53">
-        <v>192</v>
-      </c>
-      <c r="AC36" s="53">
-        <v>192</v>
-      </c>
-      <c r="AD36" s="53">
+      <c r="AB36" s="53"/>
+      <c r="AC36" s="53"/>
+      <c r="AD36" s="53"/>
+      <c r="AE36" s="53">
         <v>192</v>
       </c>
     </row>
@@ -79755,22 +79773,19 @@
         <v>193</v>
       </c>
       <c r="D37" s="53"/>
-      <c r="F37" s="53"/>
+      <c r="E37" s="69">
+        <v>193</v>
+      </c>
+      <c r="F37" s="69"/>
       <c r="Z37" s="69">
         <v>193</v>
       </c>
       <c r="AA37" s="69">
         <v>193</v>
       </c>
-      <c r="AB37" s="69">
-        <v>193</v>
-      </c>
-      <c r="AC37" s="69">
-        <v>193</v>
-      </c>
-      <c r="AD37" s="69">
-        <v>193</v>
-      </c>
+      <c r="AB37" s="69"/>
+      <c r="AC37" s="69"/>
+      <c r="AD37" s="69"/>
       <c r="AE37" s="69">
         <v>193</v>
       </c>
@@ -79792,22 +79807,19 @@
         <v>194</v>
       </c>
       <c r="D38" s="53"/>
-      <c r="F38" s="53"/>
+      <c r="E38" s="69">
+        <v>194</v>
+      </c>
+      <c r="F38" s="69"/>
       <c r="Z38" s="69">
         <v>194</v>
       </c>
       <c r="AA38" s="69">
         <v>194</v>
       </c>
-      <c r="AB38" s="69">
-        <v>194</v>
-      </c>
-      <c r="AC38" s="69">
-        <v>194</v>
-      </c>
-      <c r="AD38" s="69">
-        <v>194</v>
-      </c>
+      <c r="AB38" s="69"/>
+      <c r="AC38" s="69"/>
+      <c r="AD38" s="69"/>
       <c r="AE38" s="69">
         <v>194</v>
       </c>
@@ -79829,10 +79841,28 @@
         <v>205</v>
       </c>
       <c r="D39" s="53"/>
+      <c r="E39" s="53">
+        <v>205</v>
+      </c>
+      <c r="F39" s="53">
+        <v>205</v>
+      </c>
       <c r="V39" s="53">
         <v>205</v>
       </c>
       <c r="X39" s="53">
+        <v>205</v>
+      </c>
+      <c r="Z39" s="53">
+        <v>205</v>
+      </c>
+      <c r="AA39" s="53">
+        <v>205</v>
+      </c>
+      <c r="AC39" s="53">
+        <v>205</v>
+      </c>
+      <c r="AD39" s="53">
         <v>205</v>
       </c>
     </row>
@@ -79847,10 +79877,28 @@
         <v>206</v>
       </c>
       <c r="D40" s="53"/>
+      <c r="E40" s="53">
+        <v>206</v>
+      </c>
+      <c r="F40" s="53">
+        <v>206</v>
+      </c>
       <c r="V40" s="53">
         <v>206</v>
       </c>
       <c r="X40" s="53">
+        <v>206</v>
+      </c>
+      <c r="Z40" s="53">
+        <v>206</v>
+      </c>
+      <c r="AA40" s="53">
+        <v>206</v>
+      </c>
+      <c r="AC40" s="53">
+        <v>206</v>
+      </c>
+      <c r="AD40" s="53">
         <v>206</v>
       </c>
     </row>
@@ -80086,8 +80134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
GIF PL updated added postcentral gyrus medial segment to primary sensory cortex
</commit_message>
<xml_diff>
--- a/resources/syst_review_single_table.xlsx
+++ b/resources/syst_review_single_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\AnacondaProjects\PhD\Semiology-Visualisation-Tool\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535155EB-1852-416C-A8B3-582C0426201F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EAA11E9-8FE6-4B11-81D2-BB346587473C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -78915,7 +78915,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AG324"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="M42" sqref="M42"/>
     </sheetView>
   </sheetViews>
@@ -80134,8 +80134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -80257,6 +80257,9 @@
       <c r="C7" s="61">
         <v>149</v>
       </c>
+      <c r="D7" s="61">
+        <v>149</v>
+      </c>
       <c r="E7" s="61">
         <v>149</v>
       </c>
@@ -80269,6 +80272,9 @@
         <v>150</v>
       </c>
       <c r="C8" s="61">
+        <v>150</v>
+      </c>
+      <c r="D8" s="61">
         <v>150</v>
       </c>
       <c r="E8" s="61">

</xml_diff>

<commit_message>
GIF TL OL Fusiform gyrus OTMG and fusiform from GIF OL merged with GIF TL
</commit_message>
<xml_diff>
--- a/resources/syst_review_single_table.xlsx
+++ b/resources/syst_review_single_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\AnacondaProjects\PhD\Semiology-Visualisation-Tool\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E23C33-BC96-4AAD-8528-573B86F7F046}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823D5443-758A-4DB8-8AC6-6F0A12CC831C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6754,7 +6754,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="34">
+  <fonts count="35">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6981,6 +6981,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -7314,7 +7321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="173">
+  <cellXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -7802,6 +7809,10 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -72735,10 +72746,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20:H20"/>
+      <selection activeCell="A15" sqref="A15:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -72981,50 +72992,23 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="65" t="s">
-        <v>2103</v>
-      </c>
-      <c r="B15" s="61">
-        <v>161</v>
-      </c>
-      <c r="C15" s="61">
-        <v>161</v>
-      </c>
-      <c r="D15" s="65"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="65"/>
-      <c r="G15" s="65"/>
-      <c r="H15" s="65"/>
+        <v>2137</v>
+      </c>
+      <c r="B15" s="53">
+        <v>197</v>
+      </c>
+      <c r="C15" s="53">
+        <v>197</v>
+      </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="65" t="s">
-        <v>2104</v>
-      </c>
-      <c r="B16" s="61">
-        <v>162</v>
-      </c>
-      <c r="C16" s="61">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="65" t="s">
-        <v>2137</v>
-      </c>
-      <c r="B17" s="53">
-        <v>197</v>
-      </c>
-      <c r="C17" s="53">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="65" t="s">
         <v>2138</v>
       </c>
-      <c r="B18" s="53">
+      <c r="B16" s="53">
         <v>198</v>
       </c>
-      <c r="C18" s="53">
+      <c r="C16" s="53">
         <v>198</v>
       </c>
     </row>
@@ -77939,7 +77923,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="M9" sqref="M9:M10"/>
+      <selection pane="bottomRight" activeCell="A27" sqref="A27:W28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -78567,6 +78551,48 @@
       </c>
       <c r="H26" s="53">
         <v>208</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24">
+      <c r="A27" s="174" t="s">
+        <v>2103</v>
+      </c>
+      <c r="B27" s="173">
+        <v>161</v>
+      </c>
+      <c r="C27" s="174"/>
+      <c r="D27" s="173">
+        <v>161</v>
+      </c>
+      <c r="Q27" s="173">
+        <v>161</v>
+      </c>
+      <c r="V27" s="173">
+        <v>161</v>
+      </c>
+      <c r="W27" s="173">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24">
+      <c r="A28" s="174" t="s">
+        <v>2104</v>
+      </c>
+      <c r="B28" s="173">
+        <v>162</v>
+      </c>
+      <c r="C28" s="174"/>
+      <c r="D28" s="173">
+        <v>162</v>
+      </c>
+      <c r="Q28" s="173">
+        <v>162</v>
+      </c>
+      <c r="V28" s="173">
+        <v>162</v>
+      </c>
+      <c r="W28" s="173">
+        <v>162</v>
       </c>
     </row>
     <row r="29" spans="1:24">

</xml_diff>

<commit_message>
GIF Insula updated precentral gyrus maps to anterior insula (not posterior)
</commit_message>
<xml_diff>
--- a/resources/syst_review_single_table.xlsx
+++ b/resources/syst_review_single_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\AnacondaProjects\PhD\Semiology-Visualisation-Tool\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E85A5988-E286-4439-B2ED-3B77CD05DDA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{404EB68E-A7D5-42E8-8FBD-771D9DA85C95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -72766,7 +72766,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
@@ -73092,7 +73092,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="I7" sqref="I7:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -73221,7 +73221,7 @@
       <c r="H7" s="61">
         <v>167</v>
       </c>
-      <c r="I7" s="114">
+      <c r="I7" s="171">
         <v>167</v>
       </c>
     </row>
@@ -73238,7 +73238,7 @@
       <c r="H8" s="61">
         <v>168</v>
       </c>
-      <c r="I8" s="114">
+      <c r="I8" s="171">
         <v>168</v>
       </c>
     </row>
@@ -73282,8 +73282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -73356,7 +73356,12 @@
       <c r="G3" s="61">
         <v>103</v>
       </c>
-      <c r="K3" s="114">
+      <c r="H3" s="61">
+        <v>103</v>
+      </c>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="171">
         <v>103</v>
       </c>
     </row>
@@ -73382,7 +73387,12 @@
       <c r="G4" s="61">
         <v>104</v>
       </c>
-      <c r="K4" s="114">
+      <c r="H4" s="61">
+        <v>104</v>
+      </c>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="171">
         <v>104</v>
       </c>
     </row>
@@ -73396,15 +73406,14 @@
       <c r="C5" s="61">
         <v>173</v>
       </c>
-      <c r="H5" s="114">
+      <c r="H5" s="114"/>
+      <c r="I5" s="171">
         <v>173</v>
       </c>
-      <c r="I5" s="114">
+      <c r="J5" s="171">
         <v>173</v>
       </c>
-      <c r="J5" s="61">
-        <v>173</v>
-      </c>
+      <c r="K5" s="67"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
@@ -73416,19 +73425,20 @@
       <c r="C6" s="61">
         <v>174</v>
       </c>
-      <c r="H6" s="114">
+      <c r="H6" s="114"/>
+      <c r="I6" s="171">
         <v>174</v>
       </c>
-      <c r="I6" s="114">
+      <c r="J6" s="171">
         <v>174</v>
       </c>
-      <c r="J6" s="61">
-        <v>174</v>
-      </c>
+      <c r="K6" s="67"/>
     </row>
     <row r="7" spans="1:11">
       <c r="H7" s="65"/>
-      <c r="I7" s="65"/>
+      <c r="I7" s="67"/>
+      <c r="J7" s="67"/>
+      <c r="K7" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
updated mappings fixture for aphasia as GIF mappings changed
</commit_message>
<xml_diff>
--- a/resources/syst_review_single_table.xlsx
+++ b/resources/syst_review_single_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\AnacondaProjects\PhD\Semiology-Visualisation-Tool\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{404EB68E-A7D5-42E8-8FBD-771D9DA85C95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C8AFB3-E2CA-4D90-BC3E-9AF9BD3ABBF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -7770,6 +7770,25 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -7811,25 +7830,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -10422,11 +10422,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DU1102"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="AA724" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D744" sqref="D744:Q744"/>
+      <selection pane="bottomRight" activeCell="AE735" sqref="AE735"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -10518,106 +10518,106 @@
     <row r="1" spans="1:125" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="155"/>
       <c r="C1" s="17"/>
-      <c r="D1" s="157" t="s">
+      <c r="D1" s="164" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="157"/>
-      <c r="G1" s="165" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="166"/>
-      <c r="I1" s="166"/>
-      <c r="K1" s="167" t="s">
+      <c r="E1" s="164"/>
+      <c r="G1" s="172" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="173"/>
+      <c r="I1" s="173"/>
+      <c r="K1" s="174" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="168"/>
-      <c r="M1" s="168"/>
-      <c r="N1" s="168"/>
-      <c r="O1" s="169"/>
-      <c r="S1" s="158"/>
-      <c r="T1" s="158"/>
-      <c r="U1" s="158"/>
-      <c r="V1" s="158"/>
-      <c r="W1" s="158"/>
-      <c r="X1" s="158"/>
-      <c r="Y1" s="158"/>
-      <c r="Z1" s="158"/>
-      <c r="AA1" s="158"/>
-      <c r="AB1" s="158"/>
-      <c r="AC1" s="158"/>
-      <c r="AD1" s="158"/>
-      <c r="AE1" s="158"/>
-      <c r="AF1" s="158"/>
-      <c r="AG1" s="158"/>
-      <c r="AH1" s="158"/>
-      <c r="AI1" s="158"/>
-      <c r="AJ1" s="158"/>
-      <c r="AK1" s="158"/>
+      <c r="L1" s="175"/>
+      <c r="M1" s="175"/>
+      <c r="N1" s="175"/>
+      <c r="O1" s="176"/>
+      <c r="S1" s="165"/>
+      <c r="T1" s="165"/>
+      <c r="U1" s="165"/>
+      <c r="V1" s="165"/>
+      <c r="W1" s="165"/>
+      <c r="X1" s="165"/>
+      <c r="Y1" s="165"/>
+      <c r="Z1" s="165"/>
+      <c r="AA1" s="165"/>
+      <c r="AB1" s="165"/>
+      <c r="AC1" s="165"/>
+      <c r="AD1" s="165"/>
+      <c r="AE1" s="165"/>
+      <c r="AF1" s="165"/>
+      <c r="AG1" s="165"/>
+      <c r="AH1" s="165"/>
+      <c r="AI1" s="165"/>
+      <c r="AJ1" s="165"/>
+      <c r="AK1" s="165"/>
       <c r="AM1" s="153"/>
-      <c r="AN1" s="159" t="s">
+      <c r="AN1" s="166" t="s">
         <v>3</v>
       </c>
-      <c r="AO1" s="158"/>
-      <c r="AP1" s="158"/>
-      <c r="AQ1" s="158"/>
-      <c r="AR1" s="158"/>
-      <c r="AS1" s="158"/>
-      <c r="AT1" s="158"/>
-      <c r="AU1" s="158"/>
-      <c r="AV1" s="158"/>
-      <c r="AW1" s="158"/>
-      <c r="AX1" s="158"/>
-      <c r="AY1" s="158"/>
-      <c r="AZ1" s="158"/>
-      <c r="BA1" s="158"/>
-      <c r="BB1" s="158"/>
-      <c r="BC1" s="158"/>
-      <c r="BD1" s="158"/>
-      <c r="BE1" s="158"/>
-      <c r="BF1" s="158"/>
-      <c r="BG1" s="158"/>
-      <c r="BH1" s="158"/>
-      <c r="BI1" s="158"/>
-      <c r="BJ1" s="158"/>
-      <c r="BK1" s="158"/>
-      <c r="BL1" s="158"/>
-      <c r="BM1" s="158"/>
-      <c r="BN1" s="158"/>
-      <c r="BO1" s="158"/>
-      <c r="BP1" s="158"/>
-      <c r="BR1" s="161"/>
-      <c r="BS1" s="162"/>
-      <c r="BT1" s="162"/>
-      <c r="BU1" s="162"/>
-      <c r="BV1" s="162"/>
-      <c r="BW1" s="163"/>
+      <c r="AO1" s="165"/>
+      <c r="AP1" s="165"/>
+      <c r="AQ1" s="165"/>
+      <c r="AR1" s="165"/>
+      <c r="AS1" s="165"/>
+      <c r="AT1" s="165"/>
+      <c r="AU1" s="165"/>
+      <c r="AV1" s="165"/>
+      <c r="AW1" s="165"/>
+      <c r="AX1" s="165"/>
+      <c r="AY1" s="165"/>
+      <c r="AZ1" s="165"/>
+      <c r="BA1" s="165"/>
+      <c r="BB1" s="165"/>
+      <c r="BC1" s="165"/>
+      <c r="BD1" s="165"/>
+      <c r="BE1" s="165"/>
+      <c r="BF1" s="165"/>
+      <c r="BG1" s="165"/>
+      <c r="BH1" s="165"/>
+      <c r="BI1" s="165"/>
+      <c r="BJ1" s="165"/>
+      <c r="BK1" s="165"/>
+      <c r="BL1" s="165"/>
+      <c r="BM1" s="165"/>
+      <c r="BN1" s="165"/>
+      <c r="BO1" s="165"/>
+      <c r="BP1" s="165"/>
+      <c r="BR1" s="168"/>
+      <c r="BS1" s="169"/>
+      <c r="BT1" s="169"/>
+      <c r="BU1" s="169"/>
+      <c r="BV1" s="169"/>
+      <c r="BW1" s="170"/>
       <c r="BX1" s="156"/>
-      <c r="BZ1" s="158"/>
-      <c r="CA1" s="158"/>
-      <c r="CB1" s="158"/>
-      <c r="CC1" s="158"/>
-      <c r="CD1" s="158"/>
-      <c r="CE1" s="158"/>
-      <c r="CF1" s="158"/>
-      <c r="CG1" s="160"/>
-      <c r="CH1" s="159" t="s">
+      <c r="BZ1" s="165"/>
+      <c r="CA1" s="165"/>
+      <c r="CB1" s="165"/>
+      <c r="CC1" s="165"/>
+      <c r="CD1" s="165"/>
+      <c r="CE1" s="165"/>
+      <c r="CF1" s="165"/>
+      <c r="CG1" s="167"/>
+      <c r="CH1" s="166" t="s">
         <v>4</v>
       </c>
-      <c r="CI1" s="158"/>
-      <c r="CJ1" s="158"/>
-      <c r="CK1" s="158"/>
-      <c r="CL1" s="158"/>
-      <c r="CM1" s="160"/>
+      <c r="CI1" s="165"/>
+      <c r="CJ1" s="165"/>
+      <c r="CK1" s="165"/>
+      <c r="CL1" s="165"/>
+      <c r="CM1" s="167"/>
       <c r="CO1" s="85"/>
-      <c r="CP1" s="164" t="s">
+      <c r="CP1" s="171" t="s">
         <v>5</v>
       </c>
-      <c r="CQ1" s="164"/>
-      <c r="CR1" s="164"/>
-      <c r="CS1" s="164"/>
-      <c r="CT1" s="164"/>
-      <c r="CU1" s="164"/>
-      <c r="CV1" s="164"/>
+      <c r="CQ1" s="171"/>
+      <c r="CR1" s="171"/>
+      <c r="CS1" s="171"/>
+      <c r="CT1" s="171"/>
+      <c r="CU1" s="171"/>
+      <c r="CV1" s="171"/>
       <c r="CX1" s="140"/>
       <c r="CY1" s="140"/>
       <c r="CZ1" s="140"/>
@@ -72778,12 +72778,12 @@
     <row r="1" spans="1:11">
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="170" t="s">
+      <c r="E1" s="177" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="170"/>
-      <c r="G1" s="170"/>
-      <c r="H1" s="170"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
+      <c r="H1" s="177"/>
       <c r="I1" s="117"/>
     </row>
     <row r="2" spans="1:11" ht="45">
@@ -72805,13 +72805,13 @@
       <c r="H2" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="I2" s="175" t="s">
+      <c r="I2" s="161" t="s">
         <v>2158</v>
       </c>
-      <c r="J2" s="177" t="s">
+      <c r="J2" s="163" t="s">
         <v>2159</v>
       </c>
-      <c r="K2" s="177" t="s">
+      <c r="K2" s="163" t="s">
         <v>2160</v>
       </c>
     </row>
@@ -73061,7 +73061,7 @@
       <c r="C15" s="53">
         <v>197</v>
       </c>
-      <c r="I15" s="176">
+      <c r="I15" s="162">
         <v>197</v>
       </c>
     </row>
@@ -73075,7 +73075,7 @@
       <c r="C16" s="53">
         <v>198</v>
       </c>
-      <c r="I16" s="176">
+      <c r="I16" s="162">
         <v>198</v>
       </c>
     </row>
@@ -73104,11 +73104,11 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="C1" s="2"/>
-      <c r="D1" s="159"/>
-      <c r="E1" s="158"/>
-      <c r="F1" s="158"/>
-      <c r="G1" s="158"/>
-      <c r="H1" s="160"/>
+      <c r="D1" s="166"/>
+      <c r="E1" s="165"/>
+      <c r="F1" s="165"/>
+      <c r="G1" s="165"/>
+      <c r="H1" s="167"/>
       <c r="I1" s="156"/>
       <c r="J1" s="130"/>
     </row>
@@ -73221,7 +73221,7 @@
       <c r="H7" s="61">
         <v>167</v>
       </c>
-      <c r="I7" s="171">
+      <c r="I7" s="157">
         <v>167</v>
       </c>
     </row>
@@ -73238,7 +73238,7 @@
       <c r="H8" s="61">
         <v>168</v>
       </c>
-      <c r="I8" s="171">
+      <c r="I8" s="157">
         <v>168</v>
       </c>
     </row>
@@ -73282,7 +73282,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
@@ -73295,15 +73295,15 @@
     <row r="1" spans="1:11" ht="26.25">
       <c r="C1" s="2"/>
       <c r="D1" s="85"/>
-      <c r="E1" s="164" t="s">
+      <c r="E1" s="171" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="164"/>
-      <c r="G1" s="164"/>
-      <c r="H1" s="164"/>
-      <c r="I1" s="164"/>
-      <c r="J1" s="164"/>
-      <c r="K1" s="164"/>
+      <c r="F1" s="171"/>
+      <c r="G1" s="171"/>
+      <c r="H1" s="171"/>
+      <c r="I1" s="171"/>
+      <c r="J1" s="171"/>
+      <c r="K1" s="171"/>
     </row>
     <row r="2" spans="1:11" ht="30">
       <c r="C2" s="98" t="s">
@@ -73361,7 +73361,7 @@
       </c>
       <c r="I3" s="67"/>
       <c r="J3" s="67"/>
-      <c r="K3" s="171">
+      <c r="K3" s="157">
         <v>103</v>
       </c>
     </row>
@@ -73392,7 +73392,7 @@
       </c>
       <c r="I4" s="67"/>
       <c r="J4" s="67"/>
-      <c r="K4" s="171">
+      <c r="K4" s="157">
         <v>104</v>
       </c>
     </row>
@@ -73407,10 +73407,10 @@
         <v>173</v>
       </c>
       <c r="H5" s="114"/>
-      <c r="I5" s="171">
+      <c r="I5" s="157">
         <v>173</v>
       </c>
-      <c r="J5" s="171">
+      <c r="J5" s="157">
         <v>173</v>
       </c>
       <c r="K5" s="67"/>
@@ -73426,10 +73426,10 @@
         <v>174</v>
       </c>
       <c r="H6" s="114"/>
-      <c r="I6" s="171">
+      <c r="I6" s="157">
         <v>174</v>
       </c>
-      <c r="J6" s="171">
+      <c r="J6" s="157">
         <v>174</v>
       </c>
       <c r="K6" s="67"/>
@@ -73453,7 +73453,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -73535,7 +73535,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E9"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -78012,24 +78012,24 @@
   <sheetData>
     <row r="1" spans="1:23" ht="15" customHeight="1">
       <c r="D1" s="96"/>
-      <c r="E1" s="158"/>
-      <c r="F1" s="158"/>
-      <c r="G1" s="158"/>
-      <c r="H1" s="158"/>
-      <c r="I1" s="158"/>
-      <c r="J1" s="158"/>
-      <c r="K1" s="158"/>
-      <c r="L1" s="158"/>
-      <c r="M1" s="158"/>
-      <c r="N1" s="158"/>
-      <c r="O1" s="158"/>
-      <c r="P1" s="158"/>
-      <c r="Q1" s="158"/>
-      <c r="R1" s="158"/>
-      <c r="S1" s="158"/>
-      <c r="T1" s="158"/>
-      <c r="U1" s="158"/>
-      <c r="V1" s="158"/>
+      <c r="E1" s="165"/>
+      <c r="F1" s="165"/>
+      <c r="G1" s="165"/>
+      <c r="H1" s="165"/>
+      <c r="I1" s="165"/>
+      <c r="J1" s="165"/>
+      <c r="K1" s="165"/>
+      <c r="L1" s="165"/>
+      <c r="M1" s="165"/>
+      <c r="N1" s="165"/>
+      <c r="O1" s="165"/>
+      <c r="P1" s="165"/>
+      <c r="Q1" s="165"/>
+      <c r="R1" s="165"/>
+      <c r="S1" s="165"/>
+      <c r="T1" s="165"/>
+      <c r="U1" s="165"/>
+      <c r="V1" s="165"/>
     </row>
     <row r="2" spans="1:23" ht="96" customHeight="1">
       <c r="A2" s="58"/>
@@ -78109,10 +78109,10 @@
       <c r="M3" s="61">
         <v>32</v>
       </c>
-      <c r="N3" s="171">
+      <c r="N3" s="157">
         <v>32</v>
       </c>
-      <c r="O3" s="172"/>
+      <c r="O3" s="158"/>
       <c r="R3" s="61">
         <v>32</v>
       </c>
@@ -78132,10 +78132,10 @@
       <c r="M4" s="61">
         <v>33</v>
       </c>
-      <c r="N4" s="171">
+      <c r="N4" s="157">
         <v>33</v>
       </c>
-      <c r="O4" s="172"/>
+      <c r="O4" s="158"/>
       <c r="R4" s="61">
         <v>33</v>
       </c>
@@ -78155,8 +78155,8 @@
       <c r="M5" s="61">
         <v>48</v>
       </c>
-      <c r="N5" s="172"/>
-      <c r="O5" s="171">
+      <c r="N5" s="158"/>
+      <c r="O5" s="157">
         <v>48</v>
       </c>
       <c r="T5" s="61">
@@ -78177,8 +78177,8 @@
       <c r="M6" s="61">
         <v>49</v>
       </c>
-      <c r="N6" s="172"/>
-      <c r="O6" s="171">
+      <c r="N6" s="158"/>
+      <c r="O6" s="157">
         <v>49</v>
       </c>
       <c r="T6" s="61">
@@ -78199,10 +78199,10 @@
       <c r="M7" s="61">
         <v>117</v>
       </c>
-      <c r="N7" s="171">
+      <c r="N7" s="157">
         <v>117</v>
       </c>
-      <c r="O7" s="172"/>
+      <c r="O7" s="158"/>
       <c r="P7" s="61">
         <v>117</v>
       </c>
@@ -78221,10 +78221,10 @@
       <c r="M8" s="61">
         <v>118</v>
       </c>
-      <c r="N8" s="171">
+      <c r="N8" s="157">
         <v>118</v>
       </c>
-      <c r="O8" s="172"/>
+      <c r="O8" s="158"/>
       <c r="P8" s="61">
         <v>118</v>
       </c>
@@ -78241,7 +78241,7 @@
         <v>123</v>
       </c>
       <c r="M9" s="61"/>
-      <c r="N9" s="171"/>
+      <c r="N9" s="157"/>
       <c r="O9" s="61">
         <v>123</v>
       </c>
@@ -78269,7 +78269,7 @@
         <v>124</v>
       </c>
       <c r="M10" s="61"/>
-      <c r="N10" s="171"/>
+      <c r="N10" s="157"/>
       <c r="O10" s="61">
         <v>124</v>
       </c>
@@ -78302,8 +78302,8 @@
       <c r="L11" s="61">
         <v>133</v>
       </c>
-      <c r="N11" s="172"/>
-      <c r="O11" s="172"/>
+      <c r="N11" s="158"/>
+      <c r="O11" s="158"/>
       <c r="U11" s="61">
         <v>133</v>
       </c>
@@ -78327,8 +78327,8 @@
       <c r="L12" s="61">
         <v>134</v>
       </c>
-      <c r="N12" s="172"/>
-      <c r="O12" s="172"/>
+      <c r="N12" s="158"/>
+      <c r="O12" s="158"/>
       <c r="U12" s="61">
         <v>134</v>
       </c>
@@ -78352,8 +78352,8 @@
       <c r="K13" s="61">
         <v>155</v>
       </c>
-      <c r="N13" s="172"/>
-      <c r="O13" s="172"/>
+      <c r="N13" s="158"/>
+      <c r="O13" s="158"/>
       <c r="U13" s="61">
         <v>155</v>
       </c>
@@ -78374,8 +78374,8 @@
       <c r="K14" s="61">
         <v>156</v>
       </c>
-      <c r="N14" s="172"/>
-      <c r="O14" s="172"/>
+      <c r="N14" s="158"/>
+      <c r="O14" s="158"/>
       <c r="U14" s="61">
         <v>156</v>
       </c>
@@ -78393,8 +78393,8 @@
       <c r="M15" s="61">
         <v>171</v>
       </c>
-      <c r="N15" s="171"/>
-      <c r="O15" s="171">
+      <c r="N15" s="157"/>
+      <c r="O15" s="157">
         <v>171</v>
       </c>
       <c r="S15" s="61">
@@ -78418,8 +78418,8 @@
       <c r="M16" s="61">
         <v>172</v>
       </c>
-      <c r="N16" s="171"/>
-      <c r="O16" s="171">
+      <c r="N16" s="157"/>
+      <c r="O16" s="157">
         <v>172</v>
       </c>
       <c r="S16" s="61">
@@ -78449,8 +78449,8 @@
       <c r="J17" s="53">
         <v>181</v>
       </c>
-      <c r="N17" s="172"/>
-      <c r="O17" s="172"/>
+      <c r="N17" s="158"/>
+      <c r="O17" s="158"/>
     </row>
     <row r="18" spans="1:24">
       <c r="A18" t="s">
@@ -78471,8 +78471,8 @@
       <c r="J18" s="53">
         <v>182</v>
       </c>
-      <c r="N18" s="172"/>
-      <c r="O18" s="172"/>
+      <c r="N18" s="158"/>
+      <c r="O18" s="158"/>
     </row>
     <row r="19" spans="1:24">
       <c r="A19" t="s">
@@ -78493,8 +78493,8 @@
       <c r="I19" s="53">
         <v>185</v>
       </c>
-      <c r="N19" s="172"/>
-      <c r="O19" s="172"/>
+      <c r="N19" s="158"/>
+      <c r="O19" s="158"/>
       <c r="U19" s="53">
         <v>185</v>
       </c>
@@ -78631,44 +78631,44 @@
       </c>
     </row>
     <row r="27" spans="1:24">
-      <c r="A27" s="174" t="s">
+      <c r="A27" s="160" t="s">
         <v>2103</v>
       </c>
-      <c r="B27" s="173">
+      <c r="B27" s="159">
         <v>161</v>
       </c>
-      <c r="C27" s="174"/>
-      <c r="D27" s="173">
+      <c r="C27" s="160"/>
+      <c r="D27" s="159">
         <v>161</v>
       </c>
-      <c r="Q27" s="173">
+      <c r="Q27" s="159">
         <v>161</v>
       </c>
-      <c r="V27" s="173">
+      <c r="V27" s="159">
         <v>161</v>
       </c>
-      <c r="W27" s="173">
+      <c r="W27" s="159">
         <v>161</v>
       </c>
     </row>
     <row r="28" spans="1:24">
-      <c r="A28" s="174" t="s">
+      <c r="A28" s="160" t="s">
         <v>2104</v>
       </c>
-      <c r="B28" s="173">
+      <c r="B28" s="159">
         <v>162</v>
       </c>
-      <c r="C28" s="174"/>
-      <c r="D28" s="173">
+      <c r="C28" s="160"/>
+      <c r="D28" s="159">
         <v>162</v>
       </c>
-      <c r="Q28" s="173">
+      <c r="Q28" s="159">
         <v>162</v>
       </c>
-      <c r="V28" s="173">
+      <c r="V28" s="159">
         <v>162</v>
       </c>
-      <c r="W28" s="173">
+      <c r="W28" s="159">
         <v>162</v>
       </c>
     </row>
@@ -79020,37 +79020,37 @@
     <row r="1" spans="1:33" ht="15" customHeight="1">
       <c r="A1" s="58"/>
       <c r="B1" s="59"/>
-      <c r="E1" s="159" t="s">
+      <c r="E1" s="166" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="158"/>
-      <c r="G1" s="158"/>
-      <c r="H1" s="158"/>
-      <c r="I1" s="158"/>
-      <c r="J1" s="158"/>
-      <c r="K1" s="158"/>
-      <c r="L1" s="158"/>
-      <c r="M1" s="158"/>
-      <c r="N1" s="158"/>
-      <c r="O1" s="158"/>
-      <c r="P1" s="158"/>
-      <c r="Q1" s="158"/>
-      <c r="R1" s="158"/>
-      <c r="S1" s="158"/>
-      <c r="T1" s="158"/>
-      <c r="U1" s="158"/>
-      <c r="V1" s="158"/>
-      <c r="W1" s="158"/>
-      <c r="X1" s="158"/>
-      <c r="Y1" s="158"/>
-      <c r="Z1" s="158"/>
-      <c r="AA1" s="158"/>
-      <c r="AB1" s="158"/>
-      <c r="AC1" s="158"/>
-      <c r="AD1" s="158"/>
-      <c r="AE1" s="158"/>
-      <c r="AF1" s="158"/>
-      <c r="AG1" s="158"/>
+      <c r="F1" s="165"/>
+      <c r="G1" s="165"/>
+      <c r="H1" s="165"/>
+      <c r="I1" s="165"/>
+      <c r="J1" s="165"/>
+      <c r="K1" s="165"/>
+      <c r="L1" s="165"/>
+      <c r="M1" s="165"/>
+      <c r="N1" s="165"/>
+      <c r="O1" s="165"/>
+      <c r="P1" s="165"/>
+      <c r="Q1" s="165"/>
+      <c r="R1" s="165"/>
+      <c r="S1" s="165"/>
+      <c r="T1" s="165"/>
+      <c r="U1" s="165"/>
+      <c r="V1" s="165"/>
+      <c r="W1" s="165"/>
+      <c r="X1" s="165"/>
+      <c r="Y1" s="165"/>
+      <c r="Z1" s="165"/>
+      <c r="AA1" s="165"/>
+      <c r="AB1" s="165"/>
+      <c r="AC1" s="165"/>
+      <c r="AD1" s="165"/>
+      <c r="AE1" s="165"/>
+      <c r="AF1" s="165"/>
+      <c r="AG1" s="165"/>
     </row>
     <row r="2" spans="1:33" ht="144" customHeight="1">
       <c r="C2" s="96" t="s">

</xml_diff>

<commit_message>
Mapping calibration visualisation: TL Custom semiology "_mappings_TL#" to visualise
</commit_message>
<xml_diff>
--- a/resources/syst_review_single_table.xlsx
+++ b/resources/syst_review_single_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\AnacondaProjects\PhD\Semiology-Visualisation-Tool\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C8AFB3-E2CA-4D90-BC3E-9AF9BD3ABBF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F29B1F16-DD21-494E-A273-833D08B163BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6992" uniqueCount="2161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7053" uniqueCount="2183">
   <si>
     <t xml:space="preserve">Semiology </t>
   </si>
@@ -6757,6 +6757,72 @@
   </si>
   <si>
     <t>Inferior Occipital Gyrus</t>
+  </si>
+  <si>
+    <t>Marvasti mappings v 1.0.8</t>
+  </si>
+  <si>
+    <t>_mappings_TL</t>
+  </si>
+  <si>
+    <t>calibration visualisation</t>
+  </si>
+  <si>
+    <t>_mapiings_TL1</t>
+  </si>
+  <si>
+    <t>_mapiings_TL2</t>
+  </si>
+  <si>
+    <t>_mapiings_TL3</t>
+  </si>
+  <si>
+    <t>_mapiings_TL4</t>
+  </si>
+  <si>
+    <t>_mapiings_TL5</t>
+  </si>
+  <si>
+    <t>_mapiings_TL6</t>
+  </si>
+  <si>
+    <t>_mapiings_TL7</t>
+  </si>
+  <si>
+    <t>_mapiings_TL8</t>
+  </si>
+  <si>
+    <t>_mapiings_TL9</t>
+  </si>
+  <si>
+    <t>_mapiings_TL10</t>
+  </si>
+  <si>
+    <t>_mapiings_TL11</t>
+  </si>
+  <si>
+    <t>_mapiings_TL12</t>
+  </si>
+  <si>
+    <t>_mapiings_TL13</t>
+  </si>
+  <si>
+    <t>_mapiings_TL14</t>
+  </si>
+  <si>
+    <t>_mapiings_TL15</t>
+  </si>
+  <si>
+    <t>_mapiings_TL16</t>
+  </si>
+  <si>
+    <t>_mapiings_TL17</t>
+  </si>
+  <si>
+    <t>_mapiings_TL18</t>
+  </si>
+  <si>
+    <t>_mapiings_TL19</t>
   </si>
 </sst>
 </file>
@@ -7330,7 +7396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="178">
+  <cellXfs count="183">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -7830,6 +7896,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -10420,13 +10501,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:DU1102"/>
+  <dimension ref="A1:DU1122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="AA724" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E1097" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AE735" sqref="AE735"/>
+      <selection pane="bottomRight" activeCell="A1103" sqref="A1103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -72744,6 +72825,2568 @@
       <c r="DT1102" s="42"/>
       <c r="DU1102" s="42"/>
     </row>
+    <row r="1103" spans="1:125" s="179" customFormat="1" ht="30">
+      <c r="A1103" s="178" t="s">
+        <v>2161</v>
+      </c>
+      <c r="B1103" s="178"/>
+      <c r="C1103" s="178"/>
+      <c r="D1103" s="178" t="s">
+        <v>2162</v>
+      </c>
+      <c r="F1103" s="178" t="s">
+        <v>2163</v>
+      </c>
+      <c r="G1103" s="178" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1103" s="178"/>
+      <c r="I1103" s="178"/>
+      <c r="J1103" s="147"/>
+      <c r="K1103" s="147"/>
+      <c r="L1103" s="147"/>
+      <c r="M1103" s="147"/>
+      <c r="N1103" s="147"/>
+      <c r="O1103" s="147"/>
+      <c r="P1103" s="147"/>
+      <c r="Q1103" s="180"/>
+      <c r="R1103" s="147">
+        <v>1</v>
+      </c>
+      <c r="S1103" s="147"/>
+      <c r="T1103" s="147"/>
+      <c r="U1103" s="147"/>
+      <c r="V1103" s="147"/>
+      <c r="W1103" s="147"/>
+      <c r="X1103" s="147"/>
+      <c r="Y1103" s="147"/>
+      <c r="Z1103" s="147"/>
+      <c r="AA1103" s="147"/>
+      <c r="AB1103" s="147"/>
+      <c r="AC1103" s="147"/>
+      <c r="AD1103" s="147"/>
+      <c r="AE1103" s="147"/>
+      <c r="AF1103" s="147"/>
+      <c r="AG1103" s="147"/>
+      <c r="AH1103" s="147"/>
+      <c r="AI1103" s="147"/>
+      <c r="AJ1103" s="147"/>
+      <c r="AK1103" s="147"/>
+      <c r="AL1103" s="147"/>
+      <c r="AM1103" s="147"/>
+      <c r="AN1103" s="147"/>
+      <c r="AO1103" s="147"/>
+      <c r="AP1103" s="147"/>
+      <c r="AQ1103" s="147"/>
+      <c r="AR1103" s="147"/>
+      <c r="AS1103" s="147"/>
+      <c r="AT1103" s="147"/>
+      <c r="AU1103" s="147"/>
+      <c r="AV1103" s="147"/>
+      <c r="AW1103" s="147"/>
+      <c r="AX1103" s="147"/>
+      <c r="AY1103" s="147"/>
+      <c r="AZ1103" s="147"/>
+      <c r="BA1103" s="147"/>
+      <c r="BB1103" s="147"/>
+      <c r="BC1103" s="147"/>
+      <c r="BD1103" s="147"/>
+      <c r="BE1103" s="147"/>
+      <c r="BF1103" s="147"/>
+      <c r="BG1103" s="147"/>
+      <c r="BH1103" s="147"/>
+      <c r="BI1103" s="147"/>
+      <c r="BJ1103" s="147"/>
+      <c r="BK1103" s="147"/>
+      <c r="BL1103" s="147"/>
+      <c r="BM1103" s="147"/>
+      <c r="BN1103" s="147"/>
+      <c r="BO1103" s="147"/>
+      <c r="BP1103" s="147"/>
+      <c r="BQ1103" s="147"/>
+      <c r="BR1103" s="147"/>
+      <c r="BS1103" s="147"/>
+      <c r="BT1103" s="147"/>
+      <c r="BU1103" s="147"/>
+      <c r="BV1103" s="147"/>
+      <c r="BW1103" s="147"/>
+      <c r="BX1103" s="147"/>
+      <c r="BY1103" s="147"/>
+      <c r="BZ1103" s="147"/>
+      <c r="CA1103" s="147"/>
+      <c r="CB1103" s="147"/>
+      <c r="CC1103" s="147"/>
+      <c r="CD1103" s="147"/>
+      <c r="CE1103" s="147"/>
+      <c r="CF1103" s="147"/>
+      <c r="CG1103" s="147"/>
+      <c r="CH1103" s="147"/>
+      <c r="CI1103" s="147"/>
+      <c r="CJ1103" s="147"/>
+      <c r="CK1103" s="147"/>
+      <c r="CL1103" s="147"/>
+      <c r="CM1103" s="147"/>
+      <c r="CN1103" s="147"/>
+      <c r="CO1103" s="147"/>
+      <c r="CP1103" s="147"/>
+      <c r="CQ1103" s="147"/>
+      <c r="CR1103" s="147"/>
+      <c r="CS1103" s="147"/>
+      <c r="CT1103" s="147"/>
+      <c r="CU1103" s="147"/>
+      <c r="CV1103" s="147"/>
+      <c r="CW1103" s="147"/>
+      <c r="CX1103" s="147"/>
+      <c r="CY1103" s="147"/>
+      <c r="CZ1103" s="147"/>
+      <c r="DA1103" s="147"/>
+      <c r="DB1103" s="181"/>
+      <c r="DC1103" s="181"/>
+      <c r="DD1103" s="147"/>
+      <c r="DE1103" s="147"/>
+      <c r="DF1103" s="147"/>
+      <c r="DG1103" s="147"/>
+      <c r="DH1103" s="147"/>
+      <c r="DI1103" s="147"/>
+      <c r="DJ1103" s="147"/>
+      <c r="DK1103" s="147"/>
+      <c r="DL1103" s="147"/>
+      <c r="DM1103" s="147"/>
+      <c r="DN1103" s="147"/>
+      <c r="DO1103" s="147"/>
+    </row>
+    <row r="1104" spans="1:125" s="179" customFormat="1" ht="30">
+      <c r="A1104" s="178"/>
+      <c r="B1104" s="178"/>
+      <c r="C1104" s="178"/>
+      <c r="D1104" s="178" t="s">
+        <v>2164</v>
+      </c>
+      <c r="F1104" s="178" t="s">
+        <v>2163</v>
+      </c>
+      <c r="G1104" s="178" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1104" s="178"/>
+      <c r="I1104" s="178"/>
+      <c r="J1104" s="147"/>
+      <c r="K1104" s="147"/>
+      <c r="L1104" s="147"/>
+      <c r="M1104" s="147"/>
+      <c r="N1104" s="147"/>
+      <c r="O1104" s="147"/>
+      <c r="P1104" s="147"/>
+      <c r="Q1104" s="180"/>
+      <c r="R1104" s="147"/>
+      <c r="S1104" s="147">
+        <v>1</v>
+      </c>
+      <c r="T1104" s="147"/>
+      <c r="U1104" s="147"/>
+      <c r="V1104" s="147"/>
+      <c r="W1104" s="147"/>
+      <c r="X1104" s="147"/>
+      <c r="Y1104" s="147"/>
+      <c r="Z1104" s="147"/>
+      <c r="AA1104" s="147"/>
+      <c r="AB1104" s="147"/>
+      <c r="AC1104" s="147"/>
+      <c r="AD1104" s="147"/>
+      <c r="AE1104" s="147"/>
+      <c r="AF1104" s="147"/>
+      <c r="AG1104" s="147"/>
+      <c r="AH1104" s="147"/>
+      <c r="AI1104" s="147"/>
+      <c r="AJ1104" s="147"/>
+      <c r="AK1104" s="147"/>
+      <c r="AL1104" s="147"/>
+      <c r="AM1104" s="147"/>
+      <c r="AN1104" s="147"/>
+      <c r="AO1104" s="147"/>
+      <c r="AP1104" s="147"/>
+      <c r="AQ1104" s="147"/>
+      <c r="AR1104" s="147"/>
+      <c r="AS1104" s="147"/>
+      <c r="AT1104" s="147"/>
+      <c r="AU1104" s="147"/>
+      <c r="AV1104" s="147"/>
+      <c r="AW1104" s="147"/>
+      <c r="AX1104" s="147"/>
+      <c r="AY1104" s="147"/>
+      <c r="AZ1104" s="147"/>
+      <c r="BA1104" s="147"/>
+      <c r="BB1104" s="147"/>
+      <c r="BC1104" s="147"/>
+      <c r="BD1104" s="147"/>
+      <c r="BE1104" s="147"/>
+      <c r="BF1104" s="147"/>
+      <c r="BG1104" s="147"/>
+      <c r="BH1104" s="147"/>
+      <c r="BI1104" s="147"/>
+      <c r="BJ1104" s="147"/>
+      <c r="BK1104" s="147"/>
+      <c r="BL1104" s="147"/>
+      <c r="BM1104" s="147"/>
+      <c r="BN1104" s="147"/>
+      <c r="BO1104" s="147"/>
+      <c r="BP1104" s="147"/>
+      <c r="BQ1104" s="147"/>
+      <c r="BR1104" s="147"/>
+      <c r="BS1104" s="147"/>
+      <c r="BT1104" s="147"/>
+      <c r="BU1104" s="147"/>
+      <c r="BV1104" s="147"/>
+      <c r="BW1104" s="147"/>
+      <c r="BX1104" s="147"/>
+      <c r="BY1104" s="147"/>
+      <c r="BZ1104" s="147"/>
+      <c r="CA1104" s="147"/>
+      <c r="CB1104" s="147"/>
+      <c r="CC1104" s="147"/>
+      <c r="CD1104" s="147"/>
+      <c r="CE1104" s="147"/>
+      <c r="CF1104" s="147"/>
+      <c r="CG1104" s="147"/>
+      <c r="CH1104" s="147"/>
+      <c r="CI1104" s="147"/>
+      <c r="CJ1104" s="147"/>
+      <c r="CK1104" s="147"/>
+      <c r="CL1104" s="147"/>
+      <c r="CM1104" s="147"/>
+      <c r="CN1104" s="147"/>
+      <c r="CO1104" s="147"/>
+      <c r="CP1104" s="147"/>
+      <c r="CQ1104" s="147"/>
+      <c r="CR1104" s="147"/>
+      <c r="CS1104" s="147"/>
+      <c r="CT1104" s="147"/>
+      <c r="CU1104" s="147"/>
+      <c r="CV1104" s="147"/>
+      <c r="CW1104" s="147"/>
+      <c r="CX1104" s="147"/>
+      <c r="CY1104" s="147"/>
+      <c r="CZ1104" s="147"/>
+      <c r="DA1104" s="147"/>
+      <c r="DB1104" s="181"/>
+      <c r="DC1104" s="181"/>
+      <c r="DD1104" s="147"/>
+      <c r="DE1104" s="147"/>
+      <c r="DF1104" s="147"/>
+      <c r="DG1104" s="147"/>
+      <c r="DH1104" s="147"/>
+      <c r="DI1104" s="147"/>
+      <c r="DJ1104" s="147"/>
+      <c r="DK1104" s="147"/>
+      <c r="DL1104" s="147"/>
+      <c r="DM1104" s="147"/>
+      <c r="DN1104" s="147"/>
+      <c r="DO1104" s="147"/>
+    </row>
+    <row r="1105" spans="1:119" s="179" customFormat="1" ht="30">
+      <c r="A1105" s="178"/>
+      <c r="B1105" s="178"/>
+      <c r="C1105" s="178"/>
+      <c r="D1105" s="178" t="s">
+        <v>2165</v>
+      </c>
+      <c r="F1105" s="178" t="s">
+        <v>2163</v>
+      </c>
+      <c r="G1105" s="178" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1105" s="178"/>
+      <c r="I1105" s="178"/>
+      <c r="J1105" s="147"/>
+      <c r="K1105" s="147"/>
+      <c r="L1105" s="147"/>
+      <c r="M1105" s="147"/>
+      <c r="N1105" s="147"/>
+      <c r="O1105" s="147"/>
+      <c r="P1105" s="147"/>
+      <c r="Q1105" s="180"/>
+      <c r="R1105" s="147"/>
+      <c r="S1105" s="147"/>
+      <c r="T1105" s="147">
+        <v>1</v>
+      </c>
+      <c r="U1105" s="147"/>
+      <c r="V1105" s="147"/>
+      <c r="W1105" s="147"/>
+      <c r="X1105" s="147"/>
+      <c r="Y1105" s="147"/>
+      <c r="Z1105" s="147"/>
+      <c r="AA1105" s="147"/>
+      <c r="AB1105" s="147"/>
+      <c r="AC1105" s="147"/>
+      <c r="AD1105" s="147"/>
+      <c r="AE1105" s="147"/>
+      <c r="AF1105" s="147"/>
+      <c r="AG1105" s="147"/>
+      <c r="AH1105" s="147"/>
+      <c r="AI1105" s="147"/>
+      <c r="AJ1105" s="147"/>
+      <c r="AK1105" s="147"/>
+      <c r="AL1105" s="147"/>
+      <c r="AM1105" s="147"/>
+      <c r="AN1105" s="147"/>
+      <c r="AO1105" s="147"/>
+      <c r="AP1105" s="147"/>
+      <c r="AQ1105" s="147"/>
+      <c r="AR1105" s="147"/>
+      <c r="AS1105" s="147"/>
+      <c r="AT1105" s="147"/>
+      <c r="AU1105" s="147"/>
+      <c r="AV1105" s="147"/>
+      <c r="AW1105" s="147"/>
+      <c r="AX1105" s="147"/>
+      <c r="AY1105" s="147"/>
+      <c r="AZ1105" s="147"/>
+      <c r="BA1105" s="147"/>
+      <c r="BB1105" s="147"/>
+      <c r="BC1105" s="147"/>
+      <c r="BD1105" s="147"/>
+      <c r="BE1105" s="147"/>
+      <c r="BF1105" s="147"/>
+      <c r="BG1105" s="147"/>
+      <c r="BH1105" s="147"/>
+      <c r="BI1105" s="147"/>
+      <c r="BJ1105" s="147"/>
+      <c r="BK1105" s="147"/>
+      <c r="BL1105" s="147"/>
+      <c r="BM1105" s="147"/>
+      <c r="BN1105" s="147"/>
+      <c r="BO1105" s="147"/>
+      <c r="BP1105" s="147"/>
+      <c r="BQ1105" s="147"/>
+      <c r="BR1105" s="147"/>
+      <c r="BS1105" s="147"/>
+      <c r="BT1105" s="147"/>
+      <c r="BU1105" s="147"/>
+      <c r="BV1105" s="147"/>
+      <c r="BW1105" s="147"/>
+      <c r="BX1105" s="147"/>
+      <c r="BY1105" s="147"/>
+      <c r="BZ1105" s="147"/>
+      <c r="CA1105" s="147"/>
+      <c r="CB1105" s="147"/>
+      <c r="CC1105" s="147"/>
+      <c r="CD1105" s="147"/>
+      <c r="CE1105" s="147"/>
+      <c r="CF1105" s="147"/>
+      <c r="CG1105" s="147"/>
+      <c r="CH1105" s="147"/>
+      <c r="CI1105" s="147"/>
+      <c r="CJ1105" s="147"/>
+      <c r="CK1105" s="147"/>
+      <c r="CL1105" s="147"/>
+      <c r="CM1105" s="147"/>
+      <c r="CN1105" s="147"/>
+      <c r="CO1105" s="147"/>
+      <c r="CP1105" s="147"/>
+      <c r="CQ1105" s="147"/>
+      <c r="CR1105" s="147"/>
+      <c r="CS1105" s="147"/>
+      <c r="CT1105" s="147"/>
+      <c r="CU1105" s="147"/>
+      <c r="CV1105" s="147"/>
+      <c r="CW1105" s="147"/>
+      <c r="CX1105" s="147"/>
+      <c r="CY1105" s="147"/>
+      <c r="CZ1105" s="147"/>
+      <c r="DA1105" s="147"/>
+      <c r="DB1105" s="181"/>
+      <c r="DC1105" s="181"/>
+      <c r="DD1105" s="147"/>
+      <c r="DE1105" s="147"/>
+      <c r="DF1105" s="147"/>
+      <c r="DG1105" s="147"/>
+      <c r="DH1105" s="147"/>
+      <c r="DI1105" s="147"/>
+      <c r="DJ1105" s="147"/>
+      <c r="DK1105" s="147"/>
+      <c r="DL1105" s="147"/>
+      <c r="DM1105" s="147"/>
+      <c r="DN1105" s="147"/>
+      <c r="DO1105" s="147"/>
+    </row>
+    <row r="1106" spans="1:119" s="179" customFormat="1" ht="30">
+      <c r="A1106" s="178"/>
+      <c r="B1106" s="178"/>
+      <c r="C1106" s="178"/>
+      <c r="D1106" s="178" t="s">
+        <v>2166</v>
+      </c>
+      <c r="F1106" s="178" t="s">
+        <v>2163</v>
+      </c>
+      <c r="G1106" s="178" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1106" s="178"/>
+      <c r="I1106" s="178"/>
+      <c r="J1106" s="147"/>
+      <c r="K1106" s="147"/>
+      <c r="L1106" s="147"/>
+      <c r="M1106" s="147"/>
+      <c r="N1106" s="147"/>
+      <c r="O1106" s="147"/>
+      <c r="P1106" s="147"/>
+      <c r="Q1106" s="180"/>
+      <c r="R1106" s="147"/>
+      <c r="S1106" s="147"/>
+      <c r="T1106" s="147"/>
+      <c r="U1106" s="147">
+        <v>1</v>
+      </c>
+      <c r="V1106" s="147"/>
+      <c r="W1106" s="147"/>
+      <c r="X1106" s="147"/>
+      <c r="Y1106" s="147"/>
+      <c r="Z1106" s="147"/>
+      <c r="AA1106" s="147"/>
+      <c r="AB1106" s="147"/>
+      <c r="AC1106" s="147"/>
+      <c r="AD1106" s="147"/>
+      <c r="AE1106" s="147"/>
+      <c r="AF1106" s="147"/>
+      <c r="AG1106" s="147"/>
+      <c r="AH1106" s="147"/>
+      <c r="AI1106" s="147"/>
+      <c r="AJ1106" s="147"/>
+      <c r="AK1106" s="147"/>
+      <c r="AL1106" s="147"/>
+      <c r="AM1106" s="147"/>
+      <c r="AN1106" s="147"/>
+      <c r="AO1106" s="147"/>
+      <c r="AP1106" s="147"/>
+      <c r="AQ1106" s="147"/>
+      <c r="AR1106" s="147"/>
+      <c r="AS1106" s="147"/>
+      <c r="AT1106" s="147"/>
+      <c r="AU1106" s="147"/>
+      <c r="AV1106" s="147"/>
+      <c r="AW1106" s="147"/>
+      <c r="AX1106" s="147"/>
+      <c r="AY1106" s="147"/>
+      <c r="AZ1106" s="147"/>
+      <c r="BA1106" s="147"/>
+      <c r="BB1106" s="147"/>
+      <c r="BC1106" s="147"/>
+      <c r="BD1106" s="147"/>
+      <c r="BE1106" s="147"/>
+      <c r="BF1106" s="147"/>
+      <c r="BG1106" s="147"/>
+      <c r="BH1106" s="147"/>
+      <c r="BI1106" s="147"/>
+      <c r="BJ1106" s="147"/>
+      <c r="BK1106" s="147"/>
+      <c r="BL1106" s="147"/>
+      <c r="BM1106" s="147"/>
+      <c r="BN1106" s="147"/>
+      <c r="BO1106" s="147"/>
+      <c r="BP1106" s="147"/>
+      <c r="BQ1106" s="147"/>
+      <c r="BR1106" s="147"/>
+      <c r="BS1106" s="147"/>
+      <c r="BT1106" s="147"/>
+      <c r="BU1106" s="147"/>
+      <c r="BV1106" s="147"/>
+      <c r="BW1106" s="147"/>
+      <c r="BX1106" s="147"/>
+      <c r="BY1106" s="147"/>
+      <c r="BZ1106" s="147"/>
+      <c r="CA1106" s="147"/>
+      <c r="CB1106" s="147"/>
+      <c r="CC1106" s="147"/>
+      <c r="CD1106" s="147"/>
+      <c r="CE1106" s="147"/>
+      <c r="CF1106" s="147"/>
+      <c r="CG1106" s="147"/>
+      <c r="CH1106" s="147"/>
+      <c r="CI1106" s="147"/>
+      <c r="CJ1106" s="147"/>
+      <c r="CK1106" s="147"/>
+      <c r="CL1106" s="147"/>
+      <c r="CM1106" s="147"/>
+      <c r="CN1106" s="147"/>
+      <c r="CO1106" s="147"/>
+      <c r="CP1106" s="147"/>
+      <c r="CQ1106" s="147"/>
+      <c r="CR1106" s="147"/>
+      <c r="CS1106" s="147"/>
+      <c r="CT1106" s="147"/>
+      <c r="CU1106" s="147"/>
+      <c r="CV1106" s="147"/>
+      <c r="CW1106" s="147"/>
+      <c r="CX1106" s="147"/>
+      <c r="CY1106" s="147"/>
+      <c r="CZ1106" s="147"/>
+      <c r="DA1106" s="147"/>
+      <c r="DB1106" s="181"/>
+      <c r="DC1106" s="181"/>
+      <c r="DD1106" s="147"/>
+      <c r="DE1106" s="147"/>
+      <c r="DF1106" s="147"/>
+      <c r="DG1106" s="147"/>
+      <c r="DH1106" s="147"/>
+      <c r="DI1106" s="147"/>
+      <c r="DJ1106" s="147"/>
+      <c r="DK1106" s="147"/>
+      <c r="DL1106" s="147"/>
+      <c r="DM1106" s="147"/>
+      <c r="DN1106" s="147"/>
+      <c r="DO1106" s="147"/>
+    </row>
+    <row r="1107" spans="1:119" s="179" customFormat="1" ht="30">
+      <c r="A1107" s="178"/>
+      <c r="B1107" s="178"/>
+      <c r="C1107" s="178"/>
+      <c r="D1107" s="178" t="s">
+        <v>2167</v>
+      </c>
+      <c r="F1107" s="178" t="s">
+        <v>2163</v>
+      </c>
+      <c r="G1107" s="178" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1107" s="178"/>
+      <c r="I1107" s="178"/>
+      <c r="J1107" s="147"/>
+      <c r="K1107" s="147"/>
+      <c r="L1107" s="147"/>
+      <c r="M1107" s="147"/>
+      <c r="N1107" s="147"/>
+      <c r="O1107" s="147"/>
+      <c r="P1107" s="147"/>
+      <c r="Q1107" s="180"/>
+      <c r="R1107" s="147"/>
+      <c r="S1107" s="147"/>
+      <c r="T1107" s="147"/>
+      <c r="U1107" s="147"/>
+      <c r="V1107" s="147">
+        <v>1</v>
+      </c>
+      <c r="W1107" s="147"/>
+      <c r="X1107" s="147"/>
+      <c r="Y1107" s="147"/>
+      <c r="Z1107" s="147"/>
+      <c r="AA1107" s="147"/>
+      <c r="AB1107" s="147"/>
+      <c r="AC1107" s="147"/>
+      <c r="AD1107" s="147"/>
+      <c r="AE1107" s="147"/>
+      <c r="AF1107" s="147"/>
+      <c r="AG1107" s="147"/>
+      <c r="AH1107" s="147"/>
+      <c r="AI1107" s="147"/>
+      <c r="AJ1107" s="147"/>
+      <c r="AK1107" s="147"/>
+      <c r="AL1107" s="147"/>
+      <c r="AM1107" s="147"/>
+      <c r="AN1107" s="147"/>
+      <c r="AO1107" s="147"/>
+      <c r="AP1107" s="147"/>
+      <c r="AQ1107" s="147"/>
+      <c r="AR1107" s="147"/>
+      <c r="AS1107" s="147"/>
+      <c r="AT1107" s="147"/>
+      <c r="AU1107" s="147"/>
+      <c r="AV1107" s="147"/>
+      <c r="AW1107" s="147"/>
+      <c r="AX1107" s="147"/>
+      <c r="AY1107" s="147"/>
+      <c r="AZ1107" s="147"/>
+      <c r="BA1107" s="147"/>
+      <c r="BB1107" s="147"/>
+      <c r="BC1107" s="147"/>
+      <c r="BD1107" s="147"/>
+      <c r="BE1107" s="147"/>
+      <c r="BF1107" s="147"/>
+      <c r="BG1107" s="147"/>
+      <c r="BH1107" s="147"/>
+      <c r="BI1107" s="147"/>
+      <c r="BJ1107" s="147"/>
+      <c r="BK1107" s="147"/>
+      <c r="BL1107" s="147"/>
+      <c r="BM1107" s="147"/>
+      <c r="BN1107" s="147"/>
+      <c r="BO1107" s="147"/>
+      <c r="BP1107" s="147"/>
+      <c r="BQ1107" s="147"/>
+      <c r="BR1107" s="147"/>
+      <c r="BS1107" s="147"/>
+      <c r="BT1107" s="147"/>
+      <c r="BU1107" s="147"/>
+      <c r="BV1107" s="147"/>
+      <c r="BW1107" s="147"/>
+      <c r="BX1107" s="147"/>
+      <c r="BY1107" s="147"/>
+      <c r="BZ1107" s="147"/>
+      <c r="CA1107" s="147"/>
+      <c r="CB1107" s="147"/>
+      <c r="CC1107" s="147"/>
+      <c r="CD1107" s="147"/>
+      <c r="CE1107" s="147"/>
+      <c r="CF1107" s="147"/>
+      <c r="CG1107" s="147"/>
+      <c r="CH1107" s="147"/>
+      <c r="CI1107" s="147"/>
+      <c r="CJ1107" s="147"/>
+      <c r="CK1107" s="147"/>
+      <c r="CL1107" s="147"/>
+      <c r="CM1107" s="147"/>
+      <c r="CN1107" s="147"/>
+      <c r="CO1107" s="147"/>
+      <c r="CP1107" s="147"/>
+      <c r="CQ1107" s="147"/>
+      <c r="CR1107" s="147"/>
+      <c r="CS1107" s="147"/>
+      <c r="CT1107" s="147"/>
+      <c r="CU1107" s="147"/>
+      <c r="CV1107" s="147"/>
+      <c r="CW1107" s="147"/>
+      <c r="CX1107" s="147"/>
+      <c r="CY1107" s="147"/>
+      <c r="CZ1107" s="147"/>
+      <c r="DA1107" s="147"/>
+      <c r="DB1107" s="181"/>
+      <c r="DC1107" s="181"/>
+      <c r="DD1107" s="147"/>
+      <c r="DE1107" s="147"/>
+      <c r="DF1107" s="147"/>
+      <c r="DG1107" s="147"/>
+      <c r="DH1107" s="147"/>
+      <c r="DI1107" s="147"/>
+      <c r="DJ1107" s="147"/>
+      <c r="DK1107" s="147"/>
+      <c r="DL1107" s="147"/>
+      <c r="DM1107" s="147"/>
+      <c r="DN1107" s="147"/>
+      <c r="DO1107" s="147"/>
+    </row>
+    <row r="1108" spans="1:119" s="179" customFormat="1" ht="30">
+      <c r="A1108" s="178"/>
+      <c r="B1108" s="178"/>
+      <c r="C1108" s="178"/>
+      <c r="D1108" s="178" t="s">
+        <v>2168</v>
+      </c>
+      <c r="F1108" s="178" t="s">
+        <v>2163</v>
+      </c>
+      <c r="G1108" s="178" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1108" s="178"/>
+      <c r="I1108" s="178"/>
+      <c r="J1108" s="147"/>
+      <c r="K1108" s="147"/>
+      <c r="L1108" s="147"/>
+      <c r="M1108" s="147"/>
+      <c r="N1108" s="147"/>
+      <c r="O1108" s="147"/>
+      <c r="P1108" s="147"/>
+      <c r="Q1108" s="180"/>
+      <c r="R1108" s="147"/>
+      <c r="S1108" s="147"/>
+      <c r="T1108" s="147"/>
+      <c r="U1108" s="147"/>
+      <c r="V1108" s="147"/>
+      <c r="W1108" s="147">
+        <v>1</v>
+      </c>
+      <c r="X1108" s="147"/>
+      <c r="Y1108" s="147"/>
+      <c r="Z1108" s="147"/>
+      <c r="AA1108" s="147"/>
+      <c r="AB1108" s="147"/>
+      <c r="AC1108" s="147"/>
+      <c r="AD1108" s="147"/>
+      <c r="AE1108" s="147"/>
+      <c r="AF1108" s="147"/>
+      <c r="AG1108" s="147"/>
+      <c r="AH1108" s="147"/>
+      <c r="AI1108" s="147"/>
+      <c r="AJ1108" s="147"/>
+      <c r="AK1108" s="147"/>
+      <c r="AL1108" s="147"/>
+      <c r="AM1108" s="147"/>
+      <c r="AN1108" s="147"/>
+      <c r="AO1108" s="147"/>
+      <c r="AP1108" s="147"/>
+      <c r="AQ1108" s="147"/>
+      <c r="AR1108" s="147"/>
+      <c r="AS1108" s="147"/>
+      <c r="AT1108" s="147"/>
+      <c r="AU1108" s="147"/>
+      <c r="AV1108" s="147"/>
+      <c r="AW1108" s="147"/>
+      <c r="AX1108" s="147"/>
+      <c r="AY1108" s="147"/>
+      <c r="AZ1108" s="147"/>
+      <c r="BA1108" s="147"/>
+      <c r="BB1108" s="147"/>
+      <c r="BC1108" s="147"/>
+      <c r="BD1108" s="147"/>
+      <c r="BE1108" s="147"/>
+      <c r="BF1108" s="147"/>
+      <c r="BG1108" s="147"/>
+      <c r="BH1108" s="147"/>
+      <c r="BI1108" s="147"/>
+      <c r="BJ1108" s="147"/>
+      <c r="BK1108" s="147"/>
+      <c r="BL1108" s="147"/>
+      <c r="BM1108" s="147"/>
+      <c r="BN1108" s="147"/>
+      <c r="BO1108" s="147"/>
+      <c r="BP1108" s="147"/>
+      <c r="BQ1108" s="147"/>
+      <c r="BR1108" s="147"/>
+      <c r="BS1108" s="147"/>
+      <c r="BT1108" s="147"/>
+      <c r="BU1108" s="147"/>
+      <c r="BV1108" s="147"/>
+      <c r="BW1108" s="147"/>
+      <c r="BX1108" s="147"/>
+      <c r="BY1108" s="147"/>
+      <c r="BZ1108" s="147"/>
+      <c r="CA1108" s="147"/>
+      <c r="CB1108" s="147"/>
+      <c r="CC1108" s="147"/>
+      <c r="CD1108" s="147"/>
+      <c r="CE1108" s="147"/>
+      <c r="CF1108" s="147"/>
+      <c r="CG1108" s="147"/>
+      <c r="CH1108" s="147"/>
+      <c r="CI1108" s="147"/>
+      <c r="CJ1108" s="147"/>
+      <c r="CK1108" s="147"/>
+      <c r="CL1108" s="147"/>
+      <c r="CM1108" s="147"/>
+      <c r="CN1108" s="147"/>
+      <c r="CO1108" s="147"/>
+      <c r="CP1108" s="147"/>
+      <c r="CQ1108" s="147"/>
+      <c r="CR1108" s="147"/>
+      <c r="CS1108" s="147"/>
+      <c r="CT1108" s="147"/>
+      <c r="CU1108" s="147"/>
+      <c r="CV1108" s="147"/>
+      <c r="CW1108" s="147"/>
+      <c r="CX1108" s="147"/>
+      <c r="CY1108" s="147"/>
+      <c r="CZ1108" s="147"/>
+      <c r="DA1108" s="147"/>
+      <c r="DB1108" s="181"/>
+      <c r="DC1108" s="181"/>
+      <c r="DD1108" s="147"/>
+      <c r="DE1108" s="147"/>
+      <c r="DF1108" s="147"/>
+      <c r="DG1108" s="147"/>
+      <c r="DH1108" s="147"/>
+      <c r="DI1108" s="147"/>
+      <c r="DJ1108" s="147"/>
+      <c r="DK1108" s="147"/>
+      <c r="DL1108" s="147"/>
+      <c r="DM1108" s="147"/>
+      <c r="DN1108" s="147"/>
+      <c r="DO1108" s="147"/>
+    </row>
+    <row r="1109" spans="1:119" s="179" customFormat="1" ht="30">
+      <c r="A1109" s="182"/>
+      <c r="B1109" s="178"/>
+      <c r="C1109" s="178"/>
+      <c r="D1109" s="178" t="s">
+        <v>2169</v>
+      </c>
+      <c r="F1109" s="178" t="s">
+        <v>2163</v>
+      </c>
+      <c r="G1109" s="178" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1109" s="178"/>
+      <c r="I1109" s="178"/>
+      <c r="J1109" s="147"/>
+      <c r="K1109" s="147"/>
+      <c r="L1109" s="147"/>
+      <c r="M1109" s="147"/>
+      <c r="N1109" s="147"/>
+      <c r="O1109" s="147"/>
+      <c r="P1109" s="147"/>
+      <c r="Q1109" s="180"/>
+      <c r="R1109" s="147"/>
+      <c r="S1109" s="147"/>
+      <c r="T1109" s="147"/>
+      <c r="U1109" s="147"/>
+      <c r="V1109" s="147"/>
+      <c r="W1109" s="147"/>
+      <c r="X1109" s="147">
+        <v>1</v>
+      </c>
+      <c r="Y1109" s="147"/>
+      <c r="Z1109" s="147"/>
+      <c r="AA1109" s="147"/>
+      <c r="AB1109" s="147"/>
+      <c r="AC1109" s="147"/>
+      <c r="AD1109" s="147"/>
+      <c r="AE1109" s="147"/>
+      <c r="AF1109" s="147"/>
+      <c r="AG1109" s="147"/>
+      <c r="AH1109" s="147"/>
+      <c r="AI1109" s="147"/>
+      <c r="AJ1109" s="147"/>
+      <c r="AK1109" s="147"/>
+      <c r="AL1109" s="147"/>
+      <c r="AM1109" s="147"/>
+      <c r="AN1109" s="147"/>
+      <c r="AO1109" s="147"/>
+      <c r="AP1109" s="147"/>
+      <c r="AQ1109" s="147"/>
+      <c r="AR1109" s="147"/>
+      <c r="AS1109" s="147"/>
+      <c r="AT1109" s="147"/>
+      <c r="AU1109" s="147"/>
+      <c r="AV1109" s="147"/>
+      <c r="AW1109" s="147"/>
+      <c r="AX1109" s="147"/>
+      <c r="AY1109" s="147"/>
+      <c r="AZ1109" s="147"/>
+      <c r="BA1109" s="147"/>
+      <c r="BB1109" s="147"/>
+      <c r="BC1109" s="147"/>
+      <c r="BD1109" s="147"/>
+      <c r="BE1109" s="147"/>
+      <c r="BF1109" s="147"/>
+      <c r="BG1109" s="147"/>
+      <c r="BH1109" s="147"/>
+      <c r="BI1109" s="147"/>
+      <c r="BJ1109" s="147"/>
+      <c r="BK1109" s="147"/>
+      <c r="BL1109" s="147"/>
+      <c r="BM1109" s="147"/>
+      <c r="BN1109" s="147"/>
+      <c r="BO1109" s="147"/>
+      <c r="BP1109" s="147"/>
+      <c r="BQ1109" s="147"/>
+      <c r="BR1109" s="147"/>
+      <c r="BS1109" s="147"/>
+      <c r="BT1109" s="147"/>
+      <c r="BU1109" s="147"/>
+      <c r="BV1109" s="147"/>
+      <c r="BW1109" s="147"/>
+      <c r="BX1109" s="147"/>
+      <c r="BY1109" s="147"/>
+      <c r="BZ1109" s="147"/>
+      <c r="CA1109" s="147"/>
+      <c r="CB1109" s="147"/>
+      <c r="CC1109" s="147"/>
+      <c r="CD1109" s="147"/>
+      <c r="CE1109" s="147"/>
+      <c r="CF1109" s="147"/>
+      <c r="CG1109" s="147"/>
+      <c r="CH1109" s="147"/>
+      <c r="CI1109" s="147"/>
+      <c r="CJ1109" s="147"/>
+      <c r="CK1109" s="147"/>
+      <c r="CL1109" s="147"/>
+      <c r="CM1109" s="147"/>
+      <c r="CN1109" s="147"/>
+      <c r="CO1109" s="147"/>
+      <c r="CP1109" s="147"/>
+      <c r="CQ1109" s="147"/>
+      <c r="CR1109" s="147"/>
+      <c r="CS1109" s="147"/>
+      <c r="CT1109" s="147"/>
+      <c r="CU1109" s="147"/>
+      <c r="CV1109" s="147"/>
+      <c r="CW1109" s="147"/>
+      <c r="CX1109" s="147"/>
+      <c r="CY1109" s="147"/>
+      <c r="CZ1109" s="147"/>
+      <c r="DA1109" s="147"/>
+      <c r="DB1109" s="181"/>
+      <c r="DC1109" s="181"/>
+      <c r="DD1109" s="147"/>
+      <c r="DE1109" s="147"/>
+      <c r="DF1109" s="147"/>
+      <c r="DG1109" s="147"/>
+      <c r="DH1109" s="147"/>
+      <c r="DI1109" s="147"/>
+      <c r="DJ1109" s="147"/>
+      <c r="DK1109" s="147"/>
+      <c r="DL1109" s="147"/>
+      <c r="DM1109" s="147"/>
+      <c r="DN1109" s="147"/>
+      <c r="DO1109" s="147"/>
+    </row>
+    <row r="1110" spans="1:119" s="179" customFormat="1" ht="30">
+      <c r="A1110" s="178"/>
+      <c r="B1110" s="178"/>
+      <c r="C1110" s="178"/>
+      <c r="D1110" s="178" t="s">
+        <v>2170</v>
+      </c>
+      <c r="F1110" s="178" t="s">
+        <v>2163</v>
+      </c>
+      <c r="G1110" s="178" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1110" s="178"/>
+      <c r="I1110" s="178"/>
+      <c r="J1110" s="147"/>
+      <c r="K1110" s="147"/>
+      <c r="L1110" s="147"/>
+      <c r="M1110" s="147"/>
+      <c r="N1110" s="147"/>
+      <c r="O1110" s="147"/>
+      <c r="P1110" s="147"/>
+      <c r="Q1110" s="180"/>
+      <c r="R1110" s="147"/>
+      <c r="S1110" s="147"/>
+      <c r="T1110" s="147"/>
+      <c r="U1110" s="147"/>
+      <c r="V1110" s="147"/>
+      <c r="W1110" s="147"/>
+      <c r="X1110" s="147"/>
+      <c r="Y1110" s="147">
+        <v>1</v>
+      </c>
+      <c r="Z1110" s="147"/>
+      <c r="AA1110" s="147"/>
+      <c r="AB1110" s="147"/>
+      <c r="AC1110" s="147"/>
+      <c r="AD1110" s="147"/>
+      <c r="AE1110" s="147"/>
+      <c r="AF1110" s="147"/>
+      <c r="AG1110" s="147"/>
+      <c r="AH1110" s="147"/>
+      <c r="AI1110" s="147"/>
+      <c r="AJ1110" s="147"/>
+      <c r="AK1110" s="147"/>
+      <c r="AL1110" s="147"/>
+      <c r="AM1110" s="147"/>
+      <c r="AN1110" s="147"/>
+      <c r="AO1110" s="147"/>
+      <c r="AP1110" s="147"/>
+      <c r="AQ1110" s="147"/>
+      <c r="AR1110" s="147"/>
+      <c r="AS1110" s="147"/>
+      <c r="AT1110" s="147"/>
+      <c r="AU1110" s="147"/>
+      <c r="AV1110" s="147"/>
+      <c r="AW1110" s="147"/>
+      <c r="AX1110" s="147"/>
+      <c r="AY1110" s="147"/>
+      <c r="AZ1110" s="147"/>
+      <c r="BA1110" s="147"/>
+      <c r="BB1110" s="147"/>
+      <c r="BC1110" s="147"/>
+      <c r="BD1110" s="147"/>
+      <c r="BE1110" s="147"/>
+      <c r="BF1110" s="147"/>
+      <c r="BG1110" s="147"/>
+      <c r="BH1110" s="147"/>
+      <c r="BI1110" s="147"/>
+      <c r="BJ1110" s="147"/>
+      <c r="BK1110" s="147"/>
+      <c r="BL1110" s="147"/>
+      <c r="BM1110" s="147"/>
+      <c r="BN1110" s="147"/>
+      <c r="BO1110" s="147"/>
+      <c r="BP1110" s="147"/>
+      <c r="BQ1110" s="147"/>
+      <c r="BR1110" s="147"/>
+      <c r="BS1110" s="147"/>
+      <c r="BT1110" s="147"/>
+      <c r="BU1110" s="147"/>
+      <c r="BV1110" s="147"/>
+      <c r="BW1110" s="147"/>
+      <c r="BX1110" s="147"/>
+      <c r="BY1110" s="147"/>
+      <c r="BZ1110" s="147"/>
+      <c r="CA1110" s="147"/>
+      <c r="CB1110" s="147"/>
+      <c r="CC1110" s="147"/>
+      <c r="CD1110" s="147"/>
+      <c r="CE1110" s="147"/>
+      <c r="CF1110" s="147"/>
+      <c r="CG1110" s="147"/>
+      <c r="CH1110" s="147"/>
+      <c r="CI1110" s="147"/>
+      <c r="CJ1110" s="147"/>
+      <c r="CK1110" s="147"/>
+      <c r="CL1110" s="147"/>
+      <c r="CM1110" s="147"/>
+      <c r="CN1110" s="147"/>
+      <c r="CO1110" s="147"/>
+      <c r="CP1110" s="147"/>
+      <c r="CQ1110" s="147"/>
+      <c r="CR1110" s="147"/>
+      <c r="CS1110" s="147"/>
+      <c r="CT1110" s="147"/>
+      <c r="CU1110" s="147"/>
+      <c r="CV1110" s="147"/>
+      <c r="CW1110" s="147"/>
+      <c r="CX1110" s="147"/>
+      <c r="CY1110" s="147"/>
+      <c r="CZ1110" s="147"/>
+      <c r="DA1110" s="147"/>
+      <c r="DB1110" s="181"/>
+      <c r="DC1110" s="181"/>
+      <c r="DD1110" s="147"/>
+      <c r="DE1110" s="147"/>
+      <c r="DF1110" s="147"/>
+      <c r="DG1110" s="147"/>
+      <c r="DH1110" s="147"/>
+      <c r="DI1110" s="147"/>
+      <c r="DJ1110" s="147"/>
+      <c r="DK1110" s="147"/>
+      <c r="DL1110" s="147"/>
+      <c r="DM1110" s="147"/>
+      <c r="DN1110" s="147"/>
+      <c r="DO1110" s="147"/>
+    </row>
+    <row r="1111" spans="1:119" s="179" customFormat="1" ht="30">
+      <c r="A1111" s="178"/>
+      <c r="B1111" s="178"/>
+      <c r="C1111" s="178"/>
+      <c r="D1111" s="178" t="s">
+        <v>2171</v>
+      </c>
+      <c r="F1111" s="178" t="s">
+        <v>2163</v>
+      </c>
+      <c r="G1111" s="178" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1111" s="178"/>
+      <c r="I1111" s="178"/>
+      <c r="J1111" s="147"/>
+      <c r="K1111" s="147"/>
+      <c r="L1111" s="147"/>
+      <c r="M1111" s="147"/>
+      <c r="N1111" s="147"/>
+      <c r="O1111" s="147"/>
+      <c r="P1111" s="147"/>
+      <c r="Q1111" s="180"/>
+      <c r="R1111" s="147"/>
+      <c r="S1111" s="147"/>
+      <c r="T1111" s="147"/>
+      <c r="U1111" s="147"/>
+      <c r="V1111" s="147"/>
+      <c r="W1111" s="147"/>
+      <c r="X1111" s="147"/>
+      <c r="Y1111" s="147"/>
+      <c r="Z1111" s="147">
+        <v>1</v>
+      </c>
+      <c r="AA1111" s="147"/>
+      <c r="AB1111" s="147"/>
+      <c r="AC1111" s="147"/>
+      <c r="AD1111" s="147"/>
+      <c r="AE1111" s="147"/>
+      <c r="AF1111" s="147"/>
+      <c r="AG1111" s="147"/>
+      <c r="AH1111" s="147"/>
+      <c r="AI1111" s="147"/>
+      <c r="AJ1111" s="147"/>
+      <c r="AK1111" s="147"/>
+      <c r="AL1111" s="147"/>
+      <c r="AM1111" s="147"/>
+      <c r="AN1111" s="147"/>
+      <c r="AO1111" s="147"/>
+      <c r="AP1111" s="147"/>
+      <c r="AQ1111" s="147"/>
+      <c r="AR1111" s="147"/>
+      <c r="AS1111" s="147"/>
+      <c r="AT1111" s="147"/>
+      <c r="AU1111" s="147"/>
+      <c r="AV1111" s="147"/>
+      <c r="AW1111" s="147"/>
+      <c r="AX1111" s="147"/>
+      <c r="AY1111" s="147"/>
+      <c r="AZ1111" s="147"/>
+      <c r="BA1111" s="147"/>
+      <c r="BB1111" s="147"/>
+      <c r="BC1111" s="147"/>
+      <c r="BD1111" s="147"/>
+      <c r="BE1111" s="147"/>
+      <c r="BF1111" s="147"/>
+      <c r="BG1111" s="147"/>
+      <c r="BH1111" s="147"/>
+      <c r="BI1111" s="147"/>
+      <c r="BJ1111" s="147"/>
+      <c r="BK1111" s="147"/>
+      <c r="BL1111" s="147"/>
+      <c r="BM1111" s="147"/>
+      <c r="BN1111" s="147"/>
+      <c r="BO1111" s="147"/>
+      <c r="BP1111" s="147"/>
+      <c r="BQ1111" s="147"/>
+      <c r="BR1111" s="147"/>
+      <c r="BS1111" s="147"/>
+      <c r="BT1111" s="147"/>
+      <c r="BU1111" s="147"/>
+      <c r="BV1111" s="147"/>
+      <c r="BW1111" s="147"/>
+      <c r="BX1111" s="147"/>
+      <c r="BY1111" s="147"/>
+      <c r="BZ1111" s="147"/>
+      <c r="CA1111" s="147"/>
+      <c r="CB1111" s="147"/>
+      <c r="CC1111" s="147"/>
+      <c r="CD1111" s="147"/>
+      <c r="CE1111" s="147"/>
+      <c r="CF1111" s="147"/>
+      <c r="CG1111" s="147"/>
+      <c r="CH1111" s="147"/>
+      <c r="CI1111" s="147"/>
+      <c r="CJ1111" s="147"/>
+      <c r="CK1111" s="147"/>
+      <c r="CL1111" s="147"/>
+      <c r="CM1111" s="147"/>
+      <c r="CN1111" s="147"/>
+      <c r="CO1111" s="147"/>
+      <c r="CP1111" s="147"/>
+      <c r="CQ1111" s="147"/>
+      <c r="CR1111" s="147"/>
+      <c r="CS1111" s="147"/>
+      <c r="CT1111" s="147"/>
+      <c r="CU1111" s="147"/>
+      <c r="CV1111" s="147"/>
+      <c r="CW1111" s="147"/>
+      <c r="CX1111" s="147"/>
+      <c r="CY1111" s="147"/>
+      <c r="CZ1111" s="147"/>
+      <c r="DA1111" s="147"/>
+      <c r="DB1111" s="181"/>
+      <c r="DC1111" s="181"/>
+      <c r="DD1111" s="147"/>
+      <c r="DE1111" s="147"/>
+      <c r="DF1111" s="147"/>
+      <c r="DG1111" s="147"/>
+      <c r="DH1111" s="147"/>
+      <c r="DI1111" s="147"/>
+      <c r="DJ1111" s="147"/>
+      <c r="DK1111" s="147"/>
+      <c r="DL1111" s="147"/>
+      <c r="DM1111" s="147"/>
+      <c r="DN1111" s="147"/>
+      <c r="DO1111" s="147"/>
+    </row>
+    <row r="1112" spans="1:119" s="179" customFormat="1" ht="30">
+      <c r="A1112" s="178"/>
+      <c r="B1112" s="178"/>
+      <c r="C1112" s="178"/>
+      <c r="D1112" s="178" t="s">
+        <v>2172</v>
+      </c>
+      <c r="F1112" s="178" t="s">
+        <v>2163</v>
+      </c>
+      <c r="G1112" s="178" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1112" s="178"/>
+      <c r="I1112" s="178"/>
+      <c r="J1112" s="147"/>
+      <c r="K1112" s="147"/>
+      <c r="L1112" s="147"/>
+      <c r="M1112" s="147"/>
+      <c r="N1112" s="147"/>
+      <c r="O1112" s="147"/>
+      <c r="P1112" s="147"/>
+      <c r="Q1112" s="180"/>
+      <c r="R1112" s="147"/>
+      <c r="S1112" s="147"/>
+      <c r="T1112" s="147"/>
+      <c r="U1112" s="147"/>
+      <c r="V1112" s="147"/>
+      <c r="W1112" s="147"/>
+      <c r="X1112" s="147"/>
+      <c r="Y1112" s="147"/>
+      <c r="Z1112" s="147"/>
+      <c r="AA1112" s="147">
+        <v>1</v>
+      </c>
+      <c r="AB1112" s="147"/>
+      <c r="AC1112" s="147"/>
+      <c r="AD1112" s="147"/>
+      <c r="AE1112" s="147"/>
+      <c r="AF1112" s="147"/>
+      <c r="AG1112" s="147"/>
+      <c r="AH1112" s="147"/>
+      <c r="AI1112" s="147"/>
+      <c r="AJ1112" s="147"/>
+      <c r="AK1112" s="147"/>
+      <c r="AL1112" s="147"/>
+      <c r="AM1112" s="147"/>
+      <c r="AN1112" s="147"/>
+      <c r="AO1112" s="147"/>
+      <c r="AP1112" s="147"/>
+      <c r="AQ1112" s="147"/>
+      <c r="AR1112" s="147"/>
+      <c r="AS1112" s="147"/>
+      <c r="AT1112" s="147"/>
+      <c r="AU1112" s="147"/>
+      <c r="AV1112" s="147"/>
+      <c r="AW1112" s="147"/>
+      <c r="AX1112" s="147"/>
+      <c r="AY1112" s="147"/>
+      <c r="AZ1112" s="147"/>
+      <c r="BA1112" s="147"/>
+      <c r="BB1112" s="147"/>
+      <c r="BC1112" s="147"/>
+      <c r="BD1112" s="147"/>
+      <c r="BE1112" s="147"/>
+      <c r="BF1112" s="147"/>
+      <c r="BG1112" s="147"/>
+      <c r="BH1112" s="147"/>
+      <c r="BI1112" s="147"/>
+      <c r="BJ1112" s="147"/>
+      <c r="BK1112" s="147"/>
+      <c r="BL1112" s="147"/>
+      <c r="BM1112" s="147"/>
+      <c r="BN1112" s="147"/>
+      <c r="BO1112" s="147"/>
+      <c r="BP1112" s="147"/>
+      <c r="BQ1112" s="147"/>
+      <c r="BR1112" s="147"/>
+      <c r="BS1112" s="147"/>
+      <c r="BT1112" s="147"/>
+      <c r="BU1112" s="147"/>
+      <c r="BV1112" s="147"/>
+      <c r="BW1112" s="147"/>
+      <c r="BX1112" s="147"/>
+      <c r="BY1112" s="147"/>
+      <c r="BZ1112" s="147"/>
+      <c r="CA1112" s="147"/>
+      <c r="CB1112" s="147"/>
+      <c r="CC1112" s="147"/>
+      <c r="CD1112" s="147"/>
+      <c r="CE1112" s="147"/>
+      <c r="CF1112" s="147"/>
+      <c r="CG1112" s="147"/>
+      <c r="CH1112" s="147"/>
+      <c r="CI1112" s="147"/>
+      <c r="CJ1112" s="147"/>
+      <c r="CK1112" s="147"/>
+      <c r="CL1112" s="147"/>
+      <c r="CM1112" s="147"/>
+      <c r="CN1112" s="147"/>
+      <c r="CO1112" s="147"/>
+      <c r="CP1112" s="147"/>
+      <c r="CQ1112" s="147"/>
+      <c r="CR1112" s="147"/>
+      <c r="CS1112" s="147"/>
+      <c r="CT1112" s="147"/>
+      <c r="CU1112" s="147"/>
+      <c r="CV1112" s="147"/>
+      <c r="CW1112" s="147"/>
+      <c r="CX1112" s="147"/>
+      <c r="CY1112" s="147"/>
+      <c r="CZ1112" s="147"/>
+      <c r="DA1112" s="147"/>
+      <c r="DB1112" s="181"/>
+      <c r="DC1112" s="181"/>
+      <c r="DD1112" s="147"/>
+      <c r="DE1112" s="147"/>
+      <c r="DF1112" s="147"/>
+      <c r="DG1112" s="147"/>
+      <c r="DH1112" s="147"/>
+      <c r="DI1112" s="147"/>
+      <c r="DJ1112" s="147"/>
+      <c r="DK1112" s="147"/>
+      <c r="DL1112" s="147"/>
+      <c r="DM1112" s="147"/>
+      <c r="DN1112" s="147"/>
+      <c r="DO1112" s="147"/>
+    </row>
+    <row r="1113" spans="1:119" s="179" customFormat="1" ht="30">
+      <c r="A1113" s="178"/>
+      <c r="B1113" s="178"/>
+      <c r="C1113" s="178"/>
+      <c r="D1113" s="178" t="s">
+        <v>2173</v>
+      </c>
+      <c r="F1113" s="178" t="s">
+        <v>2163</v>
+      </c>
+      <c r="G1113" s="178" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1113" s="178"/>
+      <c r="I1113" s="178"/>
+      <c r="J1113" s="147"/>
+      <c r="K1113" s="147"/>
+      <c r="L1113" s="147"/>
+      <c r="M1113" s="147"/>
+      <c r="N1113" s="147"/>
+      <c r="O1113" s="147"/>
+      <c r="P1113" s="147"/>
+      <c r="Q1113" s="180"/>
+      <c r="R1113" s="147"/>
+      <c r="S1113" s="147"/>
+      <c r="T1113" s="147"/>
+      <c r="U1113" s="147"/>
+      <c r="V1113" s="147"/>
+      <c r="W1113" s="147"/>
+      <c r="X1113" s="147"/>
+      <c r="Y1113" s="147"/>
+      <c r="Z1113" s="147"/>
+      <c r="AA1113" s="147"/>
+      <c r="AB1113" s="147">
+        <v>1</v>
+      </c>
+      <c r="AC1113" s="147"/>
+      <c r="AD1113" s="147"/>
+      <c r="AE1113" s="147"/>
+      <c r="AF1113" s="147"/>
+      <c r="AG1113" s="147"/>
+      <c r="AH1113" s="147"/>
+      <c r="AI1113" s="147"/>
+      <c r="AJ1113" s="147"/>
+      <c r="AK1113" s="147"/>
+      <c r="AL1113" s="147"/>
+      <c r="AM1113" s="147"/>
+      <c r="AN1113" s="147"/>
+      <c r="AO1113" s="147"/>
+      <c r="AP1113" s="147"/>
+      <c r="AQ1113" s="147"/>
+      <c r="AR1113" s="147"/>
+      <c r="AS1113" s="147"/>
+      <c r="AT1113" s="147"/>
+      <c r="AU1113" s="147"/>
+      <c r="AV1113" s="147"/>
+      <c r="AW1113" s="147"/>
+      <c r="AX1113" s="147"/>
+      <c r="AY1113" s="147"/>
+      <c r="AZ1113" s="147"/>
+      <c r="BA1113" s="147"/>
+      <c r="BB1113" s="147"/>
+      <c r="BC1113" s="147"/>
+      <c r="BD1113" s="147"/>
+      <c r="BE1113" s="147"/>
+      <c r="BF1113" s="147"/>
+      <c r="BG1113" s="147"/>
+      <c r="BH1113" s="147"/>
+      <c r="BI1113" s="147"/>
+      <c r="BJ1113" s="147"/>
+      <c r="BK1113" s="147"/>
+      <c r="BL1113" s="147"/>
+      <c r="BM1113" s="147"/>
+      <c r="BN1113" s="147"/>
+      <c r="BO1113" s="147"/>
+      <c r="BP1113" s="147"/>
+      <c r="BQ1113" s="147"/>
+      <c r="BR1113" s="147"/>
+      <c r="BS1113" s="147"/>
+      <c r="BT1113" s="147"/>
+      <c r="BU1113" s="147"/>
+      <c r="BV1113" s="147"/>
+      <c r="BW1113" s="147"/>
+      <c r="BX1113" s="147"/>
+      <c r="BY1113" s="147"/>
+      <c r="BZ1113" s="147"/>
+      <c r="CA1113" s="147"/>
+      <c r="CB1113" s="147"/>
+      <c r="CC1113" s="147"/>
+      <c r="CD1113" s="147"/>
+      <c r="CE1113" s="147"/>
+      <c r="CF1113" s="147"/>
+      <c r="CG1113" s="147"/>
+      <c r="CH1113" s="147"/>
+      <c r="CI1113" s="147"/>
+      <c r="CJ1113" s="147"/>
+      <c r="CK1113" s="147"/>
+      <c r="CL1113" s="147"/>
+      <c r="CM1113" s="147"/>
+      <c r="CN1113" s="147"/>
+      <c r="CO1113" s="147"/>
+      <c r="CP1113" s="147"/>
+      <c r="CQ1113" s="147"/>
+      <c r="CR1113" s="147"/>
+      <c r="CS1113" s="147"/>
+      <c r="CT1113" s="147"/>
+      <c r="CU1113" s="147"/>
+      <c r="CV1113" s="147"/>
+      <c r="CW1113" s="147"/>
+      <c r="CX1113" s="147"/>
+      <c r="CY1113" s="147"/>
+      <c r="CZ1113" s="147"/>
+      <c r="DA1113" s="147"/>
+      <c r="DB1113" s="181"/>
+      <c r="DC1113" s="181"/>
+      <c r="DD1113" s="147"/>
+      <c r="DE1113" s="147"/>
+      <c r="DF1113" s="147"/>
+      <c r="DG1113" s="147"/>
+      <c r="DH1113" s="147"/>
+      <c r="DI1113" s="147"/>
+      <c r="DJ1113" s="147"/>
+      <c r="DK1113" s="147"/>
+      <c r="DL1113" s="147"/>
+      <c r="DM1113" s="147"/>
+      <c r="DN1113" s="147"/>
+      <c r="DO1113" s="147"/>
+    </row>
+    <row r="1114" spans="1:119" s="179" customFormat="1" ht="30">
+      <c r="A1114" s="178"/>
+      <c r="B1114" s="178"/>
+      <c r="C1114" s="178"/>
+      <c r="D1114" s="178" t="s">
+        <v>2174</v>
+      </c>
+      <c r="F1114" s="178" t="s">
+        <v>2163</v>
+      </c>
+      <c r="G1114" s="178" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1114" s="178"/>
+      <c r="I1114" s="178"/>
+      <c r="J1114" s="147"/>
+      <c r="K1114" s="147"/>
+      <c r="L1114" s="147"/>
+      <c r="M1114" s="147"/>
+      <c r="N1114" s="147"/>
+      <c r="O1114" s="147"/>
+      <c r="P1114" s="147"/>
+      <c r="Q1114" s="180"/>
+      <c r="R1114" s="147"/>
+      <c r="S1114" s="147"/>
+      <c r="T1114" s="147"/>
+      <c r="U1114" s="147"/>
+      <c r="V1114" s="147"/>
+      <c r="W1114" s="147"/>
+      <c r="X1114" s="147"/>
+      <c r="Y1114" s="147"/>
+      <c r="Z1114" s="147"/>
+      <c r="AA1114" s="147"/>
+      <c r="AB1114" s="147"/>
+      <c r="AC1114" s="147">
+        <v>1</v>
+      </c>
+      <c r="AD1114" s="147"/>
+      <c r="AE1114" s="147"/>
+      <c r="AF1114" s="147"/>
+      <c r="AG1114" s="147"/>
+      <c r="AH1114" s="147"/>
+      <c r="AI1114" s="147"/>
+      <c r="AJ1114" s="147"/>
+      <c r="AK1114" s="147"/>
+      <c r="AL1114" s="147"/>
+      <c r="AM1114" s="147"/>
+      <c r="AN1114" s="147"/>
+      <c r="AO1114" s="147"/>
+      <c r="AP1114" s="147"/>
+      <c r="AQ1114" s="147"/>
+      <c r="AR1114" s="147"/>
+      <c r="AS1114" s="147"/>
+      <c r="AT1114" s="147"/>
+      <c r="AU1114" s="147"/>
+      <c r="AV1114" s="147"/>
+      <c r="AW1114" s="147"/>
+      <c r="AX1114" s="147"/>
+      <c r="AY1114" s="147"/>
+      <c r="AZ1114" s="147"/>
+      <c r="BA1114" s="147"/>
+      <c r="BB1114" s="147"/>
+      <c r="BC1114" s="147"/>
+      <c r="BD1114" s="147"/>
+      <c r="BE1114" s="147"/>
+      <c r="BF1114" s="147"/>
+      <c r="BG1114" s="147"/>
+      <c r="BH1114" s="147"/>
+      <c r="BI1114" s="147"/>
+      <c r="BJ1114" s="147"/>
+      <c r="BK1114" s="147"/>
+      <c r="BL1114" s="147"/>
+      <c r="BM1114" s="147"/>
+      <c r="BN1114" s="147"/>
+      <c r="BO1114" s="147"/>
+      <c r="BP1114" s="147"/>
+      <c r="BQ1114" s="147"/>
+      <c r="BR1114" s="147"/>
+      <c r="BS1114" s="147"/>
+      <c r="BT1114" s="147"/>
+      <c r="BU1114" s="147"/>
+      <c r="BV1114" s="147"/>
+      <c r="BW1114" s="147"/>
+      <c r="BX1114" s="147"/>
+      <c r="BY1114" s="147"/>
+      <c r="BZ1114" s="147"/>
+      <c r="CA1114" s="147"/>
+      <c r="CB1114" s="147"/>
+      <c r="CC1114" s="147"/>
+      <c r="CD1114" s="147"/>
+      <c r="CE1114" s="147"/>
+      <c r="CF1114" s="147"/>
+      <c r="CG1114" s="147"/>
+      <c r="CH1114" s="147"/>
+      <c r="CI1114" s="147"/>
+      <c r="CJ1114" s="147"/>
+      <c r="CK1114" s="147"/>
+      <c r="CL1114" s="147"/>
+      <c r="CM1114" s="147"/>
+      <c r="CN1114" s="147"/>
+      <c r="CO1114" s="147"/>
+      <c r="CP1114" s="147"/>
+      <c r="CQ1114" s="147"/>
+      <c r="CR1114" s="147"/>
+      <c r="CS1114" s="147"/>
+      <c r="CT1114" s="147"/>
+      <c r="CU1114" s="147"/>
+      <c r="CV1114" s="147"/>
+      <c r="CW1114" s="147"/>
+      <c r="CX1114" s="147"/>
+      <c r="CY1114" s="147"/>
+      <c r="CZ1114" s="147"/>
+      <c r="DA1114" s="147"/>
+      <c r="DB1114" s="181"/>
+      <c r="DC1114" s="181"/>
+      <c r="DD1114" s="147"/>
+      <c r="DE1114" s="147"/>
+      <c r="DF1114" s="147"/>
+      <c r="DG1114" s="147"/>
+      <c r="DH1114" s="147"/>
+      <c r="DI1114" s="147"/>
+      <c r="DJ1114" s="147"/>
+      <c r="DK1114" s="147"/>
+      <c r="DL1114" s="147"/>
+      <c r="DM1114" s="147"/>
+      <c r="DN1114" s="147"/>
+      <c r="DO1114" s="147"/>
+    </row>
+    <row r="1115" spans="1:119" s="179" customFormat="1" ht="30">
+      <c r="A1115" s="178"/>
+      <c r="B1115" s="178"/>
+      <c r="C1115" s="178"/>
+      <c r="D1115" s="178" t="s">
+        <v>2175</v>
+      </c>
+      <c r="F1115" s="178" t="s">
+        <v>2163</v>
+      </c>
+      <c r="G1115" s="178" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1115" s="178"/>
+      <c r="I1115" s="178"/>
+      <c r="J1115" s="147"/>
+      <c r="K1115" s="147"/>
+      <c r="L1115" s="147"/>
+      <c r="M1115" s="147"/>
+      <c r="N1115" s="147"/>
+      <c r="O1115" s="147"/>
+      <c r="P1115" s="147"/>
+      <c r="Q1115" s="180"/>
+      <c r="R1115" s="147"/>
+      <c r="S1115" s="147"/>
+      <c r="T1115" s="147"/>
+      <c r="U1115" s="147"/>
+      <c r="V1115" s="147"/>
+      <c r="W1115" s="147"/>
+      <c r="X1115" s="147"/>
+      <c r="Y1115" s="147"/>
+      <c r="Z1115" s="147"/>
+      <c r="AA1115" s="147"/>
+      <c r="AB1115" s="147"/>
+      <c r="AC1115" s="147"/>
+      <c r="AD1115" s="147">
+        <v>1</v>
+      </c>
+      <c r="AE1115" s="147"/>
+      <c r="AF1115" s="147"/>
+      <c r="AG1115" s="147"/>
+      <c r="AH1115" s="147"/>
+      <c r="AI1115" s="147"/>
+      <c r="AJ1115" s="147"/>
+      <c r="AK1115" s="147"/>
+      <c r="AL1115" s="147"/>
+      <c r="AM1115" s="147"/>
+      <c r="AN1115" s="147"/>
+      <c r="AO1115" s="147"/>
+      <c r="AP1115" s="147"/>
+      <c r="AQ1115" s="147"/>
+      <c r="AR1115" s="147"/>
+      <c r="AS1115" s="147"/>
+      <c r="AT1115" s="147"/>
+      <c r="AU1115" s="147"/>
+      <c r="AV1115" s="147"/>
+      <c r="AW1115" s="147"/>
+      <c r="AX1115" s="147"/>
+      <c r="AY1115" s="147"/>
+      <c r="AZ1115" s="147"/>
+      <c r="BA1115" s="147"/>
+      <c r="BB1115" s="147"/>
+      <c r="BC1115" s="147"/>
+      <c r="BD1115" s="147"/>
+      <c r="BE1115" s="147"/>
+      <c r="BF1115" s="147"/>
+      <c r="BG1115" s="147"/>
+      <c r="BH1115" s="147"/>
+      <c r="BI1115" s="147"/>
+      <c r="BJ1115" s="147"/>
+      <c r="BK1115" s="147"/>
+      <c r="BL1115" s="147"/>
+      <c r="BM1115" s="147"/>
+      <c r="BN1115" s="147"/>
+      <c r="BO1115" s="147"/>
+      <c r="BP1115" s="147"/>
+      <c r="BQ1115" s="147"/>
+      <c r="BR1115" s="147"/>
+      <c r="BS1115" s="147"/>
+      <c r="BT1115" s="147"/>
+      <c r="BU1115" s="147"/>
+      <c r="BV1115" s="147"/>
+      <c r="BW1115" s="147"/>
+      <c r="BX1115" s="147"/>
+      <c r="BY1115" s="147"/>
+      <c r="BZ1115" s="147"/>
+      <c r="CA1115" s="147"/>
+      <c r="CB1115" s="147"/>
+      <c r="CC1115" s="147"/>
+      <c r="CD1115" s="147"/>
+      <c r="CE1115" s="147"/>
+      <c r="CF1115" s="147"/>
+      <c r="CG1115" s="147"/>
+      <c r="CH1115" s="147"/>
+      <c r="CI1115" s="147"/>
+      <c r="CJ1115" s="147"/>
+      <c r="CK1115" s="147"/>
+      <c r="CL1115" s="147"/>
+      <c r="CM1115" s="147"/>
+      <c r="CN1115" s="147"/>
+      <c r="CO1115" s="147"/>
+      <c r="CP1115" s="147"/>
+      <c r="CQ1115" s="147"/>
+      <c r="CR1115" s="147"/>
+      <c r="CS1115" s="147"/>
+      <c r="CT1115" s="147"/>
+      <c r="CU1115" s="147"/>
+      <c r="CV1115" s="147"/>
+      <c r="CW1115" s="147"/>
+      <c r="CX1115" s="147"/>
+      <c r="CY1115" s="147"/>
+      <c r="CZ1115" s="147"/>
+      <c r="DA1115" s="147"/>
+      <c r="DB1115" s="181"/>
+      <c r="DC1115" s="181"/>
+      <c r="DD1115" s="147"/>
+      <c r="DE1115" s="147"/>
+      <c r="DF1115" s="147"/>
+      <c r="DG1115" s="147"/>
+      <c r="DH1115" s="147"/>
+      <c r="DI1115" s="147"/>
+      <c r="DJ1115" s="147"/>
+      <c r="DK1115" s="147"/>
+      <c r="DL1115" s="147"/>
+      <c r="DM1115" s="147"/>
+      <c r="DN1115" s="147"/>
+      <c r="DO1115" s="147"/>
+    </row>
+    <row r="1116" spans="1:119" s="179" customFormat="1" ht="30">
+      <c r="A1116" s="178"/>
+      <c r="B1116" s="178"/>
+      <c r="C1116" s="178"/>
+      <c r="D1116" s="178" t="s">
+        <v>2176</v>
+      </c>
+      <c r="F1116" s="178" t="s">
+        <v>2163</v>
+      </c>
+      <c r="G1116" s="178" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1116" s="178"/>
+      <c r="I1116" s="178"/>
+      <c r="J1116" s="147"/>
+      <c r="K1116" s="147"/>
+      <c r="L1116" s="147"/>
+      <c r="M1116" s="147"/>
+      <c r="N1116" s="147"/>
+      <c r="O1116" s="147"/>
+      <c r="P1116" s="147"/>
+      <c r="Q1116" s="180"/>
+      <c r="R1116" s="147"/>
+      <c r="S1116" s="147"/>
+      <c r="T1116" s="147"/>
+      <c r="U1116" s="147"/>
+      <c r="V1116" s="147"/>
+      <c r="W1116" s="147"/>
+      <c r="X1116" s="147"/>
+      <c r="Y1116" s="147"/>
+      <c r="Z1116" s="147"/>
+      <c r="AA1116" s="147"/>
+      <c r="AB1116" s="147"/>
+      <c r="AC1116" s="147"/>
+      <c r="AD1116" s="147"/>
+      <c r="AE1116" s="147">
+        <v>1</v>
+      </c>
+      <c r="AF1116" s="147"/>
+      <c r="AG1116" s="147"/>
+      <c r="AH1116" s="147"/>
+      <c r="AI1116" s="147"/>
+      <c r="AJ1116" s="147"/>
+      <c r="AK1116" s="147"/>
+      <c r="AL1116" s="147"/>
+      <c r="AM1116" s="147"/>
+      <c r="AN1116" s="147"/>
+      <c r="AO1116" s="147"/>
+      <c r="AP1116" s="147"/>
+      <c r="AQ1116" s="147"/>
+      <c r="AR1116" s="147"/>
+      <c r="AS1116" s="147"/>
+      <c r="AT1116" s="147"/>
+      <c r="AU1116" s="147"/>
+      <c r="AV1116" s="147"/>
+      <c r="AW1116" s="147"/>
+      <c r="AX1116" s="147"/>
+      <c r="AY1116" s="147"/>
+      <c r="AZ1116" s="147"/>
+      <c r="BA1116" s="147"/>
+      <c r="BB1116" s="147"/>
+      <c r="BC1116" s="147"/>
+      <c r="BD1116" s="147"/>
+      <c r="BE1116" s="147"/>
+      <c r="BF1116" s="147"/>
+      <c r="BG1116" s="147"/>
+      <c r="BH1116" s="147"/>
+      <c r="BI1116" s="147"/>
+      <c r="BJ1116" s="147"/>
+      <c r="BK1116" s="147"/>
+      <c r="BL1116" s="147"/>
+      <c r="BM1116" s="147"/>
+      <c r="BN1116" s="147"/>
+      <c r="BO1116" s="147"/>
+      <c r="BP1116" s="147"/>
+      <c r="BQ1116" s="147"/>
+      <c r="BR1116" s="147"/>
+      <c r="BS1116" s="147"/>
+      <c r="BT1116" s="147"/>
+      <c r="BU1116" s="147"/>
+      <c r="BV1116" s="147"/>
+      <c r="BW1116" s="147"/>
+      <c r="BX1116" s="147"/>
+      <c r="BY1116" s="147"/>
+      <c r="BZ1116" s="147"/>
+      <c r="CA1116" s="147"/>
+      <c r="CB1116" s="147"/>
+      <c r="CC1116" s="147"/>
+      <c r="CD1116" s="147"/>
+      <c r="CE1116" s="147"/>
+      <c r="CF1116" s="147"/>
+      <c r="CG1116" s="147"/>
+      <c r="CH1116" s="147"/>
+      <c r="CI1116" s="147"/>
+      <c r="CJ1116" s="147"/>
+      <c r="CK1116" s="147"/>
+      <c r="CL1116" s="147"/>
+      <c r="CM1116" s="147"/>
+      <c r="CN1116" s="147"/>
+      <c r="CO1116" s="147"/>
+      <c r="CP1116" s="147"/>
+      <c r="CQ1116" s="147"/>
+      <c r="CR1116" s="147"/>
+      <c r="CS1116" s="147"/>
+      <c r="CT1116" s="147"/>
+      <c r="CU1116" s="147"/>
+      <c r="CV1116" s="147"/>
+      <c r="CW1116" s="147"/>
+      <c r="CX1116" s="147"/>
+      <c r="CY1116" s="147"/>
+      <c r="CZ1116" s="147"/>
+      <c r="DA1116" s="147"/>
+      <c r="DB1116" s="181"/>
+      <c r="DC1116" s="181"/>
+      <c r="DD1116" s="147"/>
+      <c r="DE1116" s="147"/>
+      <c r="DF1116" s="147"/>
+      <c r="DG1116" s="147"/>
+      <c r="DH1116" s="147"/>
+      <c r="DI1116" s="147"/>
+      <c r="DJ1116" s="147"/>
+      <c r="DK1116" s="147"/>
+      <c r="DL1116" s="147"/>
+      <c r="DM1116" s="147"/>
+      <c r="DN1116" s="147"/>
+      <c r="DO1116" s="147"/>
+    </row>
+    <row r="1117" spans="1:119" s="179" customFormat="1" ht="30">
+      <c r="A1117" s="178"/>
+      <c r="B1117" s="178"/>
+      <c r="C1117" s="178"/>
+      <c r="D1117" s="178" t="s">
+        <v>2177</v>
+      </c>
+      <c r="F1117" s="178" t="s">
+        <v>2163</v>
+      </c>
+      <c r="G1117" s="178" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1117" s="178"/>
+      <c r="I1117" s="178"/>
+      <c r="J1117" s="147"/>
+      <c r="K1117" s="147"/>
+      <c r="L1117" s="147"/>
+      <c r="M1117" s="147"/>
+      <c r="N1117" s="147"/>
+      <c r="O1117" s="147"/>
+      <c r="P1117" s="147"/>
+      <c r="Q1117" s="180"/>
+      <c r="R1117" s="147"/>
+      <c r="S1117" s="147"/>
+      <c r="T1117" s="147"/>
+      <c r="U1117" s="147"/>
+      <c r="V1117" s="147"/>
+      <c r="W1117" s="147"/>
+      <c r="X1117" s="147"/>
+      <c r="Y1117" s="147"/>
+      <c r="Z1117" s="147"/>
+      <c r="AA1117" s="147"/>
+      <c r="AB1117" s="147"/>
+      <c r="AC1117" s="147"/>
+      <c r="AD1117" s="147"/>
+      <c r="AE1117" s="147"/>
+      <c r="AF1117" s="147">
+        <v>1</v>
+      </c>
+      <c r="AG1117" s="147"/>
+      <c r="AH1117" s="147"/>
+      <c r="AI1117" s="147"/>
+      <c r="AJ1117" s="147"/>
+      <c r="AK1117" s="147"/>
+      <c r="AL1117" s="147"/>
+      <c r="AM1117" s="147"/>
+      <c r="AN1117" s="147"/>
+      <c r="AO1117" s="147"/>
+      <c r="AP1117" s="147"/>
+      <c r="AQ1117" s="147"/>
+      <c r="AR1117" s="147"/>
+      <c r="AS1117" s="147"/>
+      <c r="AT1117" s="147"/>
+      <c r="AU1117" s="147"/>
+      <c r="AV1117" s="147"/>
+      <c r="AW1117" s="147"/>
+      <c r="AX1117" s="147"/>
+      <c r="AY1117" s="147"/>
+      <c r="AZ1117" s="147"/>
+      <c r="BA1117" s="147"/>
+      <c r="BB1117" s="147"/>
+      <c r="BC1117" s="147"/>
+      <c r="BD1117" s="147"/>
+      <c r="BE1117" s="147"/>
+      <c r="BF1117" s="147"/>
+      <c r="BG1117" s="147"/>
+      <c r="BH1117" s="147"/>
+      <c r="BI1117" s="147"/>
+      <c r="BJ1117" s="147"/>
+      <c r="BK1117" s="147"/>
+      <c r="BL1117" s="147"/>
+      <c r="BM1117" s="147"/>
+      <c r="BN1117" s="147"/>
+      <c r="BO1117" s="147"/>
+      <c r="BP1117" s="147"/>
+      <c r="BQ1117" s="147"/>
+      <c r="BR1117" s="147"/>
+      <c r="BS1117" s="147"/>
+      <c r="BT1117" s="147"/>
+      <c r="BU1117" s="147"/>
+      <c r="BV1117" s="147"/>
+      <c r="BW1117" s="147"/>
+      <c r="BX1117" s="147"/>
+      <c r="BY1117" s="147"/>
+      <c r="BZ1117" s="147"/>
+      <c r="CA1117" s="147"/>
+      <c r="CB1117" s="147"/>
+      <c r="CC1117" s="147"/>
+      <c r="CD1117" s="147"/>
+      <c r="CE1117" s="147"/>
+      <c r="CF1117" s="147"/>
+      <c r="CG1117" s="147"/>
+      <c r="CH1117" s="147"/>
+      <c r="CI1117" s="147"/>
+      <c r="CJ1117" s="147"/>
+      <c r="CK1117" s="147"/>
+      <c r="CL1117" s="147"/>
+      <c r="CM1117" s="147"/>
+      <c r="CN1117" s="147"/>
+      <c r="CO1117" s="147"/>
+      <c r="CP1117" s="147"/>
+      <c r="CQ1117" s="147"/>
+      <c r="CR1117" s="147"/>
+      <c r="CS1117" s="147"/>
+      <c r="CT1117" s="147"/>
+      <c r="CU1117" s="147"/>
+      <c r="CV1117" s="147"/>
+      <c r="CW1117" s="147"/>
+      <c r="CX1117" s="147"/>
+      <c r="CY1117" s="147"/>
+      <c r="CZ1117" s="147"/>
+      <c r="DA1117" s="147"/>
+      <c r="DB1117" s="181"/>
+      <c r="DC1117" s="181"/>
+      <c r="DD1117" s="147"/>
+      <c r="DE1117" s="147"/>
+      <c r="DF1117" s="147"/>
+      <c r="DG1117" s="147"/>
+      <c r="DH1117" s="147"/>
+      <c r="DI1117" s="147"/>
+      <c r="DJ1117" s="147"/>
+      <c r="DK1117" s="147"/>
+      <c r="DL1117" s="147"/>
+      <c r="DM1117" s="147"/>
+      <c r="DN1117" s="147"/>
+      <c r="DO1117" s="147"/>
+    </row>
+    <row r="1118" spans="1:119" s="179" customFormat="1" ht="30">
+      <c r="A1118" s="178"/>
+      <c r="B1118" s="178"/>
+      <c r="C1118" s="178"/>
+      <c r="D1118" s="178" t="s">
+        <v>2178</v>
+      </c>
+      <c r="F1118" s="178" t="s">
+        <v>2163</v>
+      </c>
+      <c r="G1118" s="178" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1118" s="178"/>
+      <c r="I1118" s="178"/>
+      <c r="J1118" s="147"/>
+      <c r="K1118" s="147"/>
+      <c r="L1118" s="147"/>
+      <c r="M1118" s="147"/>
+      <c r="N1118" s="147"/>
+      <c r="O1118" s="147"/>
+      <c r="P1118" s="147"/>
+      <c r="Q1118" s="180"/>
+      <c r="R1118" s="147"/>
+      <c r="S1118" s="147"/>
+      <c r="T1118" s="147"/>
+      <c r="U1118" s="147"/>
+      <c r="V1118" s="147"/>
+      <c r="W1118" s="147"/>
+      <c r="X1118" s="147"/>
+      <c r="Y1118" s="147"/>
+      <c r="Z1118" s="147"/>
+      <c r="AA1118" s="147"/>
+      <c r="AB1118" s="147"/>
+      <c r="AC1118" s="147"/>
+      <c r="AD1118" s="147"/>
+      <c r="AE1118" s="147"/>
+      <c r="AF1118" s="147"/>
+      <c r="AG1118" s="147">
+        <v>1</v>
+      </c>
+      <c r="AH1118" s="147"/>
+      <c r="AI1118" s="147"/>
+      <c r="AJ1118" s="147"/>
+      <c r="AK1118" s="147"/>
+      <c r="AL1118" s="147"/>
+      <c r="AM1118" s="147"/>
+      <c r="AN1118" s="147"/>
+      <c r="AO1118" s="147"/>
+      <c r="AP1118" s="147"/>
+      <c r="AQ1118" s="147"/>
+      <c r="AR1118" s="147"/>
+      <c r="AS1118" s="147"/>
+      <c r="AT1118" s="147"/>
+      <c r="AU1118" s="147"/>
+      <c r="AV1118" s="147"/>
+      <c r="AW1118" s="147"/>
+      <c r="AX1118" s="147"/>
+      <c r="AY1118" s="147"/>
+      <c r="AZ1118" s="147"/>
+      <c r="BA1118" s="147"/>
+      <c r="BB1118" s="147"/>
+      <c r="BC1118" s="147"/>
+      <c r="BD1118" s="147"/>
+      <c r="BE1118" s="147"/>
+      <c r="BF1118" s="147"/>
+      <c r="BG1118" s="147"/>
+      <c r="BH1118" s="147"/>
+      <c r="BI1118" s="147"/>
+      <c r="BJ1118" s="147"/>
+      <c r="BK1118" s="147"/>
+      <c r="BL1118" s="147"/>
+      <c r="BM1118" s="147"/>
+      <c r="BN1118" s="147"/>
+      <c r="BO1118" s="147"/>
+      <c r="BP1118" s="147"/>
+      <c r="BQ1118" s="147"/>
+      <c r="BR1118" s="147"/>
+      <c r="BS1118" s="147"/>
+      <c r="BT1118" s="147"/>
+      <c r="BU1118" s="147"/>
+      <c r="BV1118" s="147"/>
+      <c r="BW1118" s="147"/>
+      <c r="BX1118" s="147"/>
+      <c r="BY1118" s="147"/>
+      <c r="BZ1118" s="147"/>
+      <c r="CA1118" s="147"/>
+      <c r="CB1118" s="147"/>
+      <c r="CC1118" s="147"/>
+      <c r="CD1118" s="147"/>
+      <c r="CE1118" s="147"/>
+      <c r="CF1118" s="147"/>
+      <c r="CG1118" s="147"/>
+      <c r="CH1118" s="147"/>
+      <c r="CI1118" s="147"/>
+      <c r="CJ1118" s="147"/>
+      <c r="CK1118" s="147"/>
+      <c r="CL1118" s="147"/>
+      <c r="CM1118" s="147"/>
+      <c r="CN1118" s="147"/>
+      <c r="CO1118" s="147"/>
+      <c r="CP1118" s="147"/>
+      <c r="CQ1118" s="147"/>
+      <c r="CR1118" s="147"/>
+      <c r="CS1118" s="147"/>
+      <c r="CT1118" s="147"/>
+      <c r="CU1118" s="147"/>
+      <c r="CV1118" s="147"/>
+      <c r="CW1118" s="147"/>
+      <c r="CX1118" s="147"/>
+      <c r="CY1118" s="147"/>
+      <c r="CZ1118" s="147"/>
+      <c r="DA1118" s="147"/>
+      <c r="DB1118" s="181"/>
+      <c r="DC1118" s="181"/>
+      <c r="DD1118" s="147"/>
+      <c r="DE1118" s="147"/>
+      <c r="DF1118" s="147"/>
+      <c r="DG1118" s="147"/>
+      <c r="DH1118" s="147"/>
+      <c r="DI1118" s="147"/>
+      <c r="DJ1118" s="147"/>
+      <c r="DK1118" s="147"/>
+      <c r="DL1118" s="147"/>
+      <c r="DM1118" s="147"/>
+      <c r="DN1118" s="147"/>
+      <c r="DO1118" s="147"/>
+    </row>
+    <row r="1119" spans="1:119" s="179" customFormat="1" ht="30">
+      <c r="A1119" s="178"/>
+      <c r="B1119" s="178"/>
+      <c r="C1119" s="178"/>
+      <c r="D1119" s="178" t="s">
+        <v>2179</v>
+      </c>
+      <c r="F1119" s="178" t="s">
+        <v>2163</v>
+      </c>
+      <c r="G1119" s="178" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1119" s="178"/>
+      <c r="I1119" s="178"/>
+      <c r="J1119" s="147"/>
+      <c r="K1119" s="147"/>
+      <c r="L1119" s="147"/>
+      <c r="M1119" s="147"/>
+      <c r="N1119" s="147"/>
+      <c r="O1119" s="147"/>
+      <c r="P1119" s="147"/>
+      <c r="Q1119" s="180"/>
+      <c r="R1119" s="147"/>
+      <c r="S1119" s="147"/>
+      <c r="T1119" s="147"/>
+      <c r="U1119" s="147"/>
+      <c r="V1119" s="147"/>
+      <c r="W1119" s="147"/>
+      <c r="X1119" s="147"/>
+      <c r="Y1119" s="147"/>
+      <c r="Z1119" s="147"/>
+      <c r="AA1119" s="147"/>
+      <c r="AB1119" s="147"/>
+      <c r="AC1119" s="147"/>
+      <c r="AD1119" s="147"/>
+      <c r="AE1119" s="147"/>
+      <c r="AF1119" s="147"/>
+      <c r="AG1119" s="147"/>
+      <c r="AH1119" s="147">
+        <v>1</v>
+      </c>
+      <c r="AI1119" s="147"/>
+      <c r="AJ1119" s="147"/>
+      <c r="AK1119" s="147"/>
+      <c r="AL1119" s="147"/>
+      <c r="AM1119" s="147"/>
+      <c r="AN1119" s="147"/>
+      <c r="AO1119" s="147"/>
+      <c r="AP1119" s="147"/>
+      <c r="AQ1119" s="147"/>
+      <c r="AR1119" s="147"/>
+      <c r="AS1119" s="147"/>
+      <c r="AT1119" s="147"/>
+      <c r="AU1119" s="147"/>
+      <c r="AV1119" s="147"/>
+      <c r="AW1119" s="147"/>
+      <c r="AX1119" s="147"/>
+      <c r="AY1119" s="147"/>
+      <c r="AZ1119" s="147"/>
+      <c r="BA1119" s="147"/>
+      <c r="BB1119" s="147"/>
+      <c r="BC1119" s="147"/>
+      <c r="BD1119" s="147"/>
+      <c r="BE1119" s="147"/>
+      <c r="BF1119" s="147"/>
+      <c r="BG1119" s="147"/>
+      <c r="BH1119" s="147"/>
+      <c r="BI1119" s="147"/>
+      <c r="BJ1119" s="147"/>
+      <c r="BK1119" s="147"/>
+      <c r="BL1119" s="147"/>
+      <c r="BM1119" s="147"/>
+      <c r="BN1119" s="147"/>
+      <c r="BO1119" s="147"/>
+      <c r="BP1119" s="147"/>
+      <c r="BQ1119" s="147"/>
+      <c r="BR1119" s="147"/>
+      <c r="BS1119" s="147"/>
+      <c r="BT1119" s="147"/>
+      <c r="BU1119" s="147"/>
+      <c r="BV1119" s="147"/>
+      <c r="BW1119" s="147"/>
+      <c r="BX1119" s="147"/>
+      <c r="BY1119" s="147"/>
+      <c r="BZ1119" s="147"/>
+      <c r="CA1119" s="147"/>
+      <c r="CB1119" s="147"/>
+      <c r="CC1119" s="147"/>
+      <c r="CD1119" s="147"/>
+      <c r="CE1119" s="147"/>
+      <c r="CF1119" s="147"/>
+      <c r="CG1119" s="147"/>
+      <c r="CH1119" s="147"/>
+      <c r="CI1119" s="147"/>
+      <c r="CJ1119" s="147"/>
+      <c r="CK1119" s="147"/>
+      <c r="CL1119" s="147"/>
+      <c r="CM1119" s="147"/>
+      <c r="CN1119" s="147"/>
+      <c r="CO1119" s="147"/>
+      <c r="CP1119" s="147"/>
+      <c r="CQ1119" s="147"/>
+      <c r="CR1119" s="147"/>
+      <c r="CS1119" s="147"/>
+      <c r="CT1119" s="147"/>
+      <c r="CU1119" s="147"/>
+      <c r="CV1119" s="147"/>
+      <c r="CW1119" s="147"/>
+      <c r="CX1119" s="147"/>
+      <c r="CY1119" s="147"/>
+      <c r="CZ1119" s="147"/>
+      <c r="DA1119" s="147"/>
+      <c r="DB1119" s="181"/>
+      <c r="DC1119" s="181"/>
+      <c r="DD1119" s="147"/>
+      <c r="DE1119" s="147"/>
+      <c r="DF1119" s="147"/>
+      <c r="DG1119" s="147"/>
+      <c r="DH1119" s="147"/>
+      <c r="DI1119" s="147"/>
+      <c r="DJ1119" s="147"/>
+      <c r="DK1119" s="147"/>
+      <c r="DL1119" s="147"/>
+      <c r="DM1119" s="147"/>
+      <c r="DN1119" s="147"/>
+      <c r="DO1119" s="147"/>
+    </row>
+    <row r="1120" spans="1:119" s="179" customFormat="1" ht="30">
+      <c r="A1120" s="178"/>
+      <c r="B1120" s="178"/>
+      <c r="C1120" s="178"/>
+      <c r="D1120" s="178" t="s">
+        <v>2180</v>
+      </c>
+      <c r="F1120" s="178" t="s">
+        <v>2163</v>
+      </c>
+      <c r="G1120" s="178" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1120" s="178"/>
+      <c r="I1120" s="178"/>
+      <c r="J1120" s="147"/>
+      <c r="K1120" s="147"/>
+      <c r="L1120" s="147"/>
+      <c r="M1120" s="147"/>
+      <c r="N1120" s="147"/>
+      <c r="O1120" s="147"/>
+      <c r="P1120" s="147"/>
+      <c r="Q1120" s="180"/>
+      <c r="R1120" s="147"/>
+      <c r="S1120" s="147"/>
+      <c r="T1120" s="147"/>
+      <c r="U1120" s="147"/>
+      <c r="V1120" s="147"/>
+      <c r="W1120" s="147"/>
+      <c r="X1120" s="147"/>
+      <c r="Y1120" s="147"/>
+      <c r="Z1120" s="147"/>
+      <c r="AA1120" s="147"/>
+      <c r="AB1120" s="147"/>
+      <c r="AC1120" s="147"/>
+      <c r="AD1120" s="147"/>
+      <c r="AE1120" s="147"/>
+      <c r="AF1120" s="147"/>
+      <c r="AG1120" s="147"/>
+      <c r="AH1120" s="147"/>
+      <c r="AI1120" s="147">
+        <v>1</v>
+      </c>
+      <c r="AJ1120" s="147"/>
+      <c r="AK1120" s="147"/>
+      <c r="AL1120" s="147"/>
+      <c r="AM1120" s="147"/>
+      <c r="AN1120" s="147"/>
+      <c r="AO1120" s="147"/>
+      <c r="AP1120" s="147"/>
+      <c r="AQ1120" s="147"/>
+      <c r="AR1120" s="147"/>
+      <c r="AS1120" s="147"/>
+      <c r="AT1120" s="147"/>
+      <c r="AU1120" s="147"/>
+      <c r="AV1120" s="147"/>
+      <c r="AW1120" s="147"/>
+      <c r="AX1120" s="147"/>
+      <c r="AY1120" s="147"/>
+      <c r="AZ1120" s="147"/>
+      <c r="BA1120" s="147"/>
+      <c r="BB1120" s="147"/>
+      <c r="BC1120" s="147"/>
+      <c r="BD1120" s="147"/>
+      <c r="BE1120" s="147"/>
+      <c r="BF1120" s="147"/>
+      <c r="BG1120" s="147"/>
+      <c r="BH1120" s="147"/>
+      <c r="BI1120" s="147"/>
+      <c r="BJ1120" s="147"/>
+      <c r="BK1120" s="147"/>
+      <c r="BL1120" s="147"/>
+      <c r="BM1120" s="147"/>
+      <c r="BN1120" s="147"/>
+      <c r="BO1120" s="147"/>
+      <c r="BP1120" s="147"/>
+      <c r="BQ1120" s="147"/>
+      <c r="BR1120" s="147"/>
+      <c r="BS1120" s="147"/>
+      <c r="BT1120" s="147"/>
+      <c r="BU1120" s="147"/>
+      <c r="BV1120" s="147"/>
+      <c r="BW1120" s="147"/>
+      <c r="BX1120" s="147"/>
+      <c r="BY1120" s="147"/>
+      <c r="BZ1120" s="147"/>
+      <c r="CA1120" s="147"/>
+      <c r="CB1120" s="147"/>
+      <c r="CC1120" s="147"/>
+      <c r="CD1120" s="147"/>
+      <c r="CE1120" s="147"/>
+      <c r="CF1120" s="147"/>
+      <c r="CG1120" s="147"/>
+      <c r="CH1120" s="147"/>
+      <c r="CI1120" s="147"/>
+      <c r="CJ1120" s="147"/>
+      <c r="CK1120" s="147"/>
+      <c r="CL1120" s="147"/>
+      <c r="CM1120" s="147"/>
+      <c r="CN1120" s="147"/>
+      <c r="CO1120" s="147"/>
+      <c r="CP1120" s="147"/>
+      <c r="CQ1120" s="147"/>
+      <c r="CR1120" s="147"/>
+      <c r="CS1120" s="147"/>
+      <c r="CT1120" s="147"/>
+      <c r="CU1120" s="147"/>
+      <c r="CV1120" s="147"/>
+      <c r="CW1120" s="147"/>
+      <c r="CX1120" s="147"/>
+      <c r="CY1120" s="147"/>
+      <c r="CZ1120" s="147"/>
+      <c r="DA1120" s="147"/>
+      <c r="DB1120" s="181"/>
+      <c r="DC1120" s="181"/>
+      <c r="DD1120" s="147"/>
+      <c r="DE1120" s="147"/>
+      <c r="DF1120" s="147"/>
+      <c r="DG1120" s="147"/>
+      <c r="DH1120" s="147"/>
+      <c r="DI1120" s="147"/>
+      <c r="DJ1120" s="147"/>
+      <c r="DK1120" s="147"/>
+      <c r="DL1120" s="147"/>
+      <c r="DM1120" s="147"/>
+      <c r="DN1120" s="147"/>
+      <c r="DO1120" s="147"/>
+    </row>
+    <row r="1121" spans="1:119" s="179" customFormat="1" ht="30">
+      <c r="A1121" s="178"/>
+      <c r="B1121" s="178"/>
+      <c r="C1121" s="178"/>
+      <c r="D1121" s="178" t="s">
+        <v>2181</v>
+      </c>
+      <c r="F1121" s="178" t="s">
+        <v>2163</v>
+      </c>
+      <c r="G1121" s="178" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1121" s="178"/>
+      <c r="I1121" s="178"/>
+      <c r="J1121" s="147"/>
+      <c r="K1121" s="147"/>
+      <c r="L1121" s="147"/>
+      <c r="M1121" s="147"/>
+      <c r="N1121" s="147"/>
+      <c r="O1121" s="147"/>
+      <c r="P1121" s="147"/>
+      <c r="Q1121" s="180"/>
+      <c r="R1121" s="147"/>
+      <c r="S1121" s="147"/>
+      <c r="T1121" s="147"/>
+      <c r="U1121" s="147"/>
+      <c r="V1121" s="147"/>
+      <c r="W1121" s="147"/>
+      <c r="X1121" s="147"/>
+      <c r="Y1121" s="147"/>
+      <c r="Z1121" s="147"/>
+      <c r="AA1121" s="147"/>
+      <c r="AB1121" s="147"/>
+      <c r="AC1121" s="147"/>
+      <c r="AD1121" s="147"/>
+      <c r="AE1121" s="147"/>
+      <c r="AF1121" s="147"/>
+      <c r="AG1121" s="147"/>
+      <c r="AH1121" s="147"/>
+      <c r="AI1121" s="147"/>
+      <c r="AJ1121" s="147">
+        <v>1</v>
+      </c>
+      <c r="AK1121" s="147"/>
+      <c r="AL1121" s="147"/>
+      <c r="AM1121" s="147"/>
+      <c r="AN1121" s="147"/>
+      <c r="AO1121" s="147"/>
+      <c r="AP1121" s="147"/>
+      <c r="AQ1121" s="147"/>
+      <c r="AR1121" s="147"/>
+      <c r="AS1121" s="147"/>
+      <c r="AT1121" s="147"/>
+      <c r="AU1121" s="147"/>
+      <c r="AV1121" s="147"/>
+      <c r="AW1121" s="147"/>
+      <c r="AX1121" s="147"/>
+      <c r="AY1121" s="147"/>
+      <c r="AZ1121" s="147"/>
+      <c r="BA1121" s="147"/>
+      <c r="BB1121" s="147"/>
+      <c r="BC1121" s="147"/>
+      <c r="BD1121" s="147"/>
+      <c r="BE1121" s="147"/>
+      <c r="BF1121" s="147"/>
+      <c r="BG1121" s="147"/>
+      <c r="BH1121" s="147"/>
+      <c r="BI1121" s="147"/>
+      <c r="BJ1121" s="147"/>
+      <c r="BK1121" s="147"/>
+      <c r="BL1121" s="147"/>
+      <c r="BM1121" s="147"/>
+      <c r="BN1121" s="147"/>
+      <c r="BO1121" s="147"/>
+      <c r="BP1121" s="147"/>
+      <c r="BQ1121" s="147"/>
+      <c r="BR1121" s="147"/>
+      <c r="BS1121" s="147"/>
+      <c r="BT1121" s="147"/>
+      <c r="BU1121" s="147"/>
+      <c r="BV1121" s="147"/>
+      <c r="BW1121" s="147"/>
+      <c r="BX1121" s="147"/>
+      <c r="BY1121" s="147"/>
+      <c r="BZ1121" s="147"/>
+      <c r="CA1121" s="147"/>
+      <c r="CB1121" s="147"/>
+      <c r="CC1121" s="147"/>
+      <c r="CD1121" s="147"/>
+      <c r="CE1121" s="147"/>
+      <c r="CF1121" s="147"/>
+      <c r="CG1121" s="147"/>
+      <c r="CH1121" s="147"/>
+      <c r="CI1121" s="147"/>
+      <c r="CJ1121" s="147"/>
+      <c r="CK1121" s="147"/>
+      <c r="CL1121" s="147"/>
+      <c r="CM1121" s="147"/>
+      <c r="CN1121" s="147"/>
+      <c r="CO1121" s="147"/>
+      <c r="CP1121" s="147"/>
+      <c r="CQ1121" s="147"/>
+      <c r="CR1121" s="147"/>
+      <c r="CS1121" s="147"/>
+      <c r="CT1121" s="147"/>
+      <c r="CU1121" s="147"/>
+      <c r="CV1121" s="147"/>
+      <c r="CW1121" s="147"/>
+      <c r="CX1121" s="147"/>
+      <c r="CY1121" s="147"/>
+      <c r="CZ1121" s="147"/>
+      <c r="DA1121" s="147"/>
+      <c r="DB1121" s="181"/>
+      <c r="DC1121" s="181"/>
+      <c r="DD1121" s="147"/>
+      <c r="DE1121" s="147"/>
+      <c r="DF1121" s="147"/>
+      <c r="DG1121" s="147"/>
+      <c r="DH1121" s="147"/>
+      <c r="DI1121" s="147"/>
+      <c r="DJ1121" s="147"/>
+      <c r="DK1121" s="147"/>
+      <c r="DL1121" s="147"/>
+      <c r="DM1121" s="147"/>
+      <c r="DN1121" s="147"/>
+      <c r="DO1121" s="147"/>
+    </row>
+    <row r="1122" spans="1:119" s="179" customFormat="1" ht="30">
+      <c r="A1122" s="178"/>
+      <c r="B1122" s="178"/>
+      <c r="C1122" s="178"/>
+      <c r="D1122" s="178" t="s">
+        <v>2182</v>
+      </c>
+      <c r="F1122" s="178" t="s">
+        <v>2163</v>
+      </c>
+      <c r="G1122" s="178" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1122" s="178"/>
+      <c r="I1122" s="178"/>
+      <c r="J1122" s="147"/>
+      <c r="K1122" s="147"/>
+      <c r="L1122" s="147"/>
+      <c r="M1122" s="147"/>
+      <c r="N1122" s="147"/>
+      <c r="O1122" s="147"/>
+      <c r="P1122" s="147"/>
+      <c r="Q1122" s="180"/>
+      <c r="R1122" s="147"/>
+      <c r="S1122" s="147"/>
+      <c r="T1122" s="147"/>
+      <c r="U1122" s="147"/>
+      <c r="V1122" s="147"/>
+      <c r="W1122" s="147"/>
+      <c r="X1122" s="147"/>
+      <c r="Y1122" s="147"/>
+      <c r="Z1122" s="147"/>
+      <c r="AA1122" s="147"/>
+      <c r="AB1122" s="147"/>
+      <c r="AC1122" s="147"/>
+      <c r="AD1122" s="147"/>
+      <c r="AE1122" s="147"/>
+      <c r="AF1122" s="147"/>
+      <c r="AG1122" s="147"/>
+      <c r="AH1122" s="147"/>
+      <c r="AI1122" s="147"/>
+      <c r="AJ1122" s="147"/>
+      <c r="AK1122" s="147">
+        <v>1</v>
+      </c>
+      <c r="AL1122" s="147"/>
+      <c r="AM1122" s="147"/>
+      <c r="AN1122" s="147"/>
+      <c r="AO1122" s="147"/>
+      <c r="AP1122" s="147"/>
+      <c r="AQ1122" s="147"/>
+      <c r="AR1122" s="147"/>
+      <c r="AS1122" s="147"/>
+      <c r="AT1122" s="147"/>
+      <c r="AU1122" s="147"/>
+      <c r="AV1122" s="147"/>
+      <c r="AW1122" s="147"/>
+      <c r="AX1122" s="147"/>
+      <c r="AY1122" s="147"/>
+      <c r="AZ1122" s="147"/>
+      <c r="BA1122" s="147"/>
+      <c r="BB1122" s="147"/>
+      <c r="BC1122" s="147"/>
+      <c r="BD1122" s="147"/>
+      <c r="BE1122" s="147"/>
+      <c r="BF1122" s="147"/>
+      <c r="BG1122" s="147"/>
+      <c r="BH1122" s="147"/>
+      <c r="BI1122" s="147"/>
+      <c r="BJ1122" s="147"/>
+      <c r="BK1122" s="147"/>
+      <c r="BL1122" s="147"/>
+      <c r="BM1122" s="147"/>
+      <c r="BN1122" s="147"/>
+      <c r="BO1122" s="147"/>
+      <c r="BP1122" s="147"/>
+      <c r="BQ1122" s="147"/>
+      <c r="BR1122" s="147"/>
+      <c r="BS1122" s="147"/>
+      <c r="BT1122" s="147"/>
+      <c r="BU1122" s="147"/>
+      <c r="BV1122" s="147"/>
+      <c r="BW1122" s="147"/>
+      <c r="BX1122" s="147"/>
+      <c r="BY1122" s="147"/>
+      <c r="BZ1122" s="147"/>
+      <c r="CA1122" s="147"/>
+      <c r="CB1122" s="147"/>
+      <c r="CC1122" s="147"/>
+      <c r="CD1122" s="147"/>
+      <c r="CE1122" s="147"/>
+      <c r="CF1122" s="147"/>
+      <c r="CG1122" s="147"/>
+      <c r="CH1122" s="147"/>
+      <c r="CI1122" s="147"/>
+      <c r="CJ1122" s="147"/>
+      <c r="CK1122" s="147"/>
+      <c r="CL1122" s="147"/>
+      <c r="CM1122" s="147"/>
+      <c r="CN1122" s="147"/>
+      <c r="CO1122" s="147"/>
+      <c r="CP1122" s="147"/>
+      <c r="CQ1122" s="147"/>
+      <c r="CR1122" s="147"/>
+      <c r="CS1122" s="147"/>
+      <c r="CT1122" s="147"/>
+      <c r="CU1122" s="147"/>
+      <c r="CV1122" s="147"/>
+      <c r="CW1122" s="147"/>
+      <c r="CX1122" s="147"/>
+      <c r="CY1122" s="147"/>
+      <c r="CZ1122" s="147"/>
+      <c r="DA1122" s="147"/>
+      <c r="DB1122" s="181"/>
+      <c r="DC1122" s="181"/>
+      <c r="DD1122" s="147"/>
+      <c r="DE1122" s="147"/>
+      <c r="DF1122" s="147"/>
+      <c r="DG1122" s="147"/>
+      <c r="DH1122" s="147"/>
+      <c r="DI1122" s="147"/>
+      <c r="DJ1122" s="147"/>
+      <c r="DK1122" s="147"/>
+      <c r="DL1122" s="147"/>
+      <c r="DM1122" s="147"/>
+      <c r="DN1122" s="147"/>
+      <c r="DO1122" s="147"/>
+    </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="D1:E1"/>

</xml_diff>

<commit_message>
custom mappings calibration visualisation
</commit_message>
<xml_diff>
--- a/resources/syst_review_single_table.xlsx
+++ b/resources/syst_review_single_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\AnacondaProjects\PhD\Semiology-Visualisation-Tool\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9AAB72B-6C8D-4970-BF90-3AAB4147BC4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D6201C-A03E-46EC-9A69-C1AEED2D8470}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7053" uniqueCount="2183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7077" uniqueCount="2185">
   <si>
     <t xml:space="preserve">Semiology </t>
   </si>
@@ -6823,6 +6823,12 @@
   </si>
   <si>
     <t>_mapiings_TL19</t>
+  </si>
+  <si>
+    <t>awesome</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
@@ -7855,6 +7861,21 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -7896,21 +7917,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -10504,10 +10510,10 @@
   <dimension ref="A1:DU1122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E1097" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="CX1100" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D1103" sqref="D1103"/>
+      <selection pane="bottomRight" activeCell="CY1119" sqref="CY1119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -10599,106 +10605,106 @@
     <row r="1" spans="1:125" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="155"/>
       <c r="C1" s="17"/>
-      <c r="D1" s="164" t="s">
+      <c r="D1" s="169" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="164"/>
-      <c r="G1" s="172" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="173"/>
-      <c r="I1" s="173"/>
-      <c r="K1" s="174" t="s">
+      <c r="E1" s="169"/>
+      <c r="G1" s="177" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="178"/>
+      <c r="I1" s="178"/>
+      <c r="K1" s="179" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="175"/>
-      <c r="M1" s="175"/>
-      <c r="N1" s="175"/>
-      <c r="O1" s="176"/>
-      <c r="S1" s="165"/>
-      <c r="T1" s="165"/>
-      <c r="U1" s="165"/>
-      <c r="V1" s="165"/>
-      <c r="W1" s="165"/>
-      <c r="X1" s="165"/>
-      <c r="Y1" s="165"/>
-      <c r="Z1" s="165"/>
-      <c r="AA1" s="165"/>
-      <c r="AB1" s="165"/>
-      <c r="AC1" s="165"/>
-      <c r="AD1" s="165"/>
-      <c r="AE1" s="165"/>
-      <c r="AF1" s="165"/>
-      <c r="AG1" s="165"/>
-      <c r="AH1" s="165"/>
-      <c r="AI1" s="165"/>
-      <c r="AJ1" s="165"/>
-      <c r="AK1" s="165"/>
+      <c r="L1" s="180"/>
+      <c r="M1" s="180"/>
+      <c r="N1" s="180"/>
+      <c r="O1" s="181"/>
+      <c r="S1" s="170"/>
+      <c r="T1" s="170"/>
+      <c r="U1" s="170"/>
+      <c r="V1" s="170"/>
+      <c r="W1" s="170"/>
+      <c r="X1" s="170"/>
+      <c r="Y1" s="170"/>
+      <c r="Z1" s="170"/>
+      <c r="AA1" s="170"/>
+      <c r="AB1" s="170"/>
+      <c r="AC1" s="170"/>
+      <c r="AD1" s="170"/>
+      <c r="AE1" s="170"/>
+      <c r="AF1" s="170"/>
+      <c r="AG1" s="170"/>
+      <c r="AH1" s="170"/>
+      <c r="AI1" s="170"/>
+      <c r="AJ1" s="170"/>
+      <c r="AK1" s="170"/>
       <c r="AM1" s="153"/>
-      <c r="AN1" s="166" t="s">
+      <c r="AN1" s="171" t="s">
         <v>3</v>
       </c>
-      <c r="AO1" s="165"/>
-      <c r="AP1" s="165"/>
-      <c r="AQ1" s="165"/>
-      <c r="AR1" s="165"/>
-      <c r="AS1" s="165"/>
-      <c r="AT1" s="165"/>
-      <c r="AU1" s="165"/>
-      <c r="AV1" s="165"/>
-      <c r="AW1" s="165"/>
-      <c r="AX1" s="165"/>
-      <c r="AY1" s="165"/>
-      <c r="AZ1" s="165"/>
-      <c r="BA1" s="165"/>
-      <c r="BB1" s="165"/>
-      <c r="BC1" s="165"/>
-      <c r="BD1" s="165"/>
-      <c r="BE1" s="165"/>
-      <c r="BF1" s="165"/>
-      <c r="BG1" s="165"/>
-      <c r="BH1" s="165"/>
-      <c r="BI1" s="165"/>
-      <c r="BJ1" s="165"/>
-      <c r="BK1" s="165"/>
-      <c r="BL1" s="165"/>
-      <c r="BM1" s="165"/>
-      <c r="BN1" s="165"/>
-      <c r="BO1" s="165"/>
-      <c r="BP1" s="165"/>
-      <c r="BR1" s="168"/>
-      <c r="BS1" s="169"/>
-      <c r="BT1" s="169"/>
-      <c r="BU1" s="169"/>
-      <c r="BV1" s="169"/>
-      <c r="BW1" s="170"/>
+      <c r="AO1" s="170"/>
+      <c r="AP1" s="170"/>
+      <c r="AQ1" s="170"/>
+      <c r="AR1" s="170"/>
+      <c r="AS1" s="170"/>
+      <c r="AT1" s="170"/>
+      <c r="AU1" s="170"/>
+      <c r="AV1" s="170"/>
+      <c r="AW1" s="170"/>
+      <c r="AX1" s="170"/>
+      <c r="AY1" s="170"/>
+      <c r="AZ1" s="170"/>
+      <c r="BA1" s="170"/>
+      <c r="BB1" s="170"/>
+      <c r="BC1" s="170"/>
+      <c r="BD1" s="170"/>
+      <c r="BE1" s="170"/>
+      <c r="BF1" s="170"/>
+      <c r="BG1" s="170"/>
+      <c r="BH1" s="170"/>
+      <c r="BI1" s="170"/>
+      <c r="BJ1" s="170"/>
+      <c r="BK1" s="170"/>
+      <c r="BL1" s="170"/>
+      <c r="BM1" s="170"/>
+      <c r="BN1" s="170"/>
+      <c r="BO1" s="170"/>
+      <c r="BP1" s="170"/>
+      <c r="BR1" s="173"/>
+      <c r="BS1" s="174"/>
+      <c r="BT1" s="174"/>
+      <c r="BU1" s="174"/>
+      <c r="BV1" s="174"/>
+      <c r="BW1" s="175"/>
       <c r="BX1" s="156"/>
-      <c r="BZ1" s="165"/>
-      <c r="CA1" s="165"/>
-      <c r="CB1" s="165"/>
-      <c r="CC1" s="165"/>
-      <c r="CD1" s="165"/>
-      <c r="CE1" s="165"/>
-      <c r="CF1" s="165"/>
-      <c r="CG1" s="167"/>
-      <c r="CH1" s="166" t="s">
+      <c r="BZ1" s="170"/>
+      <c r="CA1" s="170"/>
+      <c r="CB1" s="170"/>
+      <c r="CC1" s="170"/>
+      <c r="CD1" s="170"/>
+      <c r="CE1" s="170"/>
+      <c r="CF1" s="170"/>
+      <c r="CG1" s="172"/>
+      <c r="CH1" s="171" t="s">
         <v>4</v>
       </c>
-      <c r="CI1" s="165"/>
-      <c r="CJ1" s="165"/>
-      <c r="CK1" s="165"/>
-      <c r="CL1" s="165"/>
-      <c r="CM1" s="167"/>
+      <c r="CI1" s="170"/>
+      <c r="CJ1" s="170"/>
+      <c r="CK1" s="170"/>
+      <c r="CL1" s="170"/>
+      <c r="CM1" s="172"/>
       <c r="CO1" s="85"/>
-      <c r="CP1" s="171" t="s">
+      <c r="CP1" s="176" t="s">
         <v>5</v>
       </c>
-      <c r="CQ1" s="171"/>
-      <c r="CR1" s="171"/>
-      <c r="CS1" s="171"/>
-      <c r="CT1" s="171"/>
-      <c r="CU1" s="171"/>
-      <c r="CV1" s="171"/>
+      <c r="CQ1" s="176"/>
+      <c r="CR1" s="176"/>
+      <c r="CS1" s="176"/>
+      <c r="CT1" s="176"/>
+      <c r="CU1" s="176"/>
+      <c r="CV1" s="176"/>
       <c r="CX1" s="140"/>
       <c r="CY1" s="140"/>
       <c r="CZ1" s="140"/>
@@ -72810,46 +72816,167 @@
       <c r="DT1101" s="42"/>
       <c r="DU1101" s="42"/>
     </row>
-    <row r="1102" spans="1:125">
-      <c r="A1102" s="41"/>
-      <c r="B1102" s="41"/>
-      <c r="C1102" s="41"/>
-      <c r="D1102" s="41"/>
-      <c r="G1102" s="41"/>
-      <c r="H1102" s="41"/>
-      <c r="I1102" s="41"/>
-      <c r="DP1102" s="42"/>
-      <c r="DQ1102" s="42"/>
-      <c r="DR1102" s="42"/>
-      <c r="DS1102" s="42"/>
-      <c r="DT1102" s="42"/>
-      <c r="DU1102" s="42"/>
-    </row>
-    <row r="1103" spans="1:125" s="179" customFormat="1" ht="30">
-      <c r="A1103" s="178" t="s">
+    <row r="1102" spans="1:125" s="165" customFormat="1">
+      <c r="A1102" s="164"/>
+      <c r="B1102" s="164"/>
+      <c r="C1102" s="164"/>
+      <c r="D1102" s="164" t="s">
+        <v>2183</v>
+      </c>
+      <c r="E1102" s="164" t="s">
+        <v>2183</v>
+      </c>
+      <c r="F1102" s="164"/>
+      <c r="G1102" s="164"/>
+      <c r="H1102" s="164"/>
+      <c r="I1102" s="164"/>
+      <c r="J1102" s="147"/>
+      <c r="K1102" s="147"/>
+      <c r="L1102" s="147"/>
+      <c r="M1102" s="147"/>
+      <c r="N1102" s="147"/>
+      <c r="O1102" s="147"/>
+      <c r="P1102" s="147">
+        <v>1</v>
+      </c>
+      <c r="Q1102" s="166"/>
+      <c r="R1102" s="147"/>
+      <c r="S1102" s="147"/>
+      <c r="T1102" s="147"/>
+      <c r="U1102" s="147"/>
+      <c r="V1102" s="147"/>
+      <c r="W1102" s="147"/>
+      <c r="X1102" s="147"/>
+      <c r="Y1102" s="147"/>
+      <c r="Z1102" s="147"/>
+      <c r="AA1102" s="147"/>
+      <c r="AB1102" s="147"/>
+      <c r="AC1102" s="147"/>
+      <c r="AD1102" s="147"/>
+      <c r="AE1102" s="147"/>
+      <c r="AF1102" s="147"/>
+      <c r="AG1102" s="147"/>
+      <c r="AH1102" s="147"/>
+      <c r="AI1102" s="147"/>
+      <c r="AJ1102" s="147"/>
+      <c r="AK1102" s="147"/>
+      <c r="AL1102" s="147"/>
+      <c r="AM1102" s="147"/>
+      <c r="AN1102" s="147"/>
+      <c r="AO1102" s="147"/>
+      <c r="AP1102" s="147"/>
+      <c r="AQ1102" s="147"/>
+      <c r="AR1102" s="147"/>
+      <c r="AS1102" s="147"/>
+      <c r="AT1102" s="147"/>
+      <c r="AU1102" s="147"/>
+      <c r="AV1102" s="147"/>
+      <c r="AW1102" s="147"/>
+      <c r="AX1102" s="147"/>
+      <c r="AY1102" s="147"/>
+      <c r="AZ1102" s="147"/>
+      <c r="BA1102" s="147"/>
+      <c r="BB1102" s="147"/>
+      <c r="BC1102" s="147"/>
+      <c r="BD1102" s="147"/>
+      <c r="BE1102" s="147"/>
+      <c r="BF1102" s="147"/>
+      <c r="BG1102" s="147"/>
+      <c r="BH1102" s="147"/>
+      <c r="BI1102" s="147"/>
+      <c r="BJ1102" s="147"/>
+      <c r="BK1102" s="147"/>
+      <c r="BL1102" s="147"/>
+      <c r="BM1102" s="147"/>
+      <c r="BN1102" s="147"/>
+      <c r="BO1102" s="147"/>
+      <c r="BP1102" s="147"/>
+      <c r="BQ1102" s="147"/>
+      <c r="BR1102" s="147"/>
+      <c r="BS1102" s="147"/>
+      <c r="BT1102" s="147"/>
+      <c r="BU1102" s="147"/>
+      <c r="BV1102" s="147"/>
+      <c r="BW1102" s="147"/>
+      <c r="BX1102" s="147"/>
+      <c r="BY1102" s="147"/>
+      <c r="BZ1102" s="147"/>
+      <c r="CA1102" s="147"/>
+      <c r="CB1102" s="147"/>
+      <c r="CC1102" s="147"/>
+      <c r="CD1102" s="147"/>
+      <c r="CE1102" s="147"/>
+      <c r="CF1102" s="147"/>
+      <c r="CG1102" s="147"/>
+      <c r="CH1102" s="147"/>
+      <c r="CI1102" s="147"/>
+      <c r="CJ1102" s="147"/>
+      <c r="CK1102" s="147"/>
+      <c r="CL1102" s="147"/>
+      <c r="CM1102" s="147"/>
+      <c r="CN1102" s="147">
+        <v>1</v>
+      </c>
+      <c r="CO1102" s="147"/>
+      <c r="CP1102" s="147"/>
+      <c r="CQ1102" s="147"/>
+      <c r="CR1102" s="147"/>
+      <c r="CS1102" s="147"/>
+      <c r="CT1102" s="147"/>
+      <c r="CU1102" s="147"/>
+      <c r="CV1102" s="147"/>
+      <c r="CW1102" s="147"/>
+      <c r="CX1102" s="147"/>
+      <c r="CY1102" s="147"/>
+      <c r="CZ1102" s="147"/>
+      <c r="DA1102" s="147" t="s">
+        <v>2184</v>
+      </c>
+      <c r="DB1102" s="167"/>
+      <c r="DC1102" s="167"/>
+      <c r="DD1102" s="147"/>
+      <c r="DE1102" s="147"/>
+      <c r="DF1102" s="147"/>
+      <c r="DG1102" s="147"/>
+      <c r="DH1102" s="147"/>
+      <c r="DI1102" s="147"/>
+      <c r="DJ1102" s="147"/>
+      <c r="DK1102" s="147"/>
+      <c r="DL1102" s="147"/>
+      <c r="DM1102" s="147"/>
+      <c r="DN1102" s="147"/>
+      <c r="DO1102" s="147"/>
+    </row>
+    <row r="1103" spans="1:125" s="165" customFormat="1" ht="30">
+      <c r="A1103" s="164" t="s">
         <v>2161</v>
       </c>
-      <c r="B1103" s="178"/>
-      <c r="C1103" s="178"/>
-      <c r="D1103" s="178" t="s">
+      <c r="B1103" s="164"/>
+      <c r="C1103" s="164"/>
+      <c r="D1103" s="164" t="s">
         <v>2162</v>
       </c>
-      <c r="F1103" s="178" t="s">
+      <c r="E1103" s="164" t="s">
+        <v>2162</v>
+      </c>
+      <c r="F1103" s="164" t="s">
         <v>2163</v>
       </c>
-      <c r="G1103" s="178" t="s">
-        <v>121</v>
-      </c>
-      <c r="H1103" s="178"/>
-      <c r="I1103" s="178"/>
+      <c r="G1103" s="164" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1103" s="164"/>
+      <c r="I1103" s="164"/>
       <c r="J1103" s="147"/>
       <c r="K1103" s="147"/>
       <c r="L1103" s="147"/>
       <c r="M1103" s="147"/>
       <c r="N1103" s="147"/>
       <c r="O1103" s="147"/>
-      <c r="P1103" s="147"/>
-      <c r="Q1103" s="180"/>
+      <c r="P1103" s="147">
+        <v>1</v>
+      </c>
+      <c r="Q1103" s="166"/>
       <c r="R1103" s="147">
         <v>1</v>
       </c>
@@ -72939,9 +73066,11 @@
       <c r="CX1103" s="147"/>
       <c r="CY1103" s="147"/>
       <c r="CZ1103" s="147"/>
-      <c r="DA1103" s="147"/>
-      <c r="DB1103" s="181"/>
-      <c r="DC1103" s="181"/>
+      <c r="DA1103" s="147" t="s">
+        <v>2184</v>
+      </c>
+      <c r="DB1103" s="167"/>
+      <c r="DC1103" s="167"/>
       <c r="DD1103" s="147"/>
       <c r="DE1103" s="147"/>
       <c r="DF1103" s="147"/>
@@ -72955,29 +73084,31 @@
       <c r="DN1103" s="147"/>
       <c r="DO1103" s="147"/>
     </row>
-    <row r="1104" spans="1:125" s="179" customFormat="1" ht="30">
-      <c r="A1104" s="178"/>
-      <c r="B1104" s="178"/>
-      <c r="C1104" s="178"/>
-      <c r="D1104" s="178" t="s">
+    <row r="1104" spans="1:125" s="165" customFormat="1" ht="30">
+      <c r="A1104" s="164"/>
+      <c r="B1104" s="164"/>
+      <c r="C1104" s="164"/>
+      <c r="D1104" s="164" t="s">
         <v>2164</v>
       </c>
-      <c r="F1104" s="178" t="s">
+      <c r="F1104" s="164" t="s">
         <v>2163</v>
       </c>
-      <c r="G1104" s="178" t="s">
-        <v>121</v>
-      </c>
-      <c r="H1104" s="178"/>
-      <c r="I1104" s="178"/>
+      <c r="G1104" s="164" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1104" s="164"/>
+      <c r="I1104" s="164"/>
       <c r="J1104" s="147"/>
       <c r="K1104" s="147"/>
       <c r="L1104" s="147"/>
       <c r="M1104" s="147"/>
       <c r="N1104" s="147"/>
       <c r="O1104" s="147"/>
-      <c r="P1104" s="147"/>
-      <c r="Q1104" s="180"/>
+      <c r="P1104" s="147">
+        <v>1</v>
+      </c>
+      <c r="Q1104" s="166"/>
       <c r="R1104" s="147"/>
       <c r="S1104" s="147">
         <v>1</v>
@@ -73067,9 +73198,11 @@
       <c r="CX1104" s="147"/>
       <c r="CY1104" s="147"/>
       <c r="CZ1104" s="147"/>
-      <c r="DA1104" s="147"/>
-      <c r="DB1104" s="181"/>
-      <c r="DC1104" s="181"/>
+      <c r="DA1104" s="147" t="s">
+        <v>2184</v>
+      </c>
+      <c r="DB1104" s="167"/>
+      <c r="DC1104" s="167"/>
       <c r="DD1104" s="147"/>
       <c r="DE1104" s="147"/>
       <c r="DF1104" s="147"/>
@@ -73083,29 +73216,31 @@
       <c r="DN1104" s="147"/>
       <c r="DO1104" s="147"/>
     </row>
-    <row r="1105" spans="1:119" s="179" customFormat="1" ht="30">
-      <c r="A1105" s="178"/>
-      <c r="B1105" s="178"/>
-      <c r="C1105" s="178"/>
-      <c r="D1105" s="178" t="s">
+    <row r="1105" spans="1:119" s="165" customFormat="1" ht="30">
+      <c r="A1105" s="164"/>
+      <c r="B1105" s="164"/>
+      <c r="C1105" s="164"/>
+      <c r="D1105" s="164" t="s">
         <v>2165</v>
       </c>
-      <c r="F1105" s="178" t="s">
+      <c r="F1105" s="164" t="s">
         <v>2163</v>
       </c>
-      <c r="G1105" s="178" t="s">
-        <v>121</v>
-      </c>
-      <c r="H1105" s="178"/>
-      <c r="I1105" s="178"/>
+      <c r="G1105" s="164" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1105" s="164"/>
+      <c r="I1105" s="164"/>
       <c r="J1105" s="147"/>
       <c r="K1105" s="147"/>
       <c r="L1105" s="147"/>
       <c r="M1105" s="147"/>
       <c r="N1105" s="147"/>
       <c r="O1105" s="147"/>
-      <c r="P1105" s="147"/>
-      <c r="Q1105" s="180"/>
+      <c r="P1105" s="147">
+        <v>1</v>
+      </c>
+      <c r="Q1105" s="166"/>
       <c r="R1105" s="147"/>
       <c r="S1105" s="147"/>
       <c r="T1105" s="147">
@@ -73195,9 +73330,11 @@
       <c r="CX1105" s="147"/>
       <c r="CY1105" s="147"/>
       <c r="CZ1105" s="147"/>
-      <c r="DA1105" s="147"/>
-      <c r="DB1105" s="181"/>
-      <c r="DC1105" s="181"/>
+      <c r="DA1105" s="147" t="s">
+        <v>2184</v>
+      </c>
+      <c r="DB1105" s="167"/>
+      <c r="DC1105" s="167"/>
       <c r="DD1105" s="147"/>
       <c r="DE1105" s="147"/>
       <c r="DF1105" s="147"/>
@@ -73211,29 +73348,31 @@
       <c r="DN1105" s="147"/>
       <c r="DO1105" s="147"/>
     </row>
-    <row r="1106" spans="1:119" s="179" customFormat="1" ht="30">
-      <c r="A1106" s="178"/>
-      <c r="B1106" s="178"/>
-      <c r="C1106" s="178"/>
-      <c r="D1106" s="178" t="s">
+    <row r="1106" spans="1:119" s="165" customFormat="1" ht="30">
+      <c r="A1106" s="164"/>
+      <c r="B1106" s="164"/>
+      <c r="C1106" s="164"/>
+      <c r="D1106" s="164" t="s">
         <v>2166</v>
       </c>
-      <c r="F1106" s="178" t="s">
+      <c r="F1106" s="164" t="s">
         <v>2163</v>
       </c>
-      <c r="G1106" s="178" t="s">
-        <v>121</v>
-      </c>
-      <c r="H1106" s="178"/>
-      <c r="I1106" s="178"/>
+      <c r="G1106" s="164" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1106" s="164"/>
+      <c r="I1106" s="164"/>
       <c r="J1106" s="147"/>
       <c r="K1106" s="147"/>
       <c r="L1106" s="147"/>
       <c r="M1106" s="147"/>
       <c r="N1106" s="147"/>
       <c r="O1106" s="147"/>
-      <c r="P1106" s="147"/>
-      <c r="Q1106" s="180"/>
+      <c r="P1106" s="147">
+        <v>1</v>
+      </c>
+      <c r="Q1106" s="166"/>
       <c r="R1106" s="147"/>
       <c r="S1106" s="147"/>
       <c r="T1106" s="147"/>
@@ -73323,9 +73462,11 @@
       <c r="CX1106" s="147"/>
       <c r="CY1106" s="147"/>
       <c r="CZ1106" s="147"/>
-      <c r="DA1106" s="147"/>
-      <c r="DB1106" s="181"/>
-      <c r="DC1106" s="181"/>
+      <c r="DA1106" s="147" t="s">
+        <v>2184</v>
+      </c>
+      <c r="DB1106" s="167"/>
+      <c r="DC1106" s="167"/>
       <c r="DD1106" s="147"/>
       <c r="DE1106" s="147"/>
       <c r="DF1106" s="147"/>
@@ -73339,29 +73480,31 @@
       <c r="DN1106" s="147"/>
       <c r="DO1106" s="147"/>
     </row>
-    <row r="1107" spans="1:119" s="179" customFormat="1" ht="30">
-      <c r="A1107" s="178"/>
-      <c r="B1107" s="178"/>
-      <c r="C1107" s="178"/>
-      <c r="D1107" s="178" t="s">
+    <row r="1107" spans="1:119" s="165" customFormat="1" ht="30">
+      <c r="A1107" s="164"/>
+      <c r="B1107" s="164"/>
+      <c r="C1107" s="164"/>
+      <c r="D1107" s="164" t="s">
         <v>2167</v>
       </c>
-      <c r="F1107" s="178" t="s">
+      <c r="F1107" s="164" t="s">
         <v>2163</v>
       </c>
-      <c r="G1107" s="178" t="s">
-        <v>121</v>
-      </c>
-      <c r="H1107" s="178"/>
-      <c r="I1107" s="178"/>
+      <c r="G1107" s="164" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1107" s="164"/>
+      <c r="I1107" s="164"/>
       <c r="J1107" s="147"/>
       <c r="K1107" s="147"/>
       <c r="L1107" s="147"/>
       <c r="M1107" s="147"/>
       <c r="N1107" s="147"/>
       <c r="O1107" s="147"/>
-      <c r="P1107" s="147"/>
-      <c r="Q1107" s="180"/>
+      <c r="P1107" s="147">
+        <v>1</v>
+      </c>
+      <c r="Q1107" s="166"/>
       <c r="R1107" s="147"/>
       <c r="S1107" s="147"/>
       <c r="T1107" s="147"/>
@@ -73451,9 +73594,11 @@
       <c r="CX1107" s="147"/>
       <c r="CY1107" s="147"/>
       <c r="CZ1107" s="147"/>
-      <c r="DA1107" s="147"/>
-      <c r="DB1107" s="181"/>
-      <c r="DC1107" s="181"/>
+      <c r="DA1107" s="147" t="s">
+        <v>2184</v>
+      </c>
+      <c r="DB1107" s="167"/>
+      <c r="DC1107" s="167"/>
       <c r="DD1107" s="147"/>
       <c r="DE1107" s="147"/>
       <c r="DF1107" s="147"/>
@@ -73467,29 +73612,31 @@
       <c r="DN1107" s="147"/>
       <c r="DO1107" s="147"/>
     </row>
-    <row r="1108" spans="1:119" s="179" customFormat="1" ht="30">
-      <c r="A1108" s="178"/>
-      <c r="B1108" s="178"/>
-      <c r="C1108" s="178"/>
-      <c r="D1108" s="178" t="s">
+    <row r="1108" spans="1:119" s="165" customFormat="1" ht="30">
+      <c r="A1108" s="164"/>
+      <c r="B1108" s="164"/>
+      <c r="C1108" s="164"/>
+      <c r="D1108" s="164" t="s">
         <v>2168</v>
       </c>
-      <c r="F1108" s="178" t="s">
+      <c r="F1108" s="164" t="s">
         <v>2163</v>
       </c>
-      <c r="G1108" s="178" t="s">
-        <v>121</v>
-      </c>
-      <c r="H1108" s="178"/>
-      <c r="I1108" s="178"/>
+      <c r="G1108" s="164" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1108" s="164"/>
+      <c r="I1108" s="164"/>
       <c r="J1108" s="147"/>
       <c r="K1108" s="147"/>
       <c r="L1108" s="147"/>
       <c r="M1108" s="147"/>
       <c r="N1108" s="147"/>
       <c r="O1108" s="147"/>
-      <c r="P1108" s="147"/>
-      <c r="Q1108" s="180"/>
+      <c r="P1108" s="147">
+        <v>1</v>
+      </c>
+      <c r="Q1108" s="166"/>
       <c r="R1108" s="147"/>
       <c r="S1108" s="147"/>
       <c r="T1108" s="147"/>
@@ -73579,9 +73726,11 @@
       <c r="CX1108" s="147"/>
       <c r="CY1108" s="147"/>
       <c r="CZ1108" s="147"/>
-      <c r="DA1108" s="147"/>
-      <c r="DB1108" s="181"/>
-      <c r="DC1108" s="181"/>
+      <c r="DA1108" s="147" t="s">
+        <v>2184</v>
+      </c>
+      <c r="DB1108" s="167"/>
+      <c r="DC1108" s="167"/>
       <c r="DD1108" s="147"/>
       <c r="DE1108" s="147"/>
       <c r="DF1108" s="147"/>
@@ -73595,29 +73744,31 @@
       <c r="DN1108" s="147"/>
       <c r="DO1108" s="147"/>
     </row>
-    <row r="1109" spans="1:119" s="179" customFormat="1" ht="30">
-      <c r="A1109" s="182"/>
-      <c r="B1109" s="178"/>
-      <c r="C1109" s="178"/>
-      <c r="D1109" s="178" t="s">
+    <row r="1109" spans="1:119" s="165" customFormat="1" ht="30">
+      <c r="A1109" s="168"/>
+      <c r="B1109" s="164"/>
+      <c r="C1109" s="164"/>
+      <c r="D1109" s="164" t="s">
         <v>2169</v>
       </c>
-      <c r="F1109" s="178" t="s">
+      <c r="F1109" s="164" t="s">
         <v>2163</v>
       </c>
-      <c r="G1109" s="178" t="s">
-        <v>121</v>
-      </c>
-      <c r="H1109" s="178"/>
-      <c r="I1109" s="178"/>
+      <c r="G1109" s="164" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1109" s="164"/>
+      <c r="I1109" s="164"/>
       <c r="J1109" s="147"/>
       <c r="K1109" s="147"/>
       <c r="L1109" s="147"/>
       <c r="M1109" s="147"/>
       <c r="N1109" s="147"/>
       <c r="O1109" s="147"/>
-      <c r="P1109" s="147"/>
-      <c r="Q1109" s="180"/>
+      <c r="P1109" s="147">
+        <v>1</v>
+      </c>
+      <c r="Q1109" s="166"/>
       <c r="R1109" s="147"/>
       <c r="S1109" s="147"/>
       <c r="T1109" s="147"/>
@@ -73707,9 +73858,11 @@
       <c r="CX1109" s="147"/>
       <c r="CY1109" s="147"/>
       <c r="CZ1109" s="147"/>
-      <c r="DA1109" s="147"/>
-      <c r="DB1109" s="181"/>
-      <c r="DC1109" s="181"/>
+      <c r="DA1109" s="147" t="s">
+        <v>2184</v>
+      </c>
+      <c r="DB1109" s="167"/>
+      <c r="DC1109" s="167"/>
       <c r="DD1109" s="147"/>
       <c r="DE1109" s="147"/>
       <c r="DF1109" s="147"/>
@@ -73723,29 +73876,31 @@
       <c r="DN1109" s="147"/>
       <c r="DO1109" s="147"/>
     </row>
-    <row r="1110" spans="1:119" s="179" customFormat="1" ht="30">
-      <c r="A1110" s="178"/>
-      <c r="B1110" s="178"/>
-      <c r="C1110" s="178"/>
-      <c r="D1110" s="178" t="s">
+    <row r="1110" spans="1:119" s="165" customFormat="1" ht="30">
+      <c r="A1110" s="164"/>
+      <c r="B1110" s="164"/>
+      <c r="C1110" s="164"/>
+      <c r="D1110" s="164" t="s">
         <v>2170</v>
       </c>
-      <c r="F1110" s="178" t="s">
+      <c r="F1110" s="164" t="s">
         <v>2163</v>
       </c>
-      <c r="G1110" s="178" t="s">
-        <v>121</v>
-      </c>
-      <c r="H1110" s="178"/>
-      <c r="I1110" s="178"/>
+      <c r="G1110" s="164" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1110" s="164"/>
+      <c r="I1110" s="164"/>
       <c r="J1110" s="147"/>
       <c r="K1110" s="147"/>
       <c r="L1110" s="147"/>
       <c r="M1110" s="147"/>
       <c r="N1110" s="147"/>
       <c r="O1110" s="147"/>
-      <c r="P1110" s="147"/>
-      <c r="Q1110" s="180"/>
+      <c r="P1110" s="147">
+        <v>1</v>
+      </c>
+      <c r="Q1110" s="166"/>
       <c r="R1110" s="147"/>
       <c r="S1110" s="147"/>
       <c r="T1110" s="147"/>
@@ -73835,9 +73990,11 @@
       <c r="CX1110" s="147"/>
       <c r="CY1110" s="147"/>
       <c r="CZ1110" s="147"/>
-      <c r="DA1110" s="147"/>
-      <c r="DB1110" s="181"/>
-      <c r="DC1110" s="181"/>
+      <c r="DA1110" s="147" t="s">
+        <v>2184</v>
+      </c>
+      <c r="DB1110" s="167"/>
+      <c r="DC1110" s="167"/>
       <c r="DD1110" s="147"/>
       <c r="DE1110" s="147"/>
       <c r="DF1110" s="147"/>
@@ -73851,29 +74008,31 @@
       <c r="DN1110" s="147"/>
       <c r="DO1110" s="147"/>
     </row>
-    <row r="1111" spans="1:119" s="179" customFormat="1" ht="30">
-      <c r="A1111" s="178"/>
-      <c r="B1111" s="178"/>
-      <c r="C1111" s="178"/>
-      <c r="D1111" s="178" t="s">
+    <row r="1111" spans="1:119" s="165" customFormat="1" ht="30">
+      <c r="A1111" s="164"/>
+      <c r="B1111" s="164"/>
+      <c r="C1111" s="164"/>
+      <c r="D1111" s="164" t="s">
         <v>2171</v>
       </c>
-      <c r="F1111" s="178" t="s">
+      <c r="F1111" s="164" t="s">
         <v>2163</v>
       </c>
-      <c r="G1111" s="178" t="s">
-        <v>121</v>
-      </c>
-      <c r="H1111" s="178"/>
-      <c r="I1111" s="178"/>
+      <c r="G1111" s="164" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1111" s="164"/>
+      <c r="I1111" s="164"/>
       <c r="J1111" s="147"/>
       <c r="K1111" s="147"/>
       <c r="L1111" s="147"/>
       <c r="M1111" s="147"/>
       <c r="N1111" s="147"/>
       <c r="O1111" s="147"/>
-      <c r="P1111" s="147"/>
-      <c r="Q1111" s="180"/>
+      <c r="P1111" s="147">
+        <v>1</v>
+      </c>
+      <c r="Q1111" s="166"/>
       <c r="R1111" s="147"/>
       <c r="S1111" s="147"/>
       <c r="T1111" s="147"/>
@@ -73963,9 +74122,11 @@
       <c r="CX1111" s="147"/>
       <c r="CY1111" s="147"/>
       <c r="CZ1111" s="147"/>
-      <c r="DA1111" s="147"/>
-      <c r="DB1111" s="181"/>
-      <c r="DC1111" s="181"/>
+      <c r="DA1111" s="147" t="s">
+        <v>2184</v>
+      </c>
+      <c r="DB1111" s="167"/>
+      <c r="DC1111" s="167"/>
       <c r="DD1111" s="147"/>
       <c r="DE1111" s="147"/>
       <c r="DF1111" s="147"/>
@@ -73979,29 +74140,31 @@
       <c r="DN1111" s="147"/>
       <c r="DO1111" s="147"/>
     </row>
-    <row r="1112" spans="1:119" s="179" customFormat="1" ht="30">
-      <c r="A1112" s="178"/>
-      <c r="B1112" s="178"/>
-      <c r="C1112" s="178"/>
-      <c r="D1112" s="178" t="s">
+    <row r="1112" spans="1:119" s="165" customFormat="1" ht="30">
+      <c r="A1112" s="164"/>
+      <c r="B1112" s="164"/>
+      <c r="C1112" s="164"/>
+      <c r="D1112" s="164" t="s">
         <v>2172</v>
       </c>
-      <c r="F1112" s="178" t="s">
+      <c r="F1112" s="164" t="s">
         <v>2163</v>
       </c>
-      <c r="G1112" s="178" t="s">
-        <v>121</v>
-      </c>
-      <c r="H1112" s="178"/>
-      <c r="I1112" s="178"/>
+      <c r="G1112" s="164" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1112" s="164"/>
+      <c r="I1112" s="164"/>
       <c r="J1112" s="147"/>
       <c r="K1112" s="147"/>
       <c r="L1112" s="147"/>
       <c r="M1112" s="147"/>
       <c r="N1112" s="147"/>
       <c r="O1112" s="147"/>
-      <c r="P1112" s="147"/>
-      <c r="Q1112" s="180"/>
+      <c r="P1112" s="147">
+        <v>1</v>
+      </c>
+      <c r="Q1112" s="166"/>
       <c r="R1112" s="147"/>
       <c r="S1112" s="147"/>
       <c r="T1112" s="147"/>
@@ -74091,9 +74254,11 @@
       <c r="CX1112" s="147"/>
       <c r="CY1112" s="147"/>
       <c r="CZ1112" s="147"/>
-      <c r="DA1112" s="147"/>
-      <c r="DB1112" s="181"/>
-      <c r="DC1112" s="181"/>
+      <c r="DA1112" s="147" t="s">
+        <v>2184</v>
+      </c>
+      <c r="DB1112" s="167"/>
+      <c r="DC1112" s="167"/>
       <c r="DD1112" s="147"/>
       <c r="DE1112" s="147"/>
       <c r="DF1112" s="147"/>
@@ -74107,29 +74272,31 @@
       <c r="DN1112" s="147"/>
       <c r="DO1112" s="147"/>
     </row>
-    <row r="1113" spans="1:119" s="179" customFormat="1" ht="30">
-      <c r="A1113" s="178"/>
-      <c r="B1113" s="178"/>
-      <c r="C1113" s="178"/>
-      <c r="D1113" s="178" t="s">
+    <row r="1113" spans="1:119" s="165" customFormat="1" ht="30">
+      <c r="A1113" s="164"/>
+      <c r="B1113" s="164"/>
+      <c r="C1113" s="164"/>
+      <c r="D1113" s="164" t="s">
         <v>2173</v>
       </c>
-      <c r="F1113" s="178" t="s">
+      <c r="F1113" s="164" t="s">
         <v>2163</v>
       </c>
-      <c r="G1113" s="178" t="s">
-        <v>121</v>
-      </c>
-      <c r="H1113" s="178"/>
-      <c r="I1113" s="178"/>
+      <c r="G1113" s="164" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1113" s="164"/>
+      <c r="I1113" s="164"/>
       <c r="J1113" s="147"/>
       <c r="K1113" s="147"/>
       <c r="L1113" s="147"/>
       <c r="M1113" s="147"/>
       <c r="N1113" s="147"/>
       <c r="O1113" s="147"/>
-      <c r="P1113" s="147"/>
-      <c r="Q1113" s="180"/>
+      <c r="P1113" s="147">
+        <v>1</v>
+      </c>
+      <c r="Q1113" s="166"/>
       <c r="R1113" s="147"/>
       <c r="S1113" s="147"/>
       <c r="T1113" s="147"/>
@@ -74219,9 +74386,11 @@
       <c r="CX1113" s="147"/>
       <c r="CY1113" s="147"/>
       <c r="CZ1113" s="147"/>
-      <c r="DA1113" s="147"/>
-      <c r="DB1113" s="181"/>
-      <c r="DC1113" s="181"/>
+      <c r="DA1113" s="147" t="s">
+        <v>2184</v>
+      </c>
+      <c r="DB1113" s="167"/>
+      <c r="DC1113" s="167"/>
       <c r="DD1113" s="147"/>
       <c r="DE1113" s="147"/>
       <c r="DF1113" s="147"/>
@@ -74235,29 +74404,31 @@
       <c r="DN1113" s="147"/>
       <c r="DO1113" s="147"/>
     </row>
-    <row r="1114" spans="1:119" s="179" customFormat="1" ht="30">
-      <c r="A1114" s="178"/>
-      <c r="B1114" s="178"/>
-      <c r="C1114" s="178"/>
-      <c r="D1114" s="178" t="s">
+    <row r="1114" spans="1:119" s="165" customFormat="1" ht="30">
+      <c r="A1114" s="164"/>
+      <c r="B1114" s="164"/>
+      <c r="C1114" s="164"/>
+      <c r="D1114" s="164" t="s">
         <v>2174</v>
       </c>
-      <c r="F1114" s="178" t="s">
+      <c r="F1114" s="164" t="s">
         <v>2163</v>
       </c>
-      <c r="G1114" s="178" t="s">
-        <v>121</v>
-      </c>
-      <c r="H1114" s="178"/>
-      <c r="I1114" s="178"/>
+      <c r="G1114" s="164" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1114" s="164"/>
+      <c r="I1114" s="164"/>
       <c r="J1114" s="147"/>
       <c r="K1114" s="147"/>
       <c r="L1114" s="147"/>
       <c r="M1114" s="147"/>
       <c r="N1114" s="147"/>
       <c r="O1114" s="147"/>
-      <c r="P1114" s="147"/>
-      <c r="Q1114" s="180"/>
+      <c r="P1114" s="147">
+        <v>1</v>
+      </c>
+      <c r="Q1114" s="166"/>
       <c r="R1114" s="147"/>
       <c r="S1114" s="147"/>
       <c r="T1114" s="147"/>
@@ -74347,9 +74518,11 @@
       <c r="CX1114" s="147"/>
       <c r="CY1114" s="147"/>
       <c r="CZ1114" s="147"/>
-      <c r="DA1114" s="147"/>
-      <c r="DB1114" s="181"/>
-      <c r="DC1114" s="181"/>
+      <c r="DA1114" s="147" t="s">
+        <v>2184</v>
+      </c>
+      <c r="DB1114" s="167"/>
+      <c r="DC1114" s="167"/>
       <c r="DD1114" s="147"/>
       <c r="DE1114" s="147"/>
       <c r="DF1114" s="147"/>
@@ -74363,29 +74536,31 @@
       <c r="DN1114" s="147"/>
       <c r="DO1114" s="147"/>
     </row>
-    <row r="1115" spans="1:119" s="179" customFormat="1" ht="30">
-      <c r="A1115" s="178"/>
-      <c r="B1115" s="178"/>
-      <c r="C1115" s="178"/>
-      <c r="D1115" s="178" t="s">
+    <row r="1115" spans="1:119" s="165" customFormat="1" ht="30">
+      <c r="A1115" s="164"/>
+      <c r="B1115" s="164"/>
+      <c r="C1115" s="164"/>
+      <c r="D1115" s="164" t="s">
         <v>2175</v>
       </c>
-      <c r="F1115" s="178" t="s">
+      <c r="F1115" s="164" t="s">
         <v>2163</v>
       </c>
-      <c r="G1115" s="178" t="s">
-        <v>121</v>
-      </c>
-      <c r="H1115" s="178"/>
-      <c r="I1115" s="178"/>
+      <c r="G1115" s="164" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1115" s="164"/>
+      <c r="I1115" s="164"/>
       <c r="J1115" s="147"/>
       <c r="K1115" s="147"/>
       <c r="L1115" s="147"/>
       <c r="M1115" s="147"/>
       <c r="N1115" s="147"/>
       <c r="O1115" s="147"/>
-      <c r="P1115" s="147"/>
-      <c r="Q1115" s="180"/>
+      <c r="P1115" s="147">
+        <v>1</v>
+      </c>
+      <c r="Q1115" s="166"/>
       <c r="R1115" s="147"/>
       <c r="S1115" s="147"/>
       <c r="T1115" s="147"/>
@@ -74475,9 +74650,11 @@
       <c r="CX1115" s="147"/>
       <c r="CY1115" s="147"/>
       <c r="CZ1115" s="147"/>
-      <c r="DA1115" s="147"/>
-      <c r="DB1115" s="181"/>
-      <c r="DC1115" s="181"/>
+      <c r="DA1115" s="147" t="s">
+        <v>2184</v>
+      </c>
+      <c r="DB1115" s="167"/>
+      <c r="DC1115" s="167"/>
       <c r="DD1115" s="147"/>
       <c r="DE1115" s="147"/>
       <c r="DF1115" s="147"/>
@@ -74491,29 +74668,31 @@
       <c r="DN1115" s="147"/>
       <c r="DO1115" s="147"/>
     </row>
-    <row r="1116" spans="1:119" s="179" customFormat="1" ht="30">
-      <c r="A1116" s="178"/>
-      <c r="B1116" s="178"/>
-      <c r="C1116" s="178"/>
-      <c r="D1116" s="178" t="s">
+    <row r="1116" spans="1:119" s="165" customFormat="1" ht="30">
+      <c r="A1116" s="164"/>
+      <c r="B1116" s="164"/>
+      <c r="C1116" s="164"/>
+      <c r="D1116" s="164" t="s">
         <v>2176</v>
       </c>
-      <c r="F1116" s="178" t="s">
+      <c r="F1116" s="164" t="s">
         <v>2163</v>
       </c>
-      <c r="G1116" s="178" t="s">
-        <v>121</v>
-      </c>
-      <c r="H1116" s="178"/>
-      <c r="I1116" s="178"/>
+      <c r="G1116" s="164" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1116" s="164"/>
+      <c r="I1116" s="164"/>
       <c r="J1116" s="147"/>
       <c r="K1116" s="147"/>
       <c r="L1116" s="147"/>
       <c r="M1116" s="147"/>
       <c r="N1116" s="147"/>
       <c r="O1116" s="147"/>
-      <c r="P1116" s="147"/>
-      <c r="Q1116" s="180"/>
+      <c r="P1116" s="147">
+        <v>1</v>
+      </c>
+      <c r="Q1116" s="166"/>
       <c r="R1116" s="147"/>
       <c r="S1116" s="147"/>
       <c r="T1116" s="147"/>
@@ -74603,9 +74782,11 @@
       <c r="CX1116" s="147"/>
       <c r="CY1116" s="147"/>
       <c r="CZ1116" s="147"/>
-      <c r="DA1116" s="147"/>
-      <c r="DB1116" s="181"/>
-      <c r="DC1116" s="181"/>
+      <c r="DA1116" s="147" t="s">
+        <v>2184</v>
+      </c>
+      <c r="DB1116" s="167"/>
+      <c r="DC1116" s="167"/>
       <c r="DD1116" s="147"/>
       <c r="DE1116" s="147"/>
       <c r="DF1116" s="147"/>
@@ -74619,29 +74800,31 @@
       <c r="DN1116" s="147"/>
       <c r="DO1116" s="147"/>
     </row>
-    <row r="1117" spans="1:119" s="179" customFormat="1" ht="30">
-      <c r="A1117" s="178"/>
-      <c r="B1117" s="178"/>
-      <c r="C1117" s="178"/>
-      <c r="D1117" s="178" t="s">
+    <row r="1117" spans="1:119" s="165" customFormat="1" ht="30">
+      <c r="A1117" s="164"/>
+      <c r="B1117" s="164"/>
+      <c r="C1117" s="164"/>
+      <c r="D1117" s="164" t="s">
         <v>2177</v>
       </c>
-      <c r="F1117" s="178" t="s">
+      <c r="F1117" s="164" t="s">
         <v>2163</v>
       </c>
-      <c r="G1117" s="178" t="s">
-        <v>121</v>
-      </c>
-      <c r="H1117" s="178"/>
-      <c r="I1117" s="178"/>
+      <c r="G1117" s="164" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1117" s="164"/>
+      <c r="I1117" s="164"/>
       <c r="J1117" s="147"/>
       <c r="K1117" s="147"/>
       <c r="L1117" s="147"/>
       <c r="M1117" s="147"/>
       <c r="N1117" s="147"/>
       <c r="O1117" s="147"/>
-      <c r="P1117" s="147"/>
-      <c r="Q1117" s="180"/>
+      <c r="P1117" s="147">
+        <v>1</v>
+      </c>
+      <c r="Q1117" s="166"/>
       <c r="R1117" s="147"/>
       <c r="S1117" s="147"/>
       <c r="T1117" s="147"/>
@@ -74731,9 +74914,11 @@
       <c r="CX1117" s="147"/>
       <c r="CY1117" s="147"/>
       <c r="CZ1117" s="147"/>
-      <c r="DA1117" s="147"/>
-      <c r="DB1117" s="181"/>
-      <c r="DC1117" s="181"/>
+      <c r="DA1117" s="147" t="s">
+        <v>2184</v>
+      </c>
+      <c r="DB1117" s="167"/>
+      <c r="DC1117" s="167"/>
       <c r="DD1117" s="147"/>
       <c r="DE1117" s="147"/>
       <c r="DF1117" s="147"/>
@@ -74747,29 +74932,31 @@
       <c r="DN1117" s="147"/>
       <c r="DO1117" s="147"/>
     </row>
-    <row r="1118" spans="1:119" s="179" customFormat="1" ht="30">
-      <c r="A1118" s="178"/>
-      <c r="B1118" s="178"/>
-      <c r="C1118" s="178"/>
-      <c r="D1118" s="178" t="s">
+    <row r="1118" spans="1:119" s="165" customFormat="1" ht="30">
+      <c r="A1118" s="164"/>
+      <c r="B1118" s="164"/>
+      <c r="C1118" s="164"/>
+      <c r="D1118" s="164" t="s">
         <v>2178</v>
       </c>
-      <c r="F1118" s="178" t="s">
+      <c r="F1118" s="164" t="s">
         <v>2163</v>
       </c>
-      <c r="G1118" s="178" t="s">
-        <v>121</v>
-      </c>
-      <c r="H1118" s="178"/>
-      <c r="I1118" s="178"/>
+      <c r="G1118" s="164" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1118" s="164"/>
+      <c r="I1118" s="164"/>
       <c r="J1118" s="147"/>
       <c r="K1118" s="147"/>
       <c r="L1118" s="147"/>
       <c r="M1118" s="147"/>
       <c r="N1118" s="147"/>
       <c r="O1118" s="147"/>
-      <c r="P1118" s="147"/>
-      <c r="Q1118" s="180"/>
+      <c r="P1118" s="147">
+        <v>1</v>
+      </c>
+      <c r="Q1118" s="166"/>
       <c r="R1118" s="147"/>
       <c r="S1118" s="147"/>
       <c r="T1118" s="147"/>
@@ -74859,9 +75046,11 @@
       <c r="CX1118" s="147"/>
       <c r="CY1118" s="147"/>
       <c r="CZ1118" s="147"/>
-      <c r="DA1118" s="147"/>
-      <c r="DB1118" s="181"/>
-      <c r="DC1118" s="181"/>
+      <c r="DA1118" s="147" t="s">
+        <v>2184</v>
+      </c>
+      <c r="DB1118" s="167"/>
+      <c r="DC1118" s="167"/>
       <c r="DD1118" s="147"/>
       <c r="DE1118" s="147"/>
       <c r="DF1118" s="147"/>
@@ -74875,29 +75064,31 @@
       <c r="DN1118" s="147"/>
       <c r="DO1118" s="147"/>
     </row>
-    <row r="1119" spans="1:119" s="179" customFormat="1" ht="30">
-      <c r="A1119" s="178"/>
-      <c r="B1119" s="178"/>
-      <c r="C1119" s="178"/>
-      <c r="D1119" s="178" t="s">
+    <row r="1119" spans="1:119" s="165" customFormat="1" ht="30">
+      <c r="A1119" s="164"/>
+      <c r="B1119" s="164"/>
+      <c r="C1119" s="164"/>
+      <c r="D1119" s="164" t="s">
         <v>2179</v>
       </c>
-      <c r="F1119" s="178" t="s">
+      <c r="F1119" s="164" t="s">
         <v>2163</v>
       </c>
-      <c r="G1119" s="178" t="s">
-        <v>121</v>
-      </c>
-      <c r="H1119" s="178"/>
-      <c r="I1119" s="178"/>
+      <c r="G1119" s="164" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1119" s="164"/>
+      <c r="I1119" s="164"/>
       <c r="J1119" s="147"/>
       <c r="K1119" s="147"/>
       <c r="L1119" s="147"/>
       <c r="M1119" s="147"/>
       <c r="N1119" s="147"/>
       <c r="O1119" s="147"/>
-      <c r="P1119" s="147"/>
-      <c r="Q1119" s="180"/>
+      <c r="P1119" s="147">
+        <v>1</v>
+      </c>
+      <c r="Q1119" s="166"/>
       <c r="R1119" s="147"/>
       <c r="S1119" s="147"/>
       <c r="T1119" s="147"/>
@@ -74987,9 +75178,11 @@
       <c r="CX1119" s="147"/>
       <c r="CY1119" s="147"/>
       <c r="CZ1119" s="147"/>
-      <c r="DA1119" s="147"/>
-      <c r="DB1119" s="181"/>
-      <c r="DC1119" s="181"/>
+      <c r="DA1119" s="147" t="s">
+        <v>2184</v>
+      </c>
+      <c r="DB1119" s="167"/>
+      <c r="DC1119" s="167"/>
       <c r="DD1119" s="147"/>
       <c r="DE1119" s="147"/>
       <c r="DF1119" s="147"/>
@@ -75003,29 +75196,31 @@
       <c r="DN1119" s="147"/>
       <c r="DO1119" s="147"/>
     </row>
-    <row r="1120" spans="1:119" s="179" customFormat="1" ht="30">
-      <c r="A1120" s="178"/>
-      <c r="B1120" s="178"/>
-      <c r="C1120" s="178"/>
-      <c r="D1120" s="178" t="s">
+    <row r="1120" spans="1:119" s="165" customFormat="1" ht="30">
+      <c r="A1120" s="164"/>
+      <c r="B1120" s="164"/>
+      <c r="C1120" s="164"/>
+      <c r="D1120" s="164" t="s">
         <v>2180</v>
       </c>
-      <c r="F1120" s="178" t="s">
+      <c r="F1120" s="164" t="s">
         <v>2163</v>
       </c>
-      <c r="G1120" s="178" t="s">
-        <v>121</v>
-      </c>
-      <c r="H1120" s="178"/>
-      <c r="I1120" s="178"/>
+      <c r="G1120" s="164" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1120" s="164"/>
+      <c r="I1120" s="164"/>
       <c r="J1120" s="147"/>
       <c r="K1120" s="147"/>
       <c r="L1120" s="147"/>
       <c r="M1120" s="147"/>
       <c r="N1120" s="147"/>
       <c r="O1120" s="147"/>
-      <c r="P1120" s="147"/>
-      <c r="Q1120" s="180"/>
+      <c r="P1120" s="147">
+        <v>1</v>
+      </c>
+      <c r="Q1120" s="166"/>
       <c r="R1120" s="147"/>
       <c r="S1120" s="147"/>
       <c r="T1120" s="147"/>
@@ -75115,9 +75310,11 @@
       <c r="CX1120" s="147"/>
       <c r="CY1120" s="147"/>
       <c r="CZ1120" s="147"/>
-      <c r="DA1120" s="147"/>
-      <c r="DB1120" s="181"/>
-      <c r="DC1120" s="181"/>
+      <c r="DA1120" s="147" t="s">
+        <v>2184</v>
+      </c>
+      <c r="DB1120" s="167"/>
+      <c r="DC1120" s="167"/>
       <c r="DD1120" s="147"/>
       <c r="DE1120" s="147"/>
       <c r="DF1120" s="147"/>
@@ -75131,29 +75328,31 @@
       <c r="DN1120" s="147"/>
       <c r="DO1120" s="147"/>
     </row>
-    <row r="1121" spans="1:119" s="179" customFormat="1" ht="30">
-      <c r="A1121" s="178"/>
-      <c r="B1121" s="178"/>
-      <c r="C1121" s="178"/>
-      <c r="D1121" s="178" t="s">
+    <row r="1121" spans="1:119" s="165" customFormat="1" ht="30">
+      <c r="A1121" s="164"/>
+      <c r="B1121" s="164"/>
+      <c r="C1121" s="164"/>
+      <c r="D1121" s="164" t="s">
         <v>2181</v>
       </c>
-      <c r="F1121" s="178" t="s">
+      <c r="F1121" s="164" t="s">
         <v>2163</v>
       </c>
-      <c r="G1121" s="178" t="s">
-        <v>121</v>
-      </c>
-      <c r="H1121" s="178"/>
-      <c r="I1121" s="178"/>
+      <c r="G1121" s="164" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1121" s="164"/>
+      <c r="I1121" s="164"/>
       <c r="J1121" s="147"/>
       <c r="K1121" s="147"/>
       <c r="L1121" s="147"/>
       <c r="M1121" s="147"/>
       <c r="N1121" s="147"/>
       <c r="O1121" s="147"/>
-      <c r="P1121" s="147"/>
-      <c r="Q1121" s="180"/>
+      <c r="P1121" s="147">
+        <v>1</v>
+      </c>
+      <c r="Q1121" s="166"/>
       <c r="R1121" s="147"/>
       <c r="S1121" s="147"/>
       <c r="T1121" s="147"/>
@@ -75243,9 +75442,11 @@
       <c r="CX1121" s="147"/>
       <c r="CY1121" s="147"/>
       <c r="CZ1121" s="147"/>
-      <c r="DA1121" s="147"/>
-      <c r="DB1121" s="181"/>
-      <c r="DC1121" s="181"/>
+      <c r="DA1121" s="147" t="s">
+        <v>2184</v>
+      </c>
+      <c r="DB1121" s="167"/>
+      <c r="DC1121" s="167"/>
       <c r="DD1121" s="147"/>
       <c r="DE1121" s="147"/>
       <c r="DF1121" s="147"/>
@@ -75259,29 +75460,31 @@
       <c r="DN1121" s="147"/>
       <c r="DO1121" s="147"/>
     </row>
-    <row r="1122" spans="1:119" s="179" customFormat="1" ht="30">
-      <c r="A1122" s="178"/>
-      <c r="B1122" s="178"/>
-      <c r="C1122" s="178"/>
-      <c r="D1122" s="178" t="s">
+    <row r="1122" spans="1:119" s="165" customFormat="1" ht="30">
+      <c r="A1122" s="164"/>
+      <c r="B1122" s="164"/>
+      <c r="C1122" s="164"/>
+      <c r="D1122" s="164" t="s">
         <v>2182</v>
       </c>
-      <c r="F1122" s="178" t="s">
+      <c r="F1122" s="164" t="s">
         <v>2163</v>
       </c>
-      <c r="G1122" s="178" t="s">
-        <v>121</v>
-      </c>
-      <c r="H1122" s="178"/>
-      <c r="I1122" s="178"/>
+      <c r="G1122" s="164" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1122" s="164"/>
+      <c r="I1122" s="164"/>
       <c r="J1122" s="147"/>
       <c r="K1122" s="147"/>
       <c r="L1122" s="147"/>
       <c r="M1122" s="147"/>
       <c r="N1122" s="147"/>
       <c r="O1122" s="147"/>
-      <c r="P1122" s="147"/>
-      <c r="Q1122" s="180"/>
+      <c r="P1122" s="147">
+        <v>1</v>
+      </c>
+      <c r="Q1122" s="166"/>
       <c r="R1122" s="147"/>
       <c r="S1122" s="147"/>
       <c r="T1122" s="147"/>
@@ -75371,9 +75574,11 @@
       <c r="CX1122" s="147"/>
       <c r="CY1122" s="147"/>
       <c r="CZ1122" s="147"/>
-      <c r="DA1122" s="147"/>
-      <c r="DB1122" s="181"/>
-      <c r="DC1122" s="181"/>
+      <c r="DA1122" s="147" t="s">
+        <v>2184</v>
+      </c>
+      <c r="DB1122" s="167"/>
+      <c r="DC1122" s="167"/>
       <c r="DD1122" s="147"/>
       <c r="DE1122" s="147"/>
       <c r="DF1122" s="147"/>
@@ -75421,12 +75626,12 @@
     <row r="1" spans="1:11">
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="177" t="s">
+      <c r="E1" s="182" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="177"/>
-      <c r="G1" s="177"/>
-      <c r="H1" s="177"/>
+      <c r="F1" s="182"/>
+      <c r="G1" s="182"/>
+      <c r="H1" s="182"/>
       <c r="I1" s="117"/>
     </row>
     <row r="2" spans="1:11" ht="45">
@@ -75747,11 +75952,11 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="C1" s="2"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="165"/>
-      <c r="F1" s="165"/>
-      <c r="G1" s="165"/>
-      <c r="H1" s="167"/>
+      <c r="D1" s="171"/>
+      <c r="E1" s="170"/>
+      <c r="F1" s="170"/>
+      <c r="G1" s="170"/>
+      <c r="H1" s="172"/>
       <c r="I1" s="156"/>
       <c r="J1" s="130"/>
     </row>
@@ -75938,15 +76143,15 @@
     <row r="1" spans="1:11" ht="26.25">
       <c r="C1" s="2"/>
       <c r="D1" s="85"/>
-      <c r="E1" s="171" t="s">
+      <c r="E1" s="176" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="171"/>
-      <c r="G1" s="171"/>
-      <c r="H1" s="171"/>
-      <c r="I1" s="171"/>
-      <c r="J1" s="171"/>
-      <c r="K1" s="171"/>
+      <c r="F1" s="176"/>
+      <c r="G1" s="176"/>
+      <c r="H1" s="176"/>
+      <c r="I1" s="176"/>
+      <c r="J1" s="176"/>
+      <c r="K1" s="176"/>
     </row>
     <row r="2" spans="1:11" ht="30">
       <c r="C2" s="98" t="s">
@@ -80655,24 +80860,24 @@
   <sheetData>
     <row r="1" spans="1:23" ht="15" customHeight="1">
       <c r="D1" s="96"/>
-      <c r="E1" s="165"/>
-      <c r="F1" s="165"/>
-      <c r="G1" s="165"/>
-      <c r="H1" s="165"/>
-      <c r="I1" s="165"/>
-      <c r="J1" s="165"/>
-      <c r="K1" s="165"/>
-      <c r="L1" s="165"/>
-      <c r="M1" s="165"/>
-      <c r="N1" s="165"/>
-      <c r="O1" s="165"/>
-      <c r="P1" s="165"/>
-      <c r="Q1" s="165"/>
-      <c r="R1" s="165"/>
-      <c r="S1" s="165"/>
-      <c r="T1" s="165"/>
-      <c r="U1" s="165"/>
-      <c r="V1" s="165"/>
+      <c r="E1" s="170"/>
+      <c r="F1" s="170"/>
+      <c r="G1" s="170"/>
+      <c r="H1" s="170"/>
+      <c r="I1" s="170"/>
+      <c r="J1" s="170"/>
+      <c r="K1" s="170"/>
+      <c r="L1" s="170"/>
+      <c r="M1" s="170"/>
+      <c r="N1" s="170"/>
+      <c r="O1" s="170"/>
+      <c r="P1" s="170"/>
+      <c r="Q1" s="170"/>
+      <c r="R1" s="170"/>
+      <c r="S1" s="170"/>
+      <c r="T1" s="170"/>
+      <c r="U1" s="170"/>
+      <c r="V1" s="170"/>
     </row>
     <row r="2" spans="1:23" ht="96" customHeight="1">
       <c r="A2" s="58"/>
@@ -81663,37 +81868,37 @@
     <row r="1" spans="1:33" ht="15" customHeight="1">
       <c r="A1" s="58"/>
       <c r="B1" s="59"/>
-      <c r="E1" s="166" t="s">
+      <c r="E1" s="171" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="165"/>
-      <c r="G1" s="165"/>
-      <c r="H1" s="165"/>
-      <c r="I1" s="165"/>
-      <c r="J1" s="165"/>
-      <c r="K1" s="165"/>
-      <c r="L1" s="165"/>
-      <c r="M1" s="165"/>
-      <c r="N1" s="165"/>
-      <c r="O1" s="165"/>
-      <c r="P1" s="165"/>
-      <c r="Q1" s="165"/>
-      <c r="R1" s="165"/>
-      <c r="S1" s="165"/>
-      <c r="T1" s="165"/>
-      <c r="U1" s="165"/>
-      <c r="V1" s="165"/>
-      <c r="W1" s="165"/>
-      <c r="X1" s="165"/>
-      <c r="Y1" s="165"/>
-      <c r="Z1" s="165"/>
-      <c r="AA1" s="165"/>
-      <c r="AB1" s="165"/>
-      <c r="AC1" s="165"/>
-      <c r="AD1" s="165"/>
-      <c r="AE1" s="165"/>
-      <c r="AF1" s="165"/>
-      <c r="AG1" s="165"/>
+      <c r="F1" s="170"/>
+      <c r="G1" s="170"/>
+      <c r="H1" s="170"/>
+      <c r="I1" s="170"/>
+      <c r="J1" s="170"/>
+      <c r="K1" s="170"/>
+      <c r="L1" s="170"/>
+      <c r="M1" s="170"/>
+      <c r="N1" s="170"/>
+      <c r="O1" s="170"/>
+      <c r="P1" s="170"/>
+      <c r="Q1" s="170"/>
+      <c r="R1" s="170"/>
+      <c r="S1" s="170"/>
+      <c r="T1" s="170"/>
+      <c r="U1" s="170"/>
+      <c r="V1" s="170"/>
+      <c r="W1" s="170"/>
+      <c r="X1" s="170"/>
+      <c r="Y1" s="170"/>
+      <c r="Z1" s="170"/>
+      <c r="AA1" s="170"/>
+      <c r="AB1" s="170"/>
+      <c r="AC1" s="170"/>
+      <c r="AD1" s="170"/>
+      <c r="AE1" s="170"/>
+      <c r="AF1" s="170"/>
+      <c r="AG1" s="170"/>
     </row>
     <row r="2" spans="1:33" ht="144" customHeight="1">
       <c r="C2" s="96" t="s">

</xml_diff>

<commit_message>
test mpaiing TL calibration hierarchy reversals can't figure out why it's failing
</commit_message>
<xml_diff>
--- a/resources/syst_review_single_table.xlsx
+++ b/resources/syst_review_single_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\AnacondaProjects\PhD\Semiology-Visualisation-Tool\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB539E17-9073-41F5-8F80-6B154FB267FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B182F0B1-B8F0-4C10-B006-F8C55E7B3AA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10501,10 +10501,10 @@
   <dimension ref="A1:DU1122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E1100" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="P1100" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D1124" sqref="D1124"/>
+      <selection pane="bottomRight" activeCell="R1123" sqref="R1123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -73108,7 +73108,9 @@
         <v>1</v>
       </c>
       <c r="Q1104" s="76"/>
-      <c r="R1104" s="36"/>
+      <c r="R1104" s="36">
+        <v>1</v>
+      </c>
       <c r="S1104" s="36">
         <v>1</v>
       </c>
@@ -73242,7 +73244,9 @@
         <v>1</v>
       </c>
       <c r="Q1105" s="76"/>
-      <c r="R1105" s="36"/>
+      <c r="R1105" s="36">
+        <v>1</v>
+      </c>
       <c r="S1105" s="36"/>
       <c r="T1105" s="36">
         <v>1</v>
@@ -73376,9 +73380,13 @@
         <v>1</v>
       </c>
       <c r="Q1106" s="76"/>
-      <c r="R1106" s="36"/>
+      <c r="R1106" s="36">
+        <v>1</v>
+      </c>
       <c r="S1106" s="36"/>
-      <c r="T1106" s="36"/>
+      <c r="T1106" s="36">
+        <v>1</v>
+      </c>
       <c r="U1106" s="36">
         <v>1</v>
       </c>
@@ -73510,10 +73518,16 @@
         <v>1</v>
       </c>
       <c r="Q1107" s="76"/>
-      <c r="R1107" s="36"/>
+      <c r="R1107" s="36">
+        <v>1</v>
+      </c>
       <c r="S1107" s="36"/>
-      <c r="T1107" s="36"/>
-      <c r="U1107" s="36"/>
+      <c r="T1107" s="36">
+        <v>1</v>
+      </c>
+      <c r="U1107" s="36">
+        <v>1</v>
+      </c>
       <c r="V1107" s="36">
         <v>1</v>
       </c>
@@ -73644,10 +73658,16 @@
         <v>1</v>
       </c>
       <c r="Q1108" s="76"/>
-      <c r="R1108" s="36"/>
+      <c r="R1108" s="36">
+        <v>1</v>
+      </c>
       <c r="S1108" s="36"/>
-      <c r="T1108" s="36"/>
-      <c r="U1108" s="36"/>
+      <c r="T1108" s="36">
+        <v>1</v>
+      </c>
+      <c r="U1108" s="36">
+        <v>1</v>
+      </c>
       <c r="V1108" s="36"/>
       <c r="W1108" s="36">
         <v>1</v>
@@ -73778,10 +73798,16 @@
         <v>1</v>
       </c>
       <c r="Q1109" s="76"/>
-      <c r="R1109" s="36"/>
+      <c r="R1109" s="36">
+        <v>1</v>
+      </c>
       <c r="S1109" s="36"/>
-      <c r="T1109" s="36"/>
-      <c r="U1109" s="36"/>
+      <c r="T1109" s="36">
+        <v>1</v>
+      </c>
+      <c r="U1109" s="36">
+        <v>1</v>
+      </c>
       <c r="V1109" s="36"/>
       <c r="W1109" s="36"/>
       <c r="X1109" s="36">
@@ -73912,9 +73938,13 @@
         <v>1</v>
       </c>
       <c r="Q1110" s="76"/>
-      <c r="R1110" s="36"/>
+      <c r="R1110" s="36">
+        <v>1</v>
+      </c>
       <c r="S1110" s="36"/>
-      <c r="T1110" s="36"/>
+      <c r="T1110" s="36">
+        <v>1</v>
+      </c>
       <c r="U1110" s="36"/>
       <c r="V1110" s="36"/>
       <c r="W1110" s="36"/>
@@ -74046,9 +74076,13 @@
         <v>1</v>
       </c>
       <c r="Q1111" s="76"/>
-      <c r="R1111" s="36"/>
+      <c r="R1111" s="36">
+        <v>1</v>
+      </c>
       <c r="S1111" s="36"/>
-      <c r="T1111" s="36"/>
+      <c r="T1111" s="36">
+        <v>1</v>
+      </c>
       <c r="U1111" s="36"/>
       <c r="V1111" s="36"/>
       <c r="W1111" s="36"/>
@@ -74180,7 +74214,9 @@
         <v>1</v>
       </c>
       <c r="Q1112" s="76"/>
-      <c r="R1112" s="36"/>
+      <c r="R1112" s="36">
+        <v>1</v>
+      </c>
       <c r="S1112" s="36"/>
       <c r="T1112" s="36"/>
       <c r="U1112" s="36"/>
@@ -74314,7 +74350,9 @@
         <v>1</v>
       </c>
       <c r="Q1113" s="76"/>
-      <c r="R1113" s="36"/>
+      <c r="R1113" s="36">
+        <v>1</v>
+      </c>
       <c r="S1113" s="36"/>
       <c r="T1113" s="36"/>
       <c r="U1113" s="36"/>
@@ -74323,7 +74361,9 @@
       <c r="X1113" s="36"/>
       <c r="Y1113" s="36"/>
       <c r="Z1113" s="36"/>
-      <c r="AA1113" s="36"/>
+      <c r="AA1113" s="36">
+        <v>1</v>
+      </c>
       <c r="AB1113" s="36">
         <v>1</v>
       </c>
@@ -74448,7 +74488,9 @@
         <v>1</v>
       </c>
       <c r="Q1114" s="76"/>
-      <c r="R1114" s="36"/>
+      <c r="R1114" s="36">
+        <v>1</v>
+      </c>
       <c r="S1114" s="36"/>
       <c r="T1114" s="36"/>
       <c r="U1114" s="36"/>
@@ -74457,7 +74499,9 @@
       <c r="X1114" s="36"/>
       <c r="Y1114" s="36"/>
       <c r="Z1114" s="36"/>
-      <c r="AA1114" s="36"/>
+      <c r="AA1114" s="36">
+        <v>1</v>
+      </c>
       <c r="AB1114" s="36"/>
       <c r="AC1114" s="36">
         <v>1</v>
@@ -74582,7 +74626,9 @@
         <v>1</v>
       </c>
       <c r="Q1115" s="76"/>
-      <c r="R1115" s="36"/>
+      <c r="R1115" s="36">
+        <v>1</v>
+      </c>
       <c r="S1115" s="36"/>
       <c r="T1115" s="36"/>
       <c r="U1115" s="36"/>
@@ -74591,7 +74637,9 @@
       <c r="X1115" s="36"/>
       <c r="Y1115" s="36"/>
       <c r="Z1115" s="36"/>
-      <c r="AA1115" s="36"/>
+      <c r="AA1115" s="36">
+        <v>1</v>
+      </c>
       <c r="AB1115" s="36"/>
       <c r="AC1115" s="36"/>
       <c r="AD1115" s="36">
@@ -74716,7 +74764,9 @@
         <v>1</v>
       </c>
       <c r="Q1116" s="76"/>
-      <c r="R1116" s="36"/>
+      <c r="R1116" s="36">
+        <v>1</v>
+      </c>
       <c r="S1116" s="36"/>
       <c r="T1116" s="36"/>
       <c r="U1116" s="36"/>
@@ -74725,7 +74775,9 @@
       <c r="X1116" s="36"/>
       <c r="Y1116" s="36"/>
       <c r="Z1116" s="36"/>
-      <c r="AA1116" s="36"/>
+      <c r="AA1116" s="36">
+        <v>1</v>
+      </c>
       <c r="AB1116" s="36"/>
       <c r="AC1116" s="36"/>
       <c r="AD1116" s="36"/>
@@ -74850,7 +74902,9 @@
         <v>1</v>
       </c>
       <c r="Q1117" s="76"/>
-      <c r="R1117" s="36"/>
+      <c r="R1117" s="36">
+        <v>1</v>
+      </c>
       <c r="S1117" s="36"/>
       <c r="T1117" s="36"/>
       <c r="U1117" s="36"/>
@@ -74859,7 +74913,9 @@
       <c r="X1117" s="36"/>
       <c r="Y1117" s="36"/>
       <c r="Z1117" s="36"/>
-      <c r="AA1117" s="36"/>
+      <c r="AA1117" s="36">
+        <v>1</v>
+      </c>
       <c r="AB1117" s="36"/>
       <c r="AC1117" s="36"/>
       <c r="AD1117" s="36"/>
@@ -74984,7 +75040,9 @@
         <v>1</v>
       </c>
       <c r="Q1118" s="76"/>
-      <c r="R1118" s="36"/>
+      <c r="R1118" s="36">
+        <v>1</v>
+      </c>
       <c r="S1118" s="36"/>
       <c r="T1118" s="36"/>
       <c r="U1118" s="36"/>
@@ -74993,7 +75051,9 @@
       <c r="X1118" s="36"/>
       <c r="Y1118" s="36"/>
       <c r="Z1118" s="36"/>
-      <c r="AA1118" s="36"/>
+      <c r="AA1118" s="36">
+        <v>1</v>
+      </c>
       <c r="AB1118" s="36"/>
       <c r="AC1118" s="36"/>
       <c r="AD1118" s="36"/>
@@ -75118,7 +75178,9 @@
         <v>1</v>
       </c>
       <c r="Q1119" s="76"/>
-      <c r="R1119" s="36"/>
+      <c r="R1119" s="36">
+        <v>1</v>
+      </c>
       <c r="S1119" s="36"/>
       <c r="T1119" s="36"/>
       <c r="U1119" s="36"/>
@@ -75127,7 +75189,9 @@
       <c r="X1119" s="36"/>
       <c r="Y1119" s="36"/>
       <c r="Z1119" s="36"/>
-      <c r="AA1119" s="36"/>
+      <c r="AA1119" s="36">
+        <v>1</v>
+      </c>
       <c r="AB1119" s="36"/>
       <c r="AC1119" s="36"/>
       <c r="AD1119" s="36"/>
@@ -75252,7 +75316,9 @@
         <v>1</v>
       </c>
       <c r="Q1120" s="76"/>
-      <c r="R1120" s="36"/>
+      <c r="R1120" s="36">
+        <v>1</v>
+      </c>
       <c r="S1120" s="36"/>
       <c r="T1120" s="36"/>
       <c r="U1120" s="36"/>
@@ -75386,7 +75452,9 @@
         <v>1</v>
       </c>
       <c r="Q1121" s="76"/>
-      <c r="R1121" s="36"/>
+      <c r="R1121" s="36">
+        <v>1</v>
+      </c>
       <c r="S1121" s="36"/>
       <c r="T1121" s="36"/>
       <c r="U1121" s="36"/>
@@ -75520,7 +75588,9 @@
         <v>1</v>
       </c>
       <c r="Q1122" s="76"/>
-      <c r="R1122" s="36"/>
+      <c r="R1122" s="36">
+        <v>1</v>
+      </c>
       <c r="S1122" s="36"/>
       <c r="T1122" s="36"/>
       <c r="U1122" s="36"/>
@@ -75538,7 +75608,9 @@
       <c r="AG1122" s="36"/>
       <c r="AH1122" s="36"/>
       <c r="AI1122" s="36"/>
-      <c r="AJ1122" s="36"/>
+      <c r="AJ1122" s="36">
+        <v>1</v>
+      </c>
       <c r="AK1122" s="36">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
test MappingsCalibration (mappings TLs) Hierarchy Reversals (#138)
* test mpaiing TL calibration hierarchy reversals
can't figure out why it's failing

* fixed call to MEGA_ANALYSIS

* testing expanded: calibration hierarchy reversal
tests the mappings TLs for hierarchy reversal

* test complete
</commit_message>
<xml_diff>
--- a/resources/syst_review_single_table.xlsx
+++ b/resources/syst_review_single_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\AnacondaProjects\PhD\Semiology-Visualisation-Tool\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB539E17-9073-41F5-8F80-6B154FB267FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B182F0B1-B8F0-4C10-B006-F8C55E7B3AA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10501,10 +10501,10 @@
   <dimension ref="A1:DU1122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E1100" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="P1100" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D1124" sqref="D1124"/>
+      <selection pane="bottomRight" activeCell="R1123" sqref="R1123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -73108,7 +73108,9 @@
         <v>1</v>
       </c>
       <c r="Q1104" s="76"/>
-      <c r="R1104" s="36"/>
+      <c r="R1104" s="36">
+        <v>1</v>
+      </c>
       <c r="S1104" s="36">
         <v>1</v>
       </c>
@@ -73242,7 +73244,9 @@
         <v>1</v>
       </c>
       <c r="Q1105" s="76"/>
-      <c r="R1105" s="36"/>
+      <c r="R1105" s="36">
+        <v>1</v>
+      </c>
       <c r="S1105" s="36"/>
       <c r="T1105" s="36">
         <v>1</v>
@@ -73376,9 +73380,13 @@
         <v>1</v>
       </c>
       <c r="Q1106" s="76"/>
-      <c r="R1106" s="36"/>
+      <c r="R1106" s="36">
+        <v>1</v>
+      </c>
       <c r="S1106" s="36"/>
-      <c r="T1106" s="36"/>
+      <c r="T1106" s="36">
+        <v>1</v>
+      </c>
       <c r="U1106" s="36">
         <v>1</v>
       </c>
@@ -73510,10 +73518,16 @@
         <v>1</v>
       </c>
       <c r="Q1107" s="76"/>
-      <c r="R1107" s="36"/>
+      <c r="R1107" s="36">
+        <v>1</v>
+      </c>
       <c r="S1107" s="36"/>
-      <c r="T1107" s="36"/>
-      <c r="U1107" s="36"/>
+      <c r="T1107" s="36">
+        <v>1</v>
+      </c>
+      <c r="U1107" s="36">
+        <v>1</v>
+      </c>
       <c r="V1107" s="36">
         <v>1</v>
       </c>
@@ -73644,10 +73658,16 @@
         <v>1</v>
       </c>
       <c r="Q1108" s="76"/>
-      <c r="R1108" s="36"/>
+      <c r="R1108" s="36">
+        <v>1</v>
+      </c>
       <c r="S1108" s="36"/>
-      <c r="T1108" s="36"/>
-      <c r="U1108" s="36"/>
+      <c r="T1108" s="36">
+        <v>1</v>
+      </c>
+      <c r="U1108" s="36">
+        <v>1</v>
+      </c>
       <c r="V1108" s="36"/>
       <c r="W1108" s="36">
         <v>1</v>
@@ -73778,10 +73798,16 @@
         <v>1</v>
       </c>
       <c r="Q1109" s="76"/>
-      <c r="R1109" s="36"/>
+      <c r="R1109" s="36">
+        <v>1</v>
+      </c>
       <c r="S1109" s="36"/>
-      <c r="T1109" s="36"/>
-      <c r="U1109" s="36"/>
+      <c r="T1109" s="36">
+        <v>1</v>
+      </c>
+      <c r="U1109" s="36">
+        <v>1</v>
+      </c>
       <c r="V1109" s="36"/>
       <c r="W1109" s="36"/>
       <c r="X1109" s="36">
@@ -73912,9 +73938,13 @@
         <v>1</v>
       </c>
       <c r="Q1110" s="76"/>
-      <c r="R1110" s="36"/>
+      <c r="R1110" s="36">
+        <v>1</v>
+      </c>
       <c r="S1110" s="36"/>
-      <c r="T1110" s="36"/>
+      <c r="T1110" s="36">
+        <v>1</v>
+      </c>
       <c r="U1110" s="36"/>
       <c r="V1110" s="36"/>
       <c r="W1110" s="36"/>
@@ -74046,9 +74076,13 @@
         <v>1</v>
       </c>
       <c r="Q1111" s="76"/>
-      <c r="R1111" s="36"/>
+      <c r="R1111" s="36">
+        <v>1</v>
+      </c>
       <c r="S1111" s="36"/>
-      <c r="T1111" s="36"/>
+      <c r="T1111" s="36">
+        <v>1</v>
+      </c>
       <c r="U1111" s="36"/>
       <c r="V1111" s="36"/>
       <c r="W1111" s="36"/>
@@ -74180,7 +74214,9 @@
         <v>1</v>
       </c>
       <c r="Q1112" s="76"/>
-      <c r="R1112" s="36"/>
+      <c r="R1112" s="36">
+        <v>1</v>
+      </c>
       <c r="S1112" s="36"/>
       <c r="T1112" s="36"/>
       <c r="U1112" s="36"/>
@@ -74314,7 +74350,9 @@
         <v>1</v>
       </c>
       <c r="Q1113" s="76"/>
-      <c r="R1113" s="36"/>
+      <c r="R1113" s="36">
+        <v>1</v>
+      </c>
       <c r="S1113" s="36"/>
       <c r="T1113" s="36"/>
       <c r="U1113" s="36"/>
@@ -74323,7 +74361,9 @@
       <c r="X1113" s="36"/>
       <c r="Y1113" s="36"/>
       <c r="Z1113" s="36"/>
-      <c r="AA1113" s="36"/>
+      <c r="AA1113" s="36">
+        <v>1</v>
+      </c>
       <c r="AB1113" s="36">
         <v>1</v>
       </c>
@@ -74448,7 +74488,9 @@
         <v>1</v>
       </c>
       <c r="Q1114" s="76"/>
-      <c r="R1114" s="36"/>
+      <c r="R1114" s="36">
+        <v>1</v>
+      </c>
       <c r="S1114" s="36"/>
       <c r="T1114" s="36"/>
       <c r="U1114" s="36"/>
@@ -74457,7 +74499,9 @@
       <c r="X1114" s="36"/>
       <c r="Y1114" s="36"/>
       <c r="Z1114" s="36"/>
-      <c r="AA1114" s="36"/>
+      <c r="AA1114" s="36">
+        <v>1</v>
+      </c>
       <c r="AB1114" s="36"/>
       <c r="AC1114" s="36">
         <v>1</v>
@@ -74582,7 +74626,9 @@
         <v>1</v>
       </c>
       <c r="Q1115" s="76"/>
-      <c r="R1115" s="36"/>
+      <c r="R1115" s="36">
+        <v>1</v>
+      </c>
       <c r="S1115" s="36"/>
       <c r="T1115" s="36"/>
       <c r="U1115" s="36"/>
@@ -74591,7 +74637,9 @@
       <c r="X1115" s="36"/>
       <c r="Y1115" s="36"/>
       <c r="Z1115" s="36"/>
-      <c r="AA1115" s="36"/>
+      <c r="AA1115" s="36">
+        <v>1</v>
+      </c>
       <c r="AB1115" s="36"/>
       <c r="AC1115" s="36"/>
       <c r="AD1115" s="36">
@@ -74716,7 +74764,9 @@
         <v>1</v>
       </c>
       <c r="Q1116" s="76"/>
-      <c r="R1116" s="36"/>
+      <c r="R1116" s="36">
+        <v>1</v>
+      </c>
       <c r="S1116" s="36"/>
       <c r="T1116" s="36"/>
       <c r="U1116" s="36"/>
@@ -74725,7 +74775,9 @@
       <c r="X1116" s="36"/>
       <c r="Y1116" s="36"/>
       <c r="Z1116" s="36"/>
-      <c r="AA1116" s="36"/>
+      <c r="AA1116" s="36">
+        <v>1</v>
+      </c>
       <c r="AB1116" s="36"/>
       <c r="AC1116" s="36"/>
       <c r="AD1116" s="36"/>
@@ -74850,7 +74902,9 @@
         <v>1</v>
       </c>
       <c r="Q1117" s="76"/>
-      <c r="R1117" s="36"/>
+      <c r="R1117" s="36">
+        <v>1</v>
+      </c>
       <c r="S1117" s="36"/>
       <c r="T1117" s="36"/>
       <c r="U1117" s="36"/>
@@ -74859,7 +74913,9 @@
       <c r="X1117" s="36"/>
       <c r="Y1117" s="36"/>
       <c r="Z1117" s="36"/>
-      <c r="AA1117" s="36"/>
+      <c r="AA1117" s="36">
+        <v>1</v>
+      </c>
       <c r="AB1117" s="36"/>
       <c r="AC1117" s="36"/>
       <c r="AD1117" s="36"/>
@@ -74984,7 +75040,9 @@
         <v>1</v>
       </c>
       <c r="Q1118" s="76"/>
-      <c r="R1118" s="36"/>
+      <c r="R1118" s="36">
+        <v>1</v>
+      </c>
       <c r="S1118" s="36"/>
       <c r="T1118" s="36"/>
       <c r="U1118" s="36"/>
@@ -74993,7 +75051,9 @@
       <c r="X1118" s="36"/>
       <c r="Y1118" s="36"/>
       <c r="Z1118" s="36"/>
-      <c r="AA1118" s="36"/>
+      <c r="AA1118" s="36">
+        <v>1</v>
+      </c>
       <c r="AB1118" s="36"/>
       <c r="AC1118" s="36"/>
       <c r="AD1118" s="36"/>
@@ -75118,7 +75178,9 @@
         <v>1</v>
       </c>
       <c r="Q1119" s="76"/>
-      <c r="R1119" s="36"/>
+      <c r="R1119" s="36">
+        <v>1</v>
+      </c>
       <c r="S1119" s="36"/>
       <c r="T1119" s="36"/>
       <c r="U1119" s="36"/>
@@ -75127,7 +75189,9 @@
       <c r="X1119" s="36"/>
       <c r="Y1119" s="36"/>
       <c r="Z1119" s="36"/>
-      <c r="AA1119" s="36"/>
+      <c r="AA1119" s="36">
+        <v>1</v>
+      </c>
       <c r="AB1119" s="36"/>
       <c r="AC1119" s="36"/>
       <c r="AD1119" s="36"/>
@@ -75252,7 +75316,9 @@
         <v>1</v>
       </c>
       <c r="Q1120" s="76"/>
-      <c r="R1120" s="36"/>
+      <c r="R1120" s="36">
+        <v>1</v>
+      </c>
       <c r="S1120" s="36"/>
       <c r="T1120" s="36"/>
       <c r="U1120" s="36"/>
@@ -75386,7 +75452,9 @@
         <v>1</v>
       </c>
       <c r="Q1121" s="76"/>
-      <c r="R1121" s="36"/>
+      <c r="R1121" s="36">
+        <v>1</v>
+      </c>
       <c r="S1121" s="36"/>
       <c r="T1121" s="36"/>
       <c r="U1121" s="36"/>
@@ -75520,7 +75588,9 @@
         <v>1</v>
       </c>
       <c r="Q1122" s="76"/>
-      <c r="R1122" s="36"/>
+      <c r="R1122" s="36">
+        <v>1</v>
+      </c>
       <c r="S1122" s="36"/>
       <c r="T1122" s="36"/>
       <c r="U1122" s="36"/>
@@ -75538,7 +75608,9 @@
       <c r="AG1122" s="36"/>
       <c r="AH1122" s="36"/>
       <c r="AI1122" s="36"/>
-      <c r="AJ1122" s="36"/>
+      <c r="AJ1122" s="36">
+        <v>1</v>
+      </c>
       <c r="AK1122" s="36">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
homogenise resources references dummy data, beta data homogenise paeds and Other Abs cols names
</commit_message>
<xml_diff>
--- a/resources/syst_review_single_table.xlsx
+++ b/resources/syst_review_single_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\AnacondaProjects\PhD\Semiology-Visualisation-Tool\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1571DDC-2AD5-4404-82F6-1002235388B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BDC4021-C295-4977-AB69-6BE9926341A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6831,10 +6831,10 @@
     <t>mappings TLt</t>
   </si>
   <si>
-    <t>Other factors (e.g. Abs, genetic mutations)</t>
-  </si>
-  <si>
     <t>paediatric subgroup &lt;7 years (0-6 yrs) y/n</t>
+  </si>
+  <si>
+    <t>Other factors (e.g. Abs, genetic mutations)</t>
   </si>
 </sst>
 </file>
@@ -7414,7 +7414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="180">
+  <cellXfs count="179">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -7917,9 +7917,6 @@
     </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -10513,10 +10510,10 @@
   <dimension ref="A1:DU1122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="P3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="DA3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomRight" activeCell="DH2" sqref="DH2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -11041,7 +11038,7 @@
         <v>107</v>
       </c>
       <c r="DA2" s="151" t="s">
-        <v>2186</v>
+        <v>2185</v>
       </c>
       <c r="DB2" s="49" t="s">
         <v>108</v>
@@ -11061,8 +11058,8 @@
       <c r="DG2" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="DH2" s="179" t="s">
-        <v>2185</v>
+      <c r="DH2" s="13" t="s">
+        <v>2186</v>
       </c>
       <c r="DI2" s="12"/>
       <c r="DJ2" s="12"/>

</xml_diff>

<commit_message>
GIF MIXED sheet aded. Now pytest runs fails 4.
</commit_message>
<xml_diff>
--- a/resources/syst_review_single_table.xlsx
+++ b/resources/syst_review_single_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\AnacondaProjects\PhD\Semiology-Visualisation-Tool\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BDC4021-C295-4977-AB69-6BE9926341A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20176B2D-2090-40C8-AAF9-B0AD68A50498}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,7 @@
     <sheet name="GIF INSULA" sheetId="10" r:id="rId12"/>
     <sheet name="GIF HYPOTHALAMUS" sheetId="14" r:id="rId13"/>
     <sheet name="GIF CEREBELLUM" sheetId="13" r:id="rId14"/>
+    <sheet name="GIF MIXED" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -10509,11 +10510,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DU1122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="DA3" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="DH2" sqref="DH2"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -76652,6 +76653,20 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0704BAC9-76B6-477C-9CC6-23221501A352}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U12" sqref="U12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M29"/>

</xml_diff>

<commit_message>
formatting of paed col name
</commit_message>
<xml_diff>
--- a/resources/syst_review_single_table.xlsx
+++ b/resources/syst_review_single_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\AnacondaProjects\PhD\Semiology-Visualisation-Tool\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20176B2D-2090-40C8-AAF9-B0AD68A50498}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45BC3C8-BE86-4570-B58C-9FFD95D35D1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -6832,10 +6832,10 @@
     <t>mappings TLt</t>
   </si>
   <si>
-    <t>paediatric subgroup &lt;7 years (0-6 yrs) y/n</t>
-  </si>
-  <si>
     <t>Other factors (e.g. Abs, genetic mutations)</t>
+  </si>
+  <si>
+    <t>paediatric subgroup &lt;7 years (0-6 yrs) y/n</t>
   </si>
 </sst>
 </file>
@@ -10510,11 +10510,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DU1122"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="CW3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomRight" activeCell="DA2" sqref="DA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -11039,7 +11039,7 @@
         <v>107</v>
       </c>
       <c r="DA2" s="151" t="s">
-        <v>2185</v>
+        <v>2186</v>
       </c>
       <c r="DB2" s="49" t="s">
         <v>108</v>
@@ -11060,7 +11060,7 @@
         <v>113</v>
       </c>
       <c r="DH2" s="13" t="s">
-        <v>2186</v>
+        <v>2185</v>
       </c>
       <c r="DI2" s="12"/>
       <c r="DJ2" s="12"/>
@@ -76657,7 +76657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0704BAC9-76B6-477C-9CC6-23221501A352}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U12" sqref="U12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
removed duplicated Full GIF Map for Review GIFs gif #s: 24, 37, 39, 43, 56, 58, 60, 62, 76, 77, 96 and left equivalents
</commit_message>
<xml_diff>
--- a/resources/syst_review_single_table.xlsx
+++ b/resources/syst_review_single_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\AnacondaProjects\PhD\Semiology-Visualisation-Tool\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45BC3C8-BE86-4570-B58C-9FFD95D35D1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92CF69AB-6037-48A4-BA0A-B3C34DA1B3B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -30,14 +30,6 @@
     <sheet name="GIF MIXED" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -127,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7100" uniqueCount="2187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7080" uniqueCount="2187">
   <si>
     <t xml:space="preserve">Semiology </t>
   </si>
@@ -7874,6 +7866,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -7915,9 +7910,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -10510,7 +10502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DU1122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="CW3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -10606,106 +10598,106 @@
     <row r="1" spans="1:125" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1">
       <c r="A1" s="155"/>
       <c r="C1" s="17"/>
-      <c r="D1" s="164" t="s">
+      <c r="D1" s="165" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="164"/>
-      <c r="G1" s="172" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="173"/>
-      <c r="I1" s="173"/>
-      <c r="K1" s="174" t="s">
+      <c r="E1" s="165"/>
+      <c r="G1" s="173" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="174"/>
+      <c r="I1" s="174"/>
+      <c r="K1" s="175" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="175"/>
-      <c r="M1" s="175"/>
-      <c r="N1" s="175"/>
-      <c r="O1" s="176"/>
-      <c r="S1" s="165"/>
-      <c r="T1" s="165"/>
-      <c r="U1" s="165"/>
-      <c r="V1" s="165"/>
-      <c r="W1" s="165"/>
-      <c r="X1" s="165"/>
-      <c r="Y1" s="165"/>
-      <c r="Z1" s="165"/>
-      <c r="AA1" s="165"/>
-      <c r="AB1" s="165"/>
-      <c r="AC1" s="165"/>
-      <c r="AD1" s="165"/>
-      <c r="AE1" s="165"/>
-      <c r="AF1" s="165"/>
-      <c r="AG1" s="165"/>
-      <c r="AH1" s="165"/>
-      <c r="AI1" s="165"/>
-      <c r="AJ1" s="165"/>
-      <c r="AK1" s="165"/>
+      <c r="L1" s="176"/>
+      <c r="M1" s="176"/>
+      <c r="N1" s="176"/>
+      <c r="O1" s="177"/>
+      <c r="S1" s="166"/>
+      <c r="T1" s="166"/>
+      <c r="U1" s="166"/>
+      <c r="V1" s="166"/>
+      <c r="W1" s="166"/>
+      <c r="X1" s="166"/>
+      <c r="Y1" s="166"/>
+      <c r="Z1" s="166"/>
+      <c r="AA1" s="166"/>
+      <c r="AB1" s="166"/>
+      <c r="AC1" s="166"/>
+      <c r="AD1" s="166"/>
+      <c r="AE1" s="166"/>
+      <c r="AF1" s="166"/>
+      <c r="AG1" s="166"/>
+      <c r="AH1" s="166"/>
+      <c r="AI1" s="166"/>
+      <c r="AJ1" s="166"/>
+      <c r="AK1" s="166"/>
       <c r="AM1" s="153"/>
-      <c r="AN1" s="166" t="s">
+      <c r="AN1" s="167" t="s">
         <v>3</v>
       </c>
-      <c r="AO1" s="165"/>
-      <c r="AP1" s="165"/>
-      <c r="AQ1" s="165"/>
-      <c r="AR1" s="165"/>
-      <c r="AS1" s="165"/>
-      <c r="AT1" s="165"/>
-      <c r="AU1" s="165"/>
-      <c r="AV1" s="165"/>
-      <c r="AW1" s="165"/>
-      <c r="AX1" s="165"/>
-      <c r="AY1" s="165"/>
-      <c r="AZ1" s="165"/>
-      <c r="BA1" s="165"/>
-      <c r="BB1" s="165"/>
-      <c r="BC1" s="165"/>
-      <c r="BD1" s="165"/>
-      <c r="BE1" s="165"/>
-      <c r="BF1" s="165"/>
-      <c r="BG1" s="165"/>
-      <c r="BH1" s="165"/>
-      <c r="BI1" s="165"/>
-      <c r="BJ1" s="165"/>
-      <c r="BK1" s="165"/>
-      <c r="BL1" s="165"/>
-      <c r="BM1" s="165"/>
-      <c r="BN1" s="165"/>
-      <c r="BO1" s="165"/>
-      <c r="BP1" s="165"/>
-      <c r="BR1" s="168"/>
-      <c r="BS1" s="169"/>
-      <c r="BT1" s="169"/>
-      <c r="BU1" s="169"/>
-      <c r="BV1" s="169"/>
-      <c r="BW1" s="170"/>
+      <c r="AO1" s="166"/>
+      <c r="AP1" s="166"/>
+      <c r="AQ1" s="166"/>
+      <c r="AR1" s="166"/>
+      <c r="AS1" s="166"/>
+      <c r="AT1" s="166"/>
+      <c r="AU1" s="166"/>
+      <c r="AV1" s="166"/>
+      <c r="AW1" s="166"/>
+      <c r="AX1" s="166"/>
+      <c r="AY1" s="166"/>
+      <c r="AZ1" s="166"/>
+      <c r="BA1" s="166"/>
+      <c r="BB1" s="166"/>
+      <c r="BC1" s="166"/>
+      <c r="BD1" s="166"/>
+      <c r="BE1" s="166"/>
+      <c r="BF1" s="166"/>
+      <c r="BG1" s="166"/>
+      <c r="BH1" s="166"/>
+      <c r="BI1" s="166"/>
+      <c r="BJ1" s="166"/>
+      <c r="BK1" s="166"/>
+      <c r="BL1" s="166"/>
+      <c r="BM1" s="166"/>
+      <c r="BN1" s="166"/>
+      <c r="BO1" s="166"/>
+      <c r="BP1" s="166"/>
+      <c r="BR1" s="169"/>
+      <c r="BS1" s="170"/>
+      <c r="BT1" s="170"/>
+      <c r="BU1" s="170"/>
+      <c r="BV1" s="170"/>
+      <c r="BW1" s="171"/>
       <c r="BX1" s="156"/>
-      <c r="BZ1" s="165"/>
-      <c r="CA1" s="165"/>
-      <c r="CB1" s="165"/>
-      <c r="CC1" s="165"/>
-      <c r="CD1" s="165"/>
-      <c r="CE1" s="165"/>
-      <c r="CF1" s="165"/>
-      <c r="CG1" s="167"/>
-      <c r="CH1" s="166" t="s">
+      <c r="BZ1" s="166"/>
+      <c r="CA1" s="166"/>
+      <c r="CB1" s="166"/>
+      <c r="CC1" s="166"/>
+      <c r="CD1" s="166"/>
+      <c r="CE1" s="166"/>
+      <c r="CF1" s="166"/>
+      <c r="CG1" s="168"/>
+      <c r="CH1" s="167" t="s">
         <v>4</v>
       </c>
-      <c r="CI1" s="165"/>
-      <c r="CJ1" s="165"/>
-      <c r="CK1" s="165"/>
-      <c r="CL1" s="165"/>
-      <c r="CM1" s="167"/>
+      <c r="CI1" s="166"/>
+      <c r="CJ1" s="166"/>
+      <c r="CK1" s="166"/>
+      <c r="CL1" s="166"/>
+      <c r="CM1" s="168"/>
       <c r="CO1" s="85"/>
-      <c r="CP1" s="171" t="s">
+      <c r="CP1" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="CQ1" s="171"/>
-      <c r="CR1" s="171"/>
-      <c r="CS1" s="171"/>
-      <c r="CT1" s="171"/>
-      <c r="CU1" s="171"/>
-      <c r="CV1" s="171"/>
+      <c r="CQ1" s="172"/>
+      <c r="CR1" s="172"/>
+      <c r="CS1" s="172"/>
+      <c r="CT1" s="172"/>
+      <c r="CU1" s="172"/>
+      <c r="CV1" s="172"/>
       <c r="CX1" s="140"/>
       <c r="CY1" s="140"/>
       <c r="CZ1" s="140"/>
@@ -11107,7 +11099,7 @@
       <c r="CT3" s="5">
         <v>1</v>
       </c>
-      <c r="DA3" s="178"/>
+      <c r="DA3" s="164"/>
       <c r="DB3" s="6">
         <v>25</v>
       </c>
@@ -75746,12 +75738,12 @@
     <row r="1" spans="1:11">
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="177" t="s">
+      <c r="E1" s="178" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="177"/>
-      <c r="G1" s="177"/>
-      <c r="H1" s="177"/>
+      <c r="F1" s="178"/>
+      <c r="G1" s="178"/>
+      <c r="H1" s="178"/>
       <c r="I1" s="117"/>
     </row>
     <row r="2" spans="1:11" ht="45">
@@ -76072,11 +76064,11 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="C1" s="2"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="165"/>
-      <c r="F1" s="165"/>
-      <c r="G1" s="165"/>
-      <c r="H1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="166"/>
+      <c r="F1" s="166"/>
+      <c r="G1" s="166"/>
+      <c r="H1" s="168"/>
       <c r="I1" s="156"/>
       <c r="J1" s="130"/>
     </row>
@@ -76263,15 +76255,15 @@
     <row r="1" spans="1:11" ht="26.25">
       <c r="C1" s="2"/>
       <c r="D1" s="85"/>
-      <c r="E1" s="171" t="s">
+      <c r="E1" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="171"/>
-      <c r="G1" s="171"/>
-      <c r="H1" s="171"/>
-      <c r="I1" s="171"/>
-      <c r="J1" s="171"/>
-      <c r="K1" s="171"/>
+      <c r="F1" s="172"/>
+      <c r="G1" s="172"/>
+      <c r="H1" s="172"/>
+      <c r="I1" s="172"/>
+      <c r="J1" s="172"/>
+      <c r="K1" s="172"/>
     </row>
     <row r="2" spans="1:11" ht="30">
       <c r="C2" s="98" t="s">
@@ -77826,10 +77818,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D189"/>
+  <dimension ref="A1:D169"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="A170" sqref="A170:XFD173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -79151,210 +79143,50 @@
     </row>
     <row r="164" spans="1:4">
       <c r="A164" s="115" t="s">
-        <v>1993</v>
-      </c>
-      <c r="C164" s="53">
-        <v>24</v>
+        <v>1997</v>
+      </c>
+      <c r="B164" s="53">
+        <v>35</v>
       </c>
     </row>
     <row r="165" spans="1:4">
       <c r="A165" s="115" t="s">
-        <v>1994</v>
-      </c>
-      <c r="D165" s="53">
-        <v>31</v>
+        <v>1998</v>
+      </c>
+      <c r="B165" s="53">
+        <v>36</v>
       </c>
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="115" t="s">
-        <v>1997</v>
+        <v>2029</v>
       </c>
       <c r="B166" s="53">
-        <v>35</v>
+        <v>72</v>
       </c>
     </row>
     <row r="167" spans="1:4">
       <c r="A167" s="115" t="s">
-        <v>1998</v>
+        <v>2030</v>
       </c>
       <c r="B167" s="53">
-        <v>36</v>
+        <v>73</v>
       </c>
     </row>
     <row r="168" spans="1:4">
       <c r="A168" s="115" t="s">
-        <v>1999</v>
-      </c>
-      <c r="C168" s="53">
-        <v>37</v>
+        <v>2031</v>
+      </c>
+      <c r="B168" s="53">
+        <v>74</v>
       </c>
     </row>
     <row r="169" spans="1:4">
       <c r="A169" s="115" t="s">
-        <v>2000</v>
-      </c>
-      <c r="D169" s="53">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4">
-      <c r="A170" s="115" t="s">
-        <v>2001</v>
-      </c>
-      <c r="C170" s="53">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4">
-      <c r="A171" s="115" t="s">
-        <v>2002</v>
-      </c>
-      <c r="D171" s="53">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4">
-      <c r="A172" s="115" t="s">
-        <v>2005</v>
-      </c>
-      <c r="C172" s="53">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4">
-      <c r="A173" s="115" t="s">
-        <v>2006</v>
-      </c>
-      <c r="D173" s="53">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4">
-      <c r="A174" s="115" t="s">
-        <v>2016</v>
-      </c>
-      <c r="C174" s="53">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4">
-      <c r="A175" s="115" t="s">
-        <v>2017</v>
-      </c>
-      <c r="D175" s="53">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4">
-      <c r="A176" s="115" t="s">
-        <v>2018</v>
-      </c>
-      <c r="C176" s="53">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4">
-      <c r="A177" s="115" t="s">
-        <v>2019</v>
-      </c>
-      <c r="D177" s="53">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4">
-      <c r="A178" s="115" t="s">
-        <v>2020</v>
-      </c>
-      <c r="C178" s="53">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4">
-      <c r="A179" s="115" t="s">
-        <v>2021</v>
-      </c>
-      <c r="D179" s="53">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4">
-      <c r="A180" s="115" t="s">
-        <v>2022</v>
-      </c>
-      <c r="C180" s="53">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4">
-      <c r="A181" s="115" t="s">
-        <v>2023</v>
-      </c>
-      <c r="D181" s="53">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4">
-      <c r="A182" s="115" t="s">
-        <v>2029</v>
-      </c>
-      <c r="B182" s="53">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4">
-      <c r="A183" s="115" t="s">
-        <v>2030</v>
-      </c>
-      <c r="B183" s="53">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4">
-      <c r="A184" s="115" t="s">
-        <v>2031</v>
-      </c>
-      <c r="B184" s="53">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4">
-      <c r="A185" s="115" t="s">
         <v>2040</v>
       </c>
-      <c r="B185" s="53">
+      <c r="B169" s="53">
         <v>87</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4">
-      <c r="A186" s="115" t="s">
-        <v>2047</v>
-      </c>
-      <c r="C186" s="53">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4">
-      <c r="A187" s="115" t="s">
-        <v>2048</v>
-      </c>
-      <c r="D187" s="53">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4">
-      <c r="A188" s="115" t="s">
-        <v>2147</v>
-      </c>
-      <c r="D188" s="53">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4">
-      <c r="A189" s="115" t="s">
-        <v>2033</v>
-      </c>
-      <c r="C189" s="53">
-        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -80994,24 +80826,24 @@
   <sheetData>
     <row r="1" spans="1:23" ht="15" customHeight="1">
       <c r="D1" s="96"/>
-      <c r="E1" s="165"/>
-      <c r="F1" s="165"/>
-      <c r="G1" s="165"/>
-      <c r="H1" s="165"/>
-      <c r="I1" s="165"/>
-      <c r="J1" s="165"/>
-      <c r="K1" s="165"/>
-      <c r="L1" s="165"/>
-      <c r="M1" s="165"/>
-      <c r="N1" s="165"/>
-      <c r="O1" s="165"/>
-      <c r="P1" s="165"/>
-      <c r="Q1" s="165"/>
-      <c r="R1" s="165"/>
-      <c r="S1" s="165"/>
-      <c r="T1" s="165"/>
-      <c r="U1" s="165"/>
-      <c r="V1" s="165"/>
+      <c r="E1" s="166"/>
+      <c r="F1" s="166"/>
+      <c r="G1" s="166"/>
+      <c r="H1" s="166"/>
+      <c r="I1" s="166"/>
+      <c r="J1" s="166"/>
+      <c r="K1" s="166"/>
+      <c r="L1" s="166"/>
+      <c r="M1" s="166"/>
+      <c r="N1" s="166"/>
+      <c r="O1" s="166"/>
+      <c r="P1" s="166"/>
+      <c r="Q1" s="166"/>
+      <c r="R1" s="166"/>
+      <c r="S1" s="166"/>
+      <c r="T1" s="166"/>
+      <c r="U1" s="166"/>
+      <c r="V1" s="166"/>
     </row>
     <row r="2" spans="1:23" ht="96" customHeight="1">
       <c r="A2" s="58"/>
@@ -82002,37 +81834,37 @@
     <row r="1" spans="1:33" ht="15" customHeight="1">
       <c r="A1" s="58"/>
       <c r="B1" s="59"/>
-      <c r="E1" s="166" t="s">
+      <c r="E1" s="167" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="165"/>
-      <c r="G1" s="165"/>
-      <c r="H1" s="165"/>
-      <c r="I1" s="165"/>
-      <c r="J1" s="165"/>
-      <c r="K1" s="165"/>
-      <c r="L1" s="165"/>
-      <c r="M1" s="165"/>
-      <c r="N1" s="165"/>
-      <c r="O1" s="165"/>
-      <c r="P1" s="165"/>
-      <c r="Q1" s="165"/>
-      <c r="R1" s="165"/>
-      <c r="S1" s="165"/>
-      <c r="T1" s="165"/>
-      <c r="U1" s="165"/>
-      <c r="V1" s="165"/>
-      <c r="W1" s="165"/>
-      <c r="X1" s="165"/>
-      <c r="Y1" s="165"/>
-      <c r="Z1" s="165"/>
-      <c r="AA1" s="165"/>
-      <c r="AB1" s="165"/>
-      <c r="AC1" s="165"/>
-      <c r="AD1" s="165"/>
-      <c r="AE1" s="165"/>
-      <c r="AF1" s="165"/>
-      <c r="AG1" s="165"/>
+      <c r="F1" s="166"/>
+      <c r="G1" s="166"/>
+      <c r="H1" s="166"/>
+      <c r="I1" s="166"/>
+      <c r="J1" s="166"/>
+      <c r="K1" s="166"/>
+      <c r="L1" s="166"/>
+      <c r="M1" s="166"/>
+      <c r="N1" s="166"/>
+      <c r="O1" s="166"/>
+      <c r="P1" s="166"/>
+      <c r="Q1" s="166"/>
+      <c r="R1" s="166"/>
+      <c r="S1" s="166"/>
+      <c r="T1" s="166"/>
+      <c r="U1" s="166"/>
+      <c r="V1" s="166"/>
+      <c r="W1" s="166"/>
+      <c r="X1" s="166"/>
+      <c r="Y1" s="166"/>
+      <c r="Z1" s="166"/>
+      <c r="AA1" s="166"/>
+      <c r="AB1" s="166"/>
+      <c r="AC1" s="166"/>
+      <c r="AD1" s="166"/>
+      <c r="AE1" s="166"/>
+      <c r="AF1" s="166"/>
+      <c r="AG1" s="166"/>
     </row>
     <row r="2" spans="1:33" ht="144" customHeight="1">
       <c r="C2" s="96" t="s">

</xml_diff>

<commit_message>
localisation columns cannot be found one_map 3 PARAHIPPOCAMPUS fixed
</commit_message>
<xml_diff>
--- a/resources/syst_review_single_table.xlsx
+++ b/resources/syst_review_single_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali_m\AnacondaProjects\PhD\Semiology-Visualisation-Tool\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF068038-F45A-4DF7-9AE6-8D9CD5B37EFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A354CC0-D796-49F8-8010-05537D6F9549}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -10496,8 +10496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DU1122"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="AK3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="AC3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="AX2" sqref="AX2"/>
@@ -80808,7 +80808,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="L25" sqref="L25"/>
+      <selection pane="bottomRight" activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -81813,7 +81813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AG324"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>

</xml_diff>